<commit_message>
ISO3 list is updated and added more countries. added more data
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="730">
   <si>
     <t>Country Name</t>
   </si>
@@ -2189,6 +2189,21 @@
   </si>
   <si>
     <t>Tanzania - Mainland</t>
+  </si>
+  <si>
+    <t>luxembourg(a)</t>
+  </si>
+  <si>
+    <t>australia(b)</t>
+  </si>
+  <si>
+    <t>estonia(a)</t>
+  </si>
+  <si>
+    <t>hungary(a)</t>
+  </si>
+  <si>
+    <t>denmark(a)</t>
   </si>
 </sst>
 </file>
@@ -3263,10 +3278,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F450"/>
+  <dimension ref="A1:F455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215:G238"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,7 +3425,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>31</v>
+        <v>726</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
@@ -3418,127 +3433,127 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>40</v>
+      <c r="B23" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>637</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>59</v>
+        <v>637</v>
       </c>
       <c r="C34" t="s">
         <v>60</v>
@@ -3546,15 +3561,15 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>716</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>61</v>
+        <v>716</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -3562,31 +3577,31 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>65</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
         <v>638</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>67</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
@@ -3594,63 +3609,63 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>639</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>81</v>
+        <v>639</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
@@ -3658,31 +3673,31 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
         <v>88</v>
@@ -3690,47 +3705,47 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>640</v>
-      </c>
-      <c r="C56" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
-        <v>641</v>
       </c>
       <c r="C57" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>96</v>
+      <c r="B58" s="10" t="s">
+        <v>641</v>
       </c>
       <c r="C58" t="s">
         <v>97</v>
@@ -3738,55 +3753,55 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>102</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
+    <row r="63" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="11" t="s">
         <v>642</v>
-      </c>
-      <c r="C62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>643</v>
       </c>
       <c r="C63" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="10" t="s">
-        <v>644</v>
+      <c r="B64" t="s">
+        <v>643</v>
       </c>
       <c r="C64" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>104</v>
+      <c r="B65" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
@@ -3794,7 +3809,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
         <v>105</v>
@@ -3802,7 +3817,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
@@ -3810,7 +3825,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>645</v>
+        <v>107</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3818,26 +3833,26 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>108</v>
+        <v>645</v>
       </c>
       <c r="C69" t="s">
         <v>105</v>
       </c>
-      <c r="D69" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="D70" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C71" t="s">
         <v>111</v>
@@ -3845,31 +3860,31 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C74" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>633</v>
+        <v>117</v>
       </c>
       <c r="C75" t="s">
         <v>118</v>
@@ -3877,7 +3892,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C76" t="s">
         <v>118</v>
@@ -3885,7 +3900,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C77" t="s">
         <v>118</v>
@@ -3893,31 +3908,31 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C78" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C80" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C81" t="s">
         <v>125</v>
@@ -3925,63 +3940,63 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C83" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>132</v>
+        <v>729</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C86" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C87" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
-        <v>139</v>
+      <c r="B89" t="s">
+        <v>136</v>
       </c>
       <c r="C89" t="s">
         <v>137</v>
@@ -3989,63 +4004,63 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>622</v>
+        <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>140</v>
+      <c r="B91" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>144</v>
+        <v>623</v>
       </c>
       <c r="C94" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C96" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C97" t="s">
         <v>147</v>
@@ -4053,63 +4068,63 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C99" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C100" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C101" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="12" t="s">
-        <v>648</v>
+      <c r="B102" t="s">
+        <v>154</v>
       </c>
       <c r="C102" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="C103" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>649</v>
+        <v>156</v>
       </c>
       <c r="C104" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>158</v>
+      <c r="B105" s="12" t="s">
+        <v>648</v>
       </c>
       <c r="C105" t="s">
         <v>159</v>
@@ -4117,367 +4132,367 @@
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>160</v>
+        <v>720</v>
       </c>
       <c r="C106" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>624</v>
+        <v>649</v>
       </c>
       <c r="C107" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C108" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>629</v>
+        <v>160</v>
       </c>
       <c r="C109" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>164</v>
+        <v>624</v>
       </c>
       <c r="C110" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C111" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>168</v>
+        <v>629</v>
       </c>
       <c r="C112" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C113" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>650</v>
+        <v>166</v>
       </c>
       <c r="C114" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C115" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C116" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>174</v>
+        <v>650</v>
       </c>
       <c r="C117" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C118" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C119" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>651</v>
+        <v>174</v>
       </c>
       <c r="C120" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C121" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C122" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>184</v>
+        <v>651</v>
       </c>
       <c r="C123" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C124" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C125" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C126" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>652</v>
+        <v>186</v>
       </c>
       <c r="C127" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C128" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C129" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>195</v>
+        <v>652</v>
       </c>
       <c r="C130" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C131" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C132" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C133" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>653</v>
+        <v>197</v>
       </c>
       <c r="C134" t="s">
-        <v>654</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C135" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C136" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>207</v>
+        <v>653</v>
       </c>
       <c r="C137" t="s">
-        <v>208</v>
+        <v>654</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C138" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C139" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="5" t="s">
-        <v>215</v>
+      <c r="B141" t="s">
+        <v>209</v>
       </c>
       <c r="C141" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C142" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C143" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>220</v>
+      <c r="B144" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C144" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C145" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C146" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C147" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>717</v>
+        <v>222</v>
       </c>
       <c r="C148" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>655</v>
+        <v>224</v>
       </c>
       <c r="C149" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>656</v>
+        <v>226</v>
       </c>
       <c r="C150" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>657</v>
+        <v>717</v>
       </c>
       <c r="C151" t="s">
         <v>229</v>
@@ -4485,7 +4500,7 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C152" t="s">
         <v>229</v>
@@ -4493,7 +4508,7 @@
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>634</v>
+        <v>656</v>
       </c>
       <c r="C153" t="s">
         <v>229</v>
@@ -4501,7 +4516,7 @@
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>228</v>
+        <v>657</v>
       </c>
       <c r="C154" t="s">
         <v>229</v>
@@ -4509,7 +4524,7 @@
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>230</v>
+        <v>658</v>
       </c>
       <c r="C155" t="s">
         <v>229</v>
@@ -4517,7 +4532,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>231</v>
+        <v>634</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4525,95 +4540,95 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C157" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C158" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B159" s="6" t="s">
-        <v>236</v>
+      <c r="B159" t="s">
+        <v>231</v>
       </c>
       <c r="C159" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>238</v>
+        <v>728</v>
       </c>
       <c r="C160" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>659</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>240</v>
+        <v>232</v>
+      </c>
+      <c r="C161" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C162" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>660</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>242</v>
+      <c r="B163" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C163" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C164" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>635</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="C166" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>243</v>
-      </c>
-      <c r="C167" t="s">
+        <v>660</v>
+      </c>
+      <c r="C167" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="168" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B168" s="11" t="s">
-        <v>662</v>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>241</v>
       </c>
       <c r="C168" t="s">
         <v>242</v>
@@ -4621,175 +4636,175 @@
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>244</v>
-      </c>
-      <c r="C169" t="s">
+        <v>661</v>
+      </c>
+      <c r="C169" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>245</v>
-      </c>
-      <c r="C170" t="s">
-        <v>246</v>
+        <v>635</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C171" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B172" s="11" t="s">
+        <v>662</v>
       </c>
       <c r="C172" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C173" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C174" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C175" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>256</v>
+      <c r="B176" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C176" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C177" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C178" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C179" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C180" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C181" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C182" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C183" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C184" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>663</v>
+        <v>265</v>
       </c>
       <c r="C185" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="186" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B186" s="11" t="s">
-        <v>713</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>267</v>
       </c>
       <c r="C186" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>664</v>
+        <v>269</v>
       </c>
       <c r="C187" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B188" s="10" t="s">
-        <v>665</v>
+      <c r="B188" t="s">
+        <v>271</v>
       </c>
       <c r="C188" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B189" s="10" t="s">
-        <v>666</v>
+      <c r="B189" t="s">
+        <v>663</v>
       </c>
       <c r="C189" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
-        <v>273</v>
+    <row r="190" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B190" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C190" t="s">
         <v>272</v>
@@ -4797,39 +4812,39 @@
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C191" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>718</v>
+      <c r="B192" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C192" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
-        <v>274</v>
+      <c r="B193" s="10" t="s">
+        <v>666</v>
       </c>
       <c r="C193" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>668</v>
+        <v>273</v>
       </c>
       <c r="C194" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>276</v>
+        <v>667</v>
       </c>
       <c r="C195" t="s">
         <v>275</v>
@@ -4837,15 +4852,15 @@
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>636</v>
+        <v>718</v>
       </c>
       <c r="C196" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>277</v>
+      <c r="B197" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C197" t="s">
         <v>275</v>
@@ -4853,7 +4868,7 @@
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>278</v>
+        <v>668</v>
       </c>
       <c r="C198" t="s">
         <v>275</v>
@@ -4861,7 +4876,7 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>669</v>
+        <v>276</v>
       </c>
       <c r="C199" t="s">
         <v>275</v>
@@ -4869,7 +4884,7 @@
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
@@ -4877,71 +4892,71 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C201" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C202" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>283</v>
+      <c r="B203" t="s">
+        <v>669</v>
       </c>
       <c r="C203" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>285</v>
+        <v>670</v>
       </c>
       <c r="C204" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C205" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>671</v>
+        <v>281</v>
       </c>
       <c r="C206" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="10" t="s">
-        <v>672</v>
+      <c r="B207" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="C207" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C208" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>673</v>
+        <v>286</v>
       </c>
       <c r="C209" t="s">
         <v>287</v>
@@ -4949,1760 +4964,1760 @@
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>289</v>
+        <v>671</v>
       </c>
       <c r="C210" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>625</v>
+      <c r="B211" s="10" t="s">
+        <v>672</v>
       </c>
       <c r="C211" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C212" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>626</v>
+        <v>673</v>
       </c>
       <c r="C213" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C214" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>294</v>
+        <v>625</v>
       </c>
       <c r="C215" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C216" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>298</v>
+        <v>626</v>
       </c>
       <c r="C217" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C218" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C219" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="220" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B220" s="11" t="s">
-        <v>714</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>296</v>
       </c>
       <c r="C220" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C221" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B222" s="4" t="s">
-        <v>306</v>
+      <c r="B222" t="s">
+        <v>300</v>
       </c>
       <c r="C222" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C223" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
-        <v>309</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B224" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C224" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="225" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>630</v>
+        <v>304</v>
       </c>
       <c r="C225" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>311</v>
+      <c r="B226" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C226" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="227" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C227" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="228" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C228" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="229" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>317</v>
+        <v>630</v>
       </c>
       <c r="C229" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="230" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>674</v>
+        <v>311</v>
       </c>
       <c r="C230" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="231" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>675</v>
+        <v>313</v>
       </c>
       <c r="C231" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="232" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C232" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="233" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>676</v>
+        <v>725</v>
       </c>
       <c r="C233" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="234" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C234" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>322</v>
+        <v>674</v>
       </c>
       <c r="C235" t="s">
         <v>320</v>
       </c>
-      <c r="E235" s="4"/>
     </row>
     <row r="236" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>323</v>
+        <v>675</v>
       </c>
       <c r="C236" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="237" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B237" s="4" t="s">
-        <v>324</v>
+      <c r="B237" t="s">
+        <v>319</v>
       </c>
       <c r="C237" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="238" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B238" s="4" t="s">
-        <v>677</v>
+      <c r="B238" t="s">
+        <v>676</v>
       </c>
       <c r="C238" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="239" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B239" s="11" t="s">
-        <v>678</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>321</v>
       </c>
       <c r="C239" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="240" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>679</v>
+        <v>322</v>
       </c>
       <c r="C240" t="s">
-        <v>325</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="E240" s="4"/>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C241" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B242" t="s">
-        <v>327</v>
+      <c r="B242" s="4" t="s">
+        <v>324</v>
       </c>
       <c r="C242" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="243" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B243" t="s">
-        <v>328</v>
+      <c r="B243" s="4" t="s">
+        <v>677</v>
       </c>
       <c r="C243" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B244" t="s">
-        <v>329</v>
+    <row r="244" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B244" s="11" t="s">
+        <v>678</v>
       </c>
       <c r="C244" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>331</v>
+        <v>679</v>
       </c>
       <c r="C245" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C246" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C247" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C248" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
     </row>
     <row r="249" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C249" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C250" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="251" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C251" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="252" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C252" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="253" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C253" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="254" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C254" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="255" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C255" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="256" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C256" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C257" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>721</v>
+        <v>347</v>
       </c>
       <c r="C258" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B259" s="10" t="s">
-        <v>680</v>
+      <c r="B259" t="s">
+        <v>349</v>
       </c>
       <c r="C259" t="s">
-        <v>354</v>
-      </c>
-      <c r="F259" s="4"/>
+        <v>350</v>
+      </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>627</v>
+        <v>351</v>
       </c>
       <c r="C260" t="s">
-        <v>357</v>
-      </c>
-      <c r="F260" s="4"/>
+        <v>352</v>
+      </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C261" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>628</v>
+        <v>355</v>
       </c>
       <c r="C262" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>358</v>
+        <v>721</v>
       </c>
       <c r="C263" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B264" t="s">
-        <v>360</v>
+      <c r="B264" s="10" t="s">
+        <v>680</v>
       </c>
       <c r="C264" t="s">
-        <v>361</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="F264" s="4"/>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>681</v>
+        <v>627</v>
       </c>
       <c r="C265" t="s">
-        <v>363</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="F265" s="4"/>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C266" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>682</v>
+        <v>628</v>
       </c>
       <c r="C267" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B268" s="4" t="s">
-        <v>364</v>
+      <c r="B268" t="s">
+        <v>358</v>
       </c>
       <c r="C268" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C269" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>367</v>
+        <v>681</v>
       </c>
       <c r="C270" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C271" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>371</v>
+        <v>682</v>
       </c>
       <c r="C272" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B273" t="s">
-        <v>373</v>
+      <c r="B273" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C273" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C274" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C275" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="C276" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C277" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C278" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C279" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C280" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B281" s="4" t="s">
-        <v>389</v>
+      <c r="B281" t="s">
+        <v>379</v>
       </c>
       <c r="C281" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C282" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C283" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C284" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C285" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B286" t="s">
-        <v>397</v>
+      <c r="B286" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C286" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="C287" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C288" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="C289" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C290" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="C291" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="C292" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C293" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C294" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C295" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C296" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C297" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C298" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="C299" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="C300" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="C301" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>683</v>
+        <v>417</v>
       </c>
       <c r="C302" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C303" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>684</v>
+        <v>421</v>
       </c>
       <c r="C304" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C305" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B306" s="4" t="s">
-        <v>430</v>
+      <c r="B306" t="s">
+        <v>425</v>
       </c>
       <c r="C306" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C307" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C308" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>433</v>
+        <v>684</v>
       </c>
       <c r="C309" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C310" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B311" t="s">
-        <v>437</v>
+      <c r="B311" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C311" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>439</v>
+        <v>685</v>
       </c>
       <c r="C312" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C313" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="C314" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>631</v>
+        <v>435</v>
       </c>
       <c r="C315" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C316" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C317" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C318" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C319" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>453</v>
+        <v>631</v>
       </c>
       <c r="C320" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="C321" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C322" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C323" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="C324" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>686</v>
+        <v>453</v>
       </c>
       <c r="C325" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>632</v>
+        <v>455</v>
       </c>
       <c r="C326" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C327" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C328" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C329" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>466</v>
+        <v>686</v>
       </c>
       <c r="C330" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>468</v>
+        <v>632</v>
       </c>
       <c r="C331" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="332" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B332" s="11" t="s">
-        <v>715</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>462</v>
       </c>
       <c r="C332" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C333" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B334" s="4" t="s">
-        <v>472</v>
+      <c r="B334" t="s">
+        <v>465</v>
       </c>
       <c r="C334" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="C335" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C336" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="337" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B337" t="s">
-        <v>477</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="337" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B337" s="11" t="s">
+        <v>715</v>
       </c>
       <c r="C337" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="C338" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="339" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B339" t="s">
-        <v>481</v>
+      <c r="B339" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C339" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="340" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B340" s="4" t="s">
-        <v>482</v>
+      <c r="B340" t="s">
+        <v>473</v>
       </c>
       <c r="C340" t="s">
-        <v>483</v>
-      </c>
-      <c r="E340" s="4"/>
+        <v>474</v>
+      </c>
     </row>
     <row r="341" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="C341" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="342" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="C342" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="343" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C343" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="C344" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
     </row>
     <row r="345" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B345" t="s">
-        <v>491</v>
+      <c r="B345" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C345" t="s">
-        <v>492</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E345" s="4"/>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="C346" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="347" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="C347" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="C348" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
     </row>
     <row r="349" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="C349" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
     </row>
     <row r="350" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="C350" t="s">
-        <v>502</v>
-      </c>
-      <c r="E350" s="4"/>
+        <v>492</v>
+      </c>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>687</v>
+        <v>493</v>
       </c>
       <c r="C351" t="s">
-        <v>19</v>
-      </c>
-      <c r="E351" s="4"/>
+        <v>494</v>
+      </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
+        <v>495</v>
+      </c>
+      <c r="C352" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="353" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>497</v>
+      </c>
+      <c r="C353" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="354" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>499</v>
+      </c>
+      <c r="C354" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="355" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>501</v>
+      </c>
+      <c r="C355" t="s">
+        <v>502</v>
+      </c>
+      <c r="E355" s="4"/>
+    </row>
+    <row r="356" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>687</v>
+      </c>
+      <c r="C356" t="s">
+        <v>19</v>
+      </c>
+      <c r="E356" s="4"/>
+    </row>
+    <row r="357" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
         <v>503</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C357" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B353" t="s">
+    <row r="358" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
         <v>688</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C358" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B354" t="s">
+    <row r="359" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
         <v>504</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C359" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B355" t="s">
+    <row r="360" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
         <v>506</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C360" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B356" t="s">
+    <row r="361" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B361" t="s">
         <v>689</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C361" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B357" t="s">
+    <row r="362" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
         <v>507</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C362" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B358" t="s">
+    <row r="363" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
         <v>509</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C363" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B359" t="s">
+    <row r="364" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
         <v>690</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C364" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B360" t="s">
+    <row r="365" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
         <v>511</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C365" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B361" t="s">
+    <row r="366" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
         <v>513</v>
       </c>
-      <c r="C361" t="s">
+      <c r="C366" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B362" t="s">
+    <row r="367" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
         <v>514</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C367" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B363" t="s">
+    <row r="368" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B368" t="s">
         <v>691</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C368" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B364" t="s">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
         <v>516</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C369" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B365" t="s">
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
         <v>517</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C370" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B366" t="s">
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
         <v>519</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C371" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B367" t="s">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
         <v>722</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C372" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B368" t="s">
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
         <v>692</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C373" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B369" t="s">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B374" t="s">
         <v>693</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C374" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B370" t="s">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B375" t="s">
         <v>521</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C375" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B371" t="s">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B376" t="s">
         <v>523</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C376" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B372" t="s">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B377" t="s">
         <v>525</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C377" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B373" t="s">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B378" t="s">
         <v>527</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C378" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B374" t="s">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B379" t="s">
         <v>529</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C379" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B375" t="s">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B380" t="s">
         <v>531</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C380" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B376" t="s">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B381" t="s">
         <v>533</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C381" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B377" t="s">
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B382" t="s">
         <v>694</v>
       </c>
-      <c r="C377" t="s">
+      <c r="C382" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B378" t="s">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B383" t="s">
         <v>534</v>
       </c>
-      <c r="C378" t="s">
+      <c r="C383" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B379" t="s">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B384" t="s">
         <v>536</v>
       </c>
-      <c r="C379" t="s">
+      <c r="C384" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B380" t="s">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B385" t="s">
         <v>537</v>
       </c>
-      <c r="C380" t="s">
+      <c r="C385" t="s">
         <v>535</v>
       </c>
-      <c r="D380" t="s">
+      <c r="D385" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B381" t="s">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B386" t="s">
         <v>538</v>
       </c>
-      <c r="C381" t="s">
+      <c r="C386" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B382" t="s">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B387" t="s">
         <v>539</v>
       </c>
-      <c r="C382" t="s">
+      <c r="C387" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B383" t="s">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B388" t="s">
         <v>723</v>
       </c>
-      <c r="C383" t="s">
+      <c r="C388" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B384" s="10" t="s">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B389" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="C384" t="s">
+      <c r="C389" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B385" t="s">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B390" t="s">
         <v>541</v>
-      </c>
-      <c r="C385" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B386" t="s">
-        <v>724</v>
-      </c>
-      <c r="C386" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="387" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B387" s="11" t="s">
-        <v>697</v>
-      </c>
-      <c r="C387" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B388" t="s">
-        <v>698</v>
-      </c>
-      <c r="C388" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B389" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="C389" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B390" s="10" t="s">
-        <v>700</v>
       </c>
       <c r="C390" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B391" s="4" t="s">
-        <v>543</v>
+    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B391" t="s">
+        <v>724</v>
       </c>
       <c r="C391" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B392" t="s">
+    <row r="392" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B392" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="C392" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B393" t="s">
+        <v>698</v>
+      </c>
+      <c r="C393" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B394" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B395" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="C395" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B396" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="C396" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B397" t="s">
         <v>544</v>
       </c>
-      <c r="C392" t="s">
+      <c r="C397" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B393" t="s">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B398" t="s">
         <v>701</v>
       </c>
-      <c r="C393" t="s">
+      <c r="C398" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B394" t="s">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B399" t="s">
         <v>546</v>
       </c>
-      <c r="C394" t="s">
+      <c r="C399" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B395" t="s">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B400" t="s">
         <v>548</v>
       </c>
-      <c r="C395" t="s">
+      <c r="C400" t="s">
         <v>549</v>
-      </c>
-    </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B396" t="s">
-        <v>550</v>
-      </c>
-      <c r="C396" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B397" t="s">
-        <v>552</v>
-      </c>
-      <c r="C397" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B398" t="s">
-        <v>719</v>
-      </c>
-      <c r="C398" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B399" t="s">
-        <v>554</v>
-      </c>
-      <c r="C399" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B400" t="s">
-        <v>556</v>
-      </c>
-      <c r="C400" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C401" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C402" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>561</v>
+        <v>719</v>
       </c>
       <c r="C403" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="C404" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B405" s="4" t="s">
-        <v>565</v>
+      <c r="B405" t="s">
+        <v>556</v>
       </c>
       <c r="C405" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="C406" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="C407" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C408" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="C409" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B410" t="s">
-        <v>573</v>
+      <c r="B410" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C410" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>702</v>
+        <v>566</v>
       </c>
       <c r="C411" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="C412" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C413" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B414" s="4" t="s">
-        <v>579</v>
+      <c r="B414" t="s">
+        <v>571</v>
       </c>
       <c r="C414" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="C415" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>582</v>
+        <v>702</v>
       </c>
       <c r="C416" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="C417" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>703</v>
+        <v>577</v>
       </c>
       <c r="C418" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B419" t="s">
-        <v>704</v>
+      <c r="B419" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C419" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C420" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="C421" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="C422" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B423" s="4" t="s">
-        <v>591</v>
+      <c r="B423" t="s">
+        <v>703</v>
       </c>
       <c r="C423" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>593</v>
+        <v>704</v>
       </c>
       <c r="C424" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="C425" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="C426" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="427" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B427" s="11" t="s">
-        <v>705</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B427" t="s">
+        <v>589</v>
       </c>
       <c r="C427" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B428" s="10" t="s">
-        <v>706</v>
+      <c r="B428" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C428" t="s">
         <v>592</v>
@@ -6710,7 +6725,7 @@
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C429" t="s">
         <v>592</v>
@@ -6718,173 +6733,214 @@
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C430" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C431" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B432" t="s">
-        <v>600</v>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="432" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B432" s="11" t="s">
+        <v>705</v>
       </c>
       <c r="C432" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B433" t="s">
-        <v>602</v>
+      <c r="B433" s="10" t="s">
+        <v>706</v>
       </c>
       <c r="C433" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>707</v>
+        <v>596</v>
       </c>
       <c r="C434" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C435" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="C436" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" s="4" t="s">
-        <v>606</v>
+      <c r="B437" t="s">
+        <v>600</v>
       </c>
       <c r="C437" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B438" s="4" t="s">
-        <v>708</v>
+      <c r="B438" t="s">
+        <v>602</v>
       </c>
       <c r="C438" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C439" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C440" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>711</v>
+        <v>605</v>
       </c>
       <c r="C441" t="s">
-        <v>712</v>
+        <v>604</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" t="s">
-        <v>609</v>
+      <c r="B442" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C442" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B443" t="s">
-        <v>611</v>
+      <c r="B443" s="4" t="s">
+        <v>708</v>
       </c>
       <c r="C443" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>613</v>
+        <v>709</v>
       </c>
       <c r="C444" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>710</v>
+        <v>607</v>
       </c>
       <c r="C445" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B446" s="4" t="s">
-        <v>615</v>
+      <c r="B446" t="s">
+        <v>711</v>
       </c>
       <c r="C446" t="s">
-        <v>614</v>
+        <v>712</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="C447" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="C448" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="C449" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
+        <v>710</v>
+      </c>
+      <c r="C450" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B451" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C451" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B452" t="s">
+        <v>616</v>
+      </c>
+      <c r="C452" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B453" t="s">
+        <v>617</v>
+      </c>
+      <c r="C453" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B454" t="s">
+        <v>618</v>
+      </c>
+      <c r="C454" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B455" t="s">
         <v>620</v>
       </c>
-      <c r="C450" t="s">
+      <c r="C455" t="s">
         <v>621</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more data and new function for conference board data
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Country Code" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1" iterateCount="4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="732">
   <si>
     <t>Country Name</t>
   </si>
@@ -2204,6 +2204,12 @@
   </si>
   <si>
     <t>denmark(a)</t>
+  </si>
+  <si>
+    <t>DR congo</t>
+  </si>
+  <si>
+    <t>Serbia &amp; Montenegro</t>
   </si>
 </sst>
 </file>
@@ -3278,10 +3284,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F455"/>
+  <dimension ref="A1:F457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,33 +3789,33 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
-        <v>642</v>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>730</v>
       </c>
       <c r="C63" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>643</v>
+    <row r="64" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="11" t="s">
+        <v>642</v>
       </c>
       <c r="C64" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="10" t="s">
-        <v>644</v>
+      <c r="B65" t="s">
+        <v>643</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>104</v>
+      <c r="B66" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="C66" t="s">
         <v>105</v>
@@ -3817,7 +3823,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
@@ -3825,7 +3831,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3833,7 +3839,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>645</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
         <v>105</v>
@@ -3841,26 +3847,26 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>108</v>
+        <v>645</v>
       </c>
       <c r="C70" t="s">
         <v>105</v>
       </c>
-      <c r="D70" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="D71" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C72" t="s">
         <v>111</v>
@@ -3868,31 +3874,31 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C73" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>633</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
         <v>118</v>
@@ -3900,7 +3906,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C77" t="s">
         <v>118</v>
@@ -3908,7 +3914,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C78" t="s">
         <v>118</v>
@@ -3916,31 +3922,31 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C80" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C81" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C82" t="s">
         <v>125</v>
@@ -3948,31 +3954,31 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>729</v>
+        <v>128</v>
       </c>
       <c r="C85" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>130</v>
+        <v>729</v>
       </c>
       <c r="C86" t="s">
         <v>131</v>
@@ -3980,55 +3986,55 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C88" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C90" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
-        <v>139</v>
+      <c r="B91" t="s">
+        <v>138</v>
       </c>
       <c r="C91" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>622</v>
+      <c r="B92" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C92" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C93" t="s">
         <v>141</v>
@@ -4036,15 +4042,15 @@
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C94" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C95" t="s">
         <v>143</v>
@@ -4052,23 +4058,23 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C97" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C98" t="s">
         <v>147</v>
@@ -4076,7 +4082,7 @@
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" t="s">
         <v>147</v>
@@ -4084,55 +4090,55 @@
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C100" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C101" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C102" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>727</v>
+        <v>154</v>
       </c>
       <c r="C103" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>156</v>
+        <v>727</v>
       </c>
       <c r="C104" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="12" t="s">
+      <c r="B105" t="s">
+        <v>156</v>
+      </c>
+      <c r="C105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="12" t="s">
         <v>648</v>
-      </c>
-      <c r="C105" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>720</v>
       </c>
       <c r="C106" t="s">
         <v>159</v>
@@ -4140,7 +4146,7 @@
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>649</v>
+        <v>720</v>
       </c>
       <c r="C107" t="s">
         <v>159</v>
@@ -4148,7 +4154,7 @@
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>158</v>
+        <v>649</v>
       </c>
       <c r="C108" t="s">
         <v>159</v>
@@ -4156,23 +4162,23 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>624</v>
+        <v>160</v>
       </c>
       <c r="C110" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>162</v>
+        <v>624</v>
       </c>
       <c r="C111" t="s">
         <v>163</v>
@@ -4180,15 +4186,15 @@
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>629</v>
+        <v>162</v>
       </c>
       <c r="C112" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>164</v>
+        <v>629</v>
       </c>
       <c r="C113" t="s">
         <v>165</v>
@@ -4196,23 +4202,23 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C114" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C115" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C116" t="s">
         <v>169</v>
@@ -4220,15 +4226,15 @@
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>650</v>
+        <v>170</v>
       </c>
       <c r="C117" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>171</v>
+        <v>650</v>
       </c>
       <c r="C118" t="s">
         <v>172</v>
@@ -4236,7 +4242,7 @@
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C119" t="s">
         <v>172</v>
@@ -4244,39 +4250,39 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C121" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C122" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>651</v>
+        <v>178</v>
       </c>
       <c r="C123" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>180</v>
+        <v>651</v>
       </c>
       <c r="C124" t="s">
         <v>181</v>
@@ -4284,31 +4290,31 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C125" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C126" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C127" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C128" t="s">
         <v>187</v>
@@ -4316,23 +4322,23 @@
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C129" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>652</v>
+        <v>189</v>
       </c>
       <c r="C130" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>191</v>
+        <v>652</v>
       </c>
       <c r="C131" t="s">
         <v>192</v>
@@ -4340,167 +4346,167 @@
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C132" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C133" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C134" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C135" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C136" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>653</v>
+        <v>201</v>
       </c>
       <c r="C137" t="s">
-        <v>654</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>203</v>
+        <v>653</v>
       </c>
       <c r="C138" t="s">
-        <v>204</v>
+        <v>654</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C139" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C140" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C141" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C142" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
+        <v>211</v>
+      </c>
+      <c r="C143" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
         <v>213</v>
-      </c>
-      <c r="C143" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C144" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>216</v>
+      <c r="B145" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C145" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C146" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C147" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C148" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C149" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C150" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>717</v>
+        <v>226</v>
       </c>
       <c r="C151" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>655</v>
+        <v>717</v>
       </c>
       <c r="C152" t="s">
         <v>229</v>
@@ -4508,7 +4514,7 @@
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C153" t="s">
         <v>229</v>
@@ -4516,7 +4522,7 @@
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C154" t="s">
         <v>229</v>
@@ -4524,7 +4530,7 @@
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C155" t="s">
         <v>229</v>
@@ -4532,7 +4538,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>634</v>
+        <v>658</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4540,7 +4546,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>228</v>
+        <v>634</v>
       </c>
       <c r="C157" t="s">
         <v>229</v>
@@ -4548,7 +4554,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C158" t="s">
         <v>229</v>
@@ -4556,7 +4562,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4564,15 +4570,15 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>728</v>
+        <v>231</v>
       </c>
       <c r="C160" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>232</v>
+        <v>728</v>
       </c>
       <c r="C161" t="s">
         <v>233</v>
@@ -4580,23 +4586,23 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
+        <v>232</v>
+      </c>
+      <c r="C162" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>234</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="6" t="s">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="C163" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>238</v>
       </c>
       <c r="C164" t="s">
         <v>237</v>
@@ -4604,47 +4610,47 @@
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>659</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
+      </c>
+      <c r="C165" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>239</v>
-      </c>
-      <c r="C166" t="s">
+        <v>659</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>660</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="C167" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>241</v>
-      </c>
-      <c r="C168" t="s">
+        <v>660</v>
+      </c>
+      <c r="C168" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>661</v>
-      </c>
-      <c r="C169" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C169" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>635</v>
+        <v>661</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>242</v>
@@ -4652,23 +4658,23 @@
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
+        <v>635</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>243</v>
-      </c>
-      <c r="C171" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="172" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B172" s="11" t="s">
-        <v>662</v>
       </c>
       <c r="C172" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>244</v>
+    <row r="173" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B173" s="11" t="s">
+        <v>662</v>
       </c>
       <c r="C173" t="s">
         <v>242</v>
@@ -4676,79 +4682,79 @@
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C174" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
+        <v>245</v>
+      </c>
+      <c r="C175" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
         <v>247</v>
-      </c>
-      <c r="C175" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B176" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="C176" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
-        <v>250</v>
+      <c r="B177" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C177" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C178" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C179" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C180" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C181" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C182" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C183" t="s">
         <v>261</v>
@@ -4756,71 +4762,71 @@
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C184" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C185" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C186" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C187" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C188" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>663</v>
+        <v>271</v>
       </c>
       <c r="C189" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="190" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B190" s="11" t="s">
-        <v>713</v>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>663</v>
       </c>
       <c r="C190" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
-        <v>664</v>
+    <row r="191" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B191" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C191" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B192" s="10" t="s">
-        <v>665</v>
+      <c r="B192" t="s">
+        <v>664</v>
       </c>
       <c r="C192" t="s">
         <v>272</v>
@@ -4828,15 +4834,15 @@
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C193" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
-        <v>273</v>
+      <c r="B194" s="10" t="s">
+        <v>666</v>
       </c>
       <c r="C194" t="s">
         <v>272</v>
@@ -4844,31 +4850,31 @@
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>667</v>
+        <v>273</v>
       </c>
       <c r="C195" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>718</v>
+        <v>667</v>
       </c>
       <c r="C196" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="4" t="s">
-        <v>274</v>
+      <c r="B197" t="s">
+        <v>718</v>
       </c>
       <c r="C197" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>668</v>
+      <c r="B198" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C198" t="s">
         <v>275</v>
@@ -4876,7 +4882,7 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>276</v>
+        <v>668</v>
       </c>
       <c r="C199" t="s">
         <v>275</v>
@@ -4884,7 +4890,7 @@
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>636</v>
+        <v>276</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
@@ -4892,7 +4898,7 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>277</v>
+        <v>636</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4900,7 +4906,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
@@ -4908,7 +4914,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>669</v>
+        <v>278</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
@@ -4916,7 +4922,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4924,31 +4930,31 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>279</v>
+        <v>670</v>
       </c>
       <c r="C205" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
+        <v>279</v>
+      </c>
+      <c r="C206" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
         <v>281</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C207" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="4" t="s">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C207" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
-        <v>285</v>
       </c>
       <c r="C208" t="s">
         <v>284</v>
@@ -4956,31 +4962,31 @@
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C209" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>671</v>
+        <v>286</v>
       </c>
       <c r="C210" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" s="10" t="s">
-        <v>672</v>
+      <c r="B211" t="s">
+        <v>671</v>
       </c>
       <c r="C211" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>288</v>
+      <c r="B212" s="10" t="s">
+        <v>672</v>
       </c>
       <c r="C212" t="s">
         <v>287</v>
@@ -4988,7 +4994,7 @@
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>673</v>
+        <v>288</v>
       </c>
       <c r="C213" t="s">
         <v>287</v>
@@ -4996,7 +5002,7 @@
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>289</v>
+        <v>673</v>
       </c>
       <c r="C214" t="s">
         <v>287</v>
@@ -5004,15 +5010,15 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>625</v>
+        <v>289</v>
       </c>
       <c r="C215" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>290</v>
+        <v>625</v>
       </c>
       <c r="C216" t="s">
         <v>291</v>
@@ -5020,15 +5026,15 @@
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>626</v>
+        <v>290</v>
       </c>
       <c r="C217" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>292</v>
+        <v>626</v>
       </c>
       <c r="C218" t="s">
         <v>293</v>
@@ -5036,352 +5042,352 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C219" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C220" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C221" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C222" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
+        <v>300</v>
+      </c>
+      <c r="C223" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>302</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C224" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="224" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B224" s="11" t="s">
+    <row r="225" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B225" s="11" t="s">
         <v>714</v>
-      </c>
-      <c r="C224" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B225" t="s">
-        <v>304</v>
       </c>
       <c r="C225" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B226" s="4" t="s">
-        <v>306</v>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>304</v>
       </c>
       <c r="C226" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B227" t="s">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C227" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
         <v>307</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C228" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="228" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
         <v>309</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C229" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
         <v>630</v>
-      </c>
-      <c r="C229" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="230" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B230" t="s">
-        <v>311</v>
       </c>
       <c r="C230" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="231" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
+        <v>311</v>
+      </c>
+      <c r="C231" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
         <v>313</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C232" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
         <v>315</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C233" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="233" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B233" t="s">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
         <v>725</v>
-      </c>
-      <c r="C233" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="234" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B234" t="s">
-        <v>317</v>
       </c>
       <c r="C234" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="235" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
+        <v>317</v>
+      </c>
+      <c r="C235" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
         <v>674</v>
-      </c>
-      <c r="C235" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="236" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B236" t="s">
-        <v>675</v>
       </c>
       <c r="C236" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="237" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>319</v>
+        <v>675</v>
       </c>
       <c r="C237" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="238" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>676</v>
+        <v>319</v>
       </c>
       <c r="C238" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>321</v>
+        <v>676</v>
       </c>
       <c r="C239" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="240" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C240" t="s">
         <v>320</v>
       </c>
-      <c r="E240" s="4"/>
-    </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C241" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B242" s="4" t="s">
+      <c r="E241" s="4"/>
+    </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>323</v>
+      </c>
+      <c r="C242" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="C242" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B243" s="4" t="s">
-        <v>677</v>
       </c>
       <c r="C243" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="244" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B244" s="11" t="s">
-        <v>678</v>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244" s="4" t="s">
+        <v>677</v>
       </c>
       <c r="C244" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B245" t="s">
-        <v>679</v>
+    <row r="245" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B245" s="11" t="s">
+        <v>678</v>
       </c>
       <c r="C245" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>326</v>
+        <v>679</v>
       </c>
       <c r="C246" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C247" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C248" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
+        <v>328</v>
+      </c>
+      <c r="C249" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
         <v>329</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C250" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B250" t="s">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
         <v>331</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C251" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
         <v>333</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C252" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B252" t="s">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
         <v>335</v>
       </c>
-      <c r="C252" t="s">
+      <c r="C253" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B253" t="s">
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
         <v>337</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C254" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B254" t="s">
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
         <v>339</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C255" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B255" t="s">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
         <v>341</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C256" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
-        <v>343</v>
-      </c>
-      <c r="C256" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C257" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C258" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C259" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C260" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C261" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C262" t="s">
         <v>354</v>
@@ -5389,49 +5395,49 @@
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>721</v>
+        <v>355</v>
       </c>
       <c r="C263" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B264" s="10" t="s">
-        <v>680</v>
+      <c r="B264" t="s">
+        <v>721</v>
       </c>
       <c r="C264" t="s">
         <v>354</v>
       </c>
-      <c r="F264" s="4"/>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B265" t="s">
-        <v>627</v>
+      <c r="B265" s="10" t="s">
+        <v>680</v>
       </c>
       <c r="C265" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F265" s="4"/>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>356</v>
+        <v>627</v>
       </c>
       <c r="C266" t="s">
         <v>357</v>
       </c>
+      <c r="F266" s="4"/>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>628</v>
+        <v>356</v>
       </c>
       <c r="C267" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>358</v>
+        <v>628</v>
       </c>
       <c r="C268" t="s">
         <v>359</v>
@@ -5439,23 +5445,23 @@
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C269" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>681</v>
+        <v>360</v>
       </c>
       <c r="C270" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>362</v>
+        <v>681</v>
       </c>
       <c r="C271" t="s">
         <v>363</v>
@@ -5463,127 +5469,127 @@
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>682</v>
+        <v>362</v>
       </c>
       <c r="C272" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B273" s="4" t="s">
-        <v>364</v>
+      <c r="B273" t="s">
+        <v>682</v>
       </c>
       <c r="C273" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B274" t="s">
-        <v>365</v>
+      <c r="B274" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C274" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C275" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C276" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C277" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C278" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C279" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C280" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C281" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C282" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C283" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C284" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
+        <v>385</v>
+      </c>
+      <c r="C285" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
         <v>387</v>
-      </c>
-      <c r="C285" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B286" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="C286" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B287" t="s">
-        <v>390</v>
+      <c r="B287" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C287" t="s">
         <v>388</v>
@@ -5591,63 +5597,63 @@
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C288" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C289" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C290" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C291" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C292" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C293" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C294" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C295" t="s">
         <v>404</v>
@@ -5655,23 +5661,23 @@
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C296" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C297" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C298" t="s">
         <v>409</v>
@@ -5679,79 +5685,79 @@
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C299" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C300" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C301" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C302" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C303" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C304" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C305" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C306" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>683</v>
+        <v>425</v>
       </c>
       <c r="C307" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>427</v>
+        <v>683</v>
       </c>
       <c r="C308" t="s">
         <v>428</v>
@@ -5759,7 +5765,7 @@
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>684</v>
+        <v>427</v>
       </c>
       <c r="C309" t="s">
         <v>428</v>
@@ -5767,31 +5773,31 @@
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>429</v>
+        <v>684</v>
       </c>
       <c r="C310" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B311" s="4" t="s">
-        <v>430</v>
+      <c r="B311" t="s">
+        <v>429</v>
       </c>
       <c r="C311" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B312" t="s">
-        <v>685</v>
+      <c r="B312" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C312" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>431</v>
+        <v>685</v>
       </c>
       <c r="C313" t="s">
         <v>432</v>
@@ -5799,63 +5805,63 @@
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C314" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C315" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C316" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C317" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C318" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C319" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>631</v>
+        <v>443</v>
       </c>
       <c r="C320" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>445</v>
+        <v>631</v>
       </c>
       <c r="C321" t="s">
         <v>446</v>
@@ -5863,39 +5869,39 @@
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C322" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C323" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C324" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C325" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C326" t="s">
         <v>454</v>
@@ -5903,39 +5909,39 @@
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C327" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C328" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C329" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>686</v>
+        <v>460</v>
       </c>
       <c r="C330" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>632</v>
+        <v>686</v>
       </c>
       <c r="C331" t="s">
         <v>463</v>
@@ -5943,7 +5949,7 @@
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>462</v>
+        <v>632</v>
       </c>
       <c r="C332" t="s">
         <v>463</v>
@@ -5951,7 +5957,7 @@
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C333" t="s">
         <v>463</v>
@@ -5959,7 +5965,7 @@
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C334" t="s">
         <v>463</v>
@@ -5967,39 +5973,39 @@
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C335" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
+        <v>466</v>
+      </c>
+      <c r="C336" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="337" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
         <v>468</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C337" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="337" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B337" s="11" t="s">
-        <v>715</v>
-      </c>
-      <c r="C337" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="338" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B338" t="s">
-        <v>470</v>
+    <row r="338" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B338" s="11" t="s">
+        <v>731</v>
       </c>
       <c r="C338" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="339" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B339" s="4" t="s">
-        <v>472</v>
+    <row r="339" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B339" s="11" t="s">
+        <v>715</v>
       </c>
       <c r="C339" t="s">
         <v>471</v>
@@ -6007,170 +6013,170 @@
     </row>
     <row r="340" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C340" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="341" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B341" t="s">
-        <v>475</v>
+      <c r="B341" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C341" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="342" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C342" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="343" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C343" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C344" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="345" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
+        <v>479</v>
+      </c>
+      <c r="C345" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="345" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B345" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C345" t="s">
-        <v>483</v>
-      </c>
-      <c r="E345" s="4"/>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C346" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="347" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B347" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="C347" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B347" t="s">
-        <v>485</v>
-      </c>
-      <c r="C347" t="s">
-        <v>486</v>
-      </c>
+      <c r="E347" s="4"/>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C348" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="349" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C349" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="350" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C350" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C351" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C352" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C353" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C354" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C355" t="s">
-        <v>502</v>
-      </c>
-      <c r="E355" s="4"/>
+        <v>498</v>
+      </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>687</v>
+        <v>499</v>
       </c>
       <c r="C356" t="s">
-        <v>19</v>
-      </c>
-      <c r="E356" s="4"/>
+        <v>500</v>
+      </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C357" t="s">
-        <v>19</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E357" s="4"/>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C358" t="s">
-        <v>505</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E358" s="4"/>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C359" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>506</v>
+        <v>688</v>
       </c>
       <c r="C360" t="s">
         <v>505</v>
@@ -6178,47 +6184,47 @@
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>689</v>
+        <v>504</v>
       </c>
       <c r="C361" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C362" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>509</v>
+        <v>689</v>
       </c>
       <c r="C363" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>690</v>
+        <v>507</v>
       </c>
       <c r="C364" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C365" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>513</v>
+        <v>690</v>
       </c>
       <c r="C366" t="s">
         <v>512</v>
@@ -6226,23 +6232,23 @@
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C367" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>691</v>
+        <v>513</v>
       </c>
       <c r="C368" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C369" t="s">
         <v>515</v>
@@ -6250,39 +6256,39 @@
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>517</v>
+        <v>691</v>
       </c>
       <c r="C370" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C371" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>722</v>
+        <v>517</v>
       </c>
       <c r="C372" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>692</v>
+        <v>519</v>
       </c>
       <c r="C373" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>693</v>
+        <v>722</v>
       </c>
       <c r="C374" t="s">
         <v>522</v>
@@ -6290,7 +6296,7 @@
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>521</v>
+        <v>692</v>
       </c>
       <c r="C375" t="s">
         <v>522</v>
@@ -6298,71 +6304,71 @@
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>523</v>
+        <v>693</v>
       </c>
       <c r="C376" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C377" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C378" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="C379" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C380" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C381" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>694</v>
+        <v>531</v>
       </c>
       <c r="C382" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C383" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>536</v>
+        <v>694</v>
       </c>
       <c r="C384" t="s">
         <v>535</v>
@@ -6370,18 +6376,15 @@
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C385" t="s">
         <v>535</v>
       </c>
-      <c r="D385" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C386" t="s">
         <v>535</v>
@@ -6389,47 +6392,50 @@
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C387" t="s">
-        <v>540</v>
+        <v>535</v>
+      </c>
+      <c r="D387" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>723</v>
+        <v>538</v>
       </c>
       <c r="C388" t="s">
-        <v>696</v>
+        <v>535</v>
       </c>
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B389" s="10" t="s">
-        <v>695</v>
+      <c r="B389" t="s">
+        <v>539</v>
       </c>
       <c r="C389" t="s">
-        <v>696</v>
+        <v>540</v>
       </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
+        <v>723</v>
+      </c>
+      <c r="C390" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B391" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="C391" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B392" t="s">
         <v>541</v>
-      </c>
-      <c r="C390" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B391" t="s">
-        <v>724</v>
-      </c>
-      <c r="C391" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="392" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B392" s="11" t="s">
-        <v>697</v>
       </c>
       <c r="C392" t="s">
         <v>542</v>
@@ -6437,263 +6443,263 @@
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>698</v>
+        <v>724</v>
       </c>
       <c r="C393" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B394" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="C394" s="1" t="s">
+    <row r="394" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B394" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="C394" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B395" s="10" t="s">
-        <v>700</v>
+      <c r="B395" t="s">
+        <v>698</v>
       </c>
       <c r="C395" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B396" s="4" t="s">
+      <c r="B396" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B397" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="C397" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B398" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C396" t="s">
+      <c r="C398" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B397" t="s">
-        <v>544</v>
-      </c>
-      <c r="C397" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B398" t="s">
-        <v>701</v>
-      </c>
-      <c r="C398" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C399" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>548</v>
+        <v>701</v>
       </c>
       <c r="C400" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C401" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C402" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>719</v>
+        <v>550</v>
       </c>
       <c r="C403" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C404" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>556</v>
+        <v>719</v>
       </c>
       <c r="C405" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C406" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C407" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C408" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C409" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B410" s="4" t="s">
-        <v>565</v>
+      <c r="B410" t="s">
+        <v>561</v>
       </c>
       <c r="C410" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C411" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B412" t="s">
-        <v>567</v>
+      <c r="B412" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C412" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C413" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C414" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C415" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>702</v>
+        <v>571</v>
       </c>
       <c r="C416" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C417" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>577</v>
+        <v>702</v>
       </c>
       <c r="C418" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B419" s="4" t="s">
-        <v>579</v>
+      <c r="B419" t="s">
+        <v>575</v>
       </c>
       <c r="C419" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C420" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B421" t="s">
-        <v>582</v>
+      <c r="B421" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C421" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C422" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>703</v>
+        <v>582</v>
       </c>
       <c r="C423" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>704</v>
+        <v>584</v>
       </c>
       <c r="C424" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>586</v>
+        <v>703</v>
       </c>
       <c r="C425" t="s">
         <v>587</v>
@@ -6701,7 +6707,7 @@
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>588</v>
+        <v>704</v>
       </c>
       <c r="C426" t="s">
         <v>587</v>
@@ -6709,31 +6715,31 @@
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C427" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B428" s="4" t="s">
-        <v>591</v>
+      <c r="B428" t="s">
+        <v>588</v>
       </c>
       <c r="C428" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C429" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B430" t="s">
-        <v>594</v>
+      <c r="B430" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C430" t="s">
         <v>592</v>
@@ -6741,119 +6747,119 @@
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C431" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="432" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B432" s="11" t="s">
-        <v>705</v>
+    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B432" t="s">
+        <v>594</v>
       </c>
       <c r="C432" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B433" s="10" t="s">
-        <v>706</v>
+      <c r="B433" t="s">
+        <v>595</v>
       </c>
       <c r="C433" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B434" t="s">
-        <v>596</v>
+    <row r="434" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B434" s="11" t="s">
+        <v>705</v>
       </c>
       <c r="C434" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B435" t="s">
-        <v>597</v>
+      <c r="B435" s="10" t="s">
+        <v>706</v>
       </c>
       <c r="C435" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C436" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C437" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C438" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>707</v>
+        <v>600</v>
       </c>
       <c r="C439" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C440" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>605</v>
+        <v>707</v>
       </c>
       <c r="C441" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" s="4" t="s">
-        <v>606</v>
+      <c r="B442" t="s">
+        <v>603</v>
       </c>
       <c r="C442" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B443" s="4" t="s">
+      <c r="B443" t="s">
+        <v>605</v>
+      </c>
+      <c r="C443" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B444" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C444" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B445" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="C443" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B444" t="s">
-        <v>709</v>
-      </c>
-      <c r="C444" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" t="s">
-        <v>607</v>
       </c>
       <c r="C445" t="s">
         <v>608</v>
@@ -6861,47 +6867,47 @@
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C446" t="s">
-        <v>712</v>
+        <v>608</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C447" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>611</v>
+        <v>711</v>
       </c>
       <c r="C448" t="s">
-        <v>612</v>
+        <v>712</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C449" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>710</v>
+        <v>611</v>
       </c>
       <c r="C450" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B451" s="4" t="s">
-        <v>615</v>
+      <c r="B451" t="s">
+        <v>613</v>
       </c>
       <c r="C451" t="s">
         <v>614</v>
@@ -6909,15 +6915,15 @@
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>616</v>
+        <v>710</v>
       </c>
       <c r="C452" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B453" t="s">
-        <v>617</v>
+      <c r="B453" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C453" t="s">
         <v>614</v>
@@ -6925,17 +6931,33 @@
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C454" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
+        <v>617</v>
+      </c>
+      <c r="C455" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B456" t="s">
+        <v>618</v>
+      </c>
+      <c r="C456" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B457" t="s">
         <v>620</v>
       </c>
-      <c r="C455" t="s">
+      <c r="C457" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added scaling with GDP PPP
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Country Code" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1" iterateCount="4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="734">
   <si>
     <t>Country Name</t>
   </si>
@@ -2210,6 +2210,12 @@
   </si>
   <si>
     <t>Serbia &amp; Montenegro</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Islamic Republic of Iran</t>
   </si>
 </sst>
 </file>
@@ -3284,10 +3290,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F457"/>
+  <dimension ref="A1:F459"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="B339" sqref="B339"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="B459" sqref="B459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,31 +4640,31 @@
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>660</v>
-      </c>
-      <c r="C168" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="C168" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>241</v>
-      </c>
-      <c r="C169" t="s">
+        <v>660</v>
+      </c>
+      <c r="C169" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>661</v>
-      </c>
-      <c r="C170" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C170" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>635</v>
+        <v>661</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>242</v>
@@ -4666,23 +4672,23 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
+        <v>635</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
         <v>243</v>
-      </c>
-      <c r="C172" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="173" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B173" s="11" t="s">
-        <v>662</v>
       </c>
       <c r="C173" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>244</v>
+    <row r="174" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B174" s="11" t="s">
+        <v>662</v>
       </c>
       <c r="C174" t="s">
         <v>242</v>
@@ -4690,79 +4696,79 @@
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C175" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
+        <v>245</v>
+      </c>
+      <c r="C176" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
         <v>247</v>
-      </c>
-      <c r="C176" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="C177" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>250</v>
+      <c r="B178" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C178" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C179" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C180" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C181" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C182" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C183" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C184" t="s">
         <v>261</v>
@@ -4770,71 +4776,71 @@
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C185" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C186" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C187" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C188" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C189" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>663</v>
+        <v>271</v>
       </c>
       <c r="C190" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B191" s="11" t="s">
-        <v>713</v>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>663</v>
       </c>
       <c r="C191" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>664</v>
+    <row r="192" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B192" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C192" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="10" t="s">
-        <v>665</v>
+      <c r="B193" t="s">
+        <v>664</v>
       </c>
       <c r="C193" t="s">
         <v>272</v>
@@ -4842,15 +4848,15 @@
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C194" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
-        <v>273</v>
+      <c r="B195" s="10" t="s">
+        <v>666</v>
       </c>
       <c r="C195" t="s">
         <v>272</v>
@@ -4858,23 +4864,23 @@
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>667</v>
+        <v>273</v>
       </c>
       <c r="C196" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>718</v>
+        <v>732</v>
       </c>
       <c r="C197" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B198" s="4" t="s">
-        <v>274</v>
+      <c r="B198" t="s">
+        <v>667</v>
       </c>
       <c r="C198" t="s">
         <v>275</v>
@@ -4882,15 +4888,15 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>668</v>
+        <v>718</v>
       </c>
       <c r="C199" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>276</v>
+      <c r="B200" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
@@ -4898,7 +4904,7 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>636</v>
+        <v>668</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4906,7 +4912,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
@@ -4914,7 +4920,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>278</v>
+        <v>636</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
@@ -4922,7 +4928,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>669</v>
+        <v>277</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4930,7 +4936,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>670</v>
+        <v>278</v>
       </c>
       <c r="C205" t="s">
         <v>275</v>
@@ -4938,55 +4944,55 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>279</v>
+        <v>669</v>
       </c>
       <c r="C206" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>281</v>
+        <v>670</v>
       </c>
       <c r="C207" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B208" s="4" t="s">
-        <v>283</v>
+      <c r="B208" t="s">
+        <v>279</v>
       </c>
       <c r="C208" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C209" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C210" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>286</v>
-      </c>
-      <c r="C210" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>671</v>
+        <v>285</v>
       </c>
       <c r="C211" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B212" s="10" t="s">
-        <v>672</v>
+      <c r="B212" t="s">
+        <v>286</v>
       </c>
       <c r="C212" t="s">
         <v>287</v>
@@ -4994,15 +5000,15 @@
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>288</v>
+        <v>671</v>
       </c>
       <c r="C213" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>673</v>
+      <c r="B214" s="10" t="s">
+        <v>672</v>
       </c>
       <c r="C214" t="s">
         <v>287</v>
@@ -5010,7 +5016,7 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C215" t="s">
         <v>287</v>
@@ -5018,95 +5024,95 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>625</v>
+        <v>673</v>
       </c>
       <c r="C216" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C217" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C218" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C219" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>294</v>
+        <v>626</v>
       </c>
       <c r="C220" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C221" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C222" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C223" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C224" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="225" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B225" s="11" t="s">
-        <v>714</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>300</v>
       </c>
       <c r="C225" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C226" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B227" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C227" t="s">
         <v>305</v>
@@ -5114,87 +5120,87 @@
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C228" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
-        <v>309</v>
+      <c r="B229" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C229" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>630</v>
+        <v>307</v>
       </c>
       <c r="C230" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C231" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>313</v>
+        <v>630</v>
       </c>
       <c r="C232" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C233" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>725</v>
+        <v>313</v>
       </c>
       <c r="C234" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C235" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>674</v>
+        <v>725</v>
       </c>
       <c r="C236" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>675</v>
+        <v>317</v>
       </c>
       <c r="C237" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>319</v>
+        <v>674</v>
       </c>
       <c r="C238" t="s">
         <v>320</v>
@@ -5202,7 +5208,7 @@
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C239" t="s">
         <v>320</v>
@@ -5210,7 +5216,7 @@
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C240" t="s">
         <v>320</v>
@@ -5218,56 +5224,56 @@
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>322</v>
+        <v>676</v>
       </c>
       <c r="C241" t="s">
         <v>320</v>
       </c>
-      <c r="E241" s="4"/>
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C242" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B243" s="4" t="s">
+      <c r="B243" t="s">
+        <v>322</v>
+      </c>
+      <c r="C243" t="s">
+        <v>320</v>
+      </c>
+      <c r="E243" s="4"/>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>323</v>
+      </c>
+      <c r="C244" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="C243" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B244" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="C244" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="245" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B245" s="11" t="s">
-        <v>678</v>
       </c>
       <c r="C245" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B246" t="s">
-        <v>679</v>
+      <c r="B246" s="4" t="s">
+        <v>677</v>
       </c>
       <c r="C246" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B247" t="s">
-        <v>326</v>
+    <row r="247" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B247" s="11" t="s">
+        <v>678</v>
       </c>
       <c r="C247" t="s">
         <v>325</v>
@@ -5275,7 +5281,7 @@
     </row>
     <row r="248" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>327</v>
+        <v>679</v>
       </c>
       <c r="C248" t="s">
         <v>325</v>
@@ -5283,7 +5289,7 @@
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C249" t="s">
         <v>325</v>
@@ -5291,201 +5297,201 @@
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C250" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C251" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C252" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C253" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C254" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C255" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C256" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C257" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C258" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C259" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C260" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C261" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C262" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C263" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>721</v>
+        <v>353</v>
       </c>
       <c r="C264" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B265" s="10" t="s">
-        <v>680</v>
+      <c r="B265" t="s">
+        <v>355</v>
       </c>
       <c r="C265" t="s">
         <v>354</v>
       </c>
-      <c r="F265" s="4"/>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>627</v>
+        <v>721</v>
       </c>
       <c r="C266" t="s">
-        <v>357</v>
-      </c>
-      <c r="F266" s="4"/>
+        <v>354</v>
+      </c>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B267" t="s">
-        <v>356</v>
+      <c r="B267" s="10" t="s">
+        <v>680</v>
       </c>
       <c r="C267" t="s">
-        <v>357</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="F267" s="4"/>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C268" t="s">
-        <v>359</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="F268" s="4"/>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C269" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>360</v>
+        <v>628</v>
       </c>
       <c r="C270" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>681</v>
+        <v>358</v>
       </c>
       <c r="C271" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C272" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C273" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B274" s="4" t="s">
-        <v>364</v>
+      <c r="B274" t="s">
+        <v>362</v>
       </c>
       <c r="C274" t="s">
         <v>363</v>
@@ -5493,287 +5499,287 @@
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>365</v>
+        <v>682</v>
       </c>
       <c r="C275" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B276" t="s">
-        <v>367</v>
+      <c r="B276" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C276" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C277" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C278" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C279" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C280" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C281" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C282" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C283" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C284" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C285" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C286" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B287" s="4" t="s">
-        <v>389</v>
+      <c r="B287" t="s">
+        <v>385</v>
       </c>
       <c r="C287" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C288" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B289" t="s">
-        <v>391</v>
+      <c r="B289" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C289" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C290" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C291" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C292" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C293" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C294" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C295" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C296" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C297" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C298" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C299" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C300" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C301" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C302" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C303" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C304" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C305" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C306" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C307" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>683</v>
+        <v>423</v>
       </c>
       <c r="C308" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C309" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C310" t="s">
         <v>428</v>
@@ -5781,15 +5787,15 @@
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C311" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B312" s="4" t="s">
-        <v>430</v>
+      <c r="B312" t="s">
+        <v>684</v>
       </c>
       <c r="C312" t="s">
         <v>428</v>
@@ -5797,167 +5803,167 @@
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>685</v>
+        <v>429</v>
       </c>
       <c r="C313" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B314" t="s">
-        <v>431</v>
+      <c r="B314" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C314" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>433</v>
+        <v>685</v>
       </c>
       <c r="C315" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C316" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C317" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C318" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C319" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C320" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>631</v>
+        <v>441</v>
       </c>
       <c r="C321" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C322" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>447</v>
+        <v>631</v>
       </c>
       <c r="C323" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C324" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C325" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C326" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C327" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C328" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C329" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C330" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>686</v>
+        <v>458</v>
       </c>
       <c r="C331" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>632</v>
+        <v>460</v>
       </c>
       <c r="C332" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>462</v>
+        <v>686</v>
       </c>
       <c r="C333" t="s">
         <v>463</v>
@@ -5965,7 +5971,7 @@
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>464</v>
+        <v>632</v>
       </c>
       <c r="C334" t="s">
         <v>463</v>
@@ -5973,7 +5979,7 @@
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C335" t="s">
         <v>463</v>
@@ -5981,47 +5987,47 @@
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C336" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="337" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
+        <v>465</v>
+      </c>
+      <c r="C337" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="338" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>466</v>
+      </c>
+      <c r="C338" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="339" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
         <v>468</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C339" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="338" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B338" s="11" t="s">
+    <row r="340" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B340" s="11" t="s">
         <v>731</v>
-      </c>
-      <c r="C338" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="339" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B339" s="11" t="s">
-        <v>715</v>
-      </c>
-      <c r="C339" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="340" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B340" t="s">
-        <v>470</v>
       </c>
       <c r="C340" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="341" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B341" s="4" t="s">
-        <v>472</v>
+    <row r="341" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B341" s="11" t="s">
+        <v>715</v>
       </c>
       <c r="C341" t="s">
         <v>471</v>
@@ -6029,170 +6035,170 @@
     </row>
     <row r="342" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C342" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="343" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B343" t="s">
-        <v>475</v>
+      <c r="B343" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C343" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C344" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="345" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C345" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C346" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="347" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>479</v>
+      </c>
+      <c r="C347" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B347" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C347" t="s">
-        <v>483</v>
-      </c>
-      <c r="E347" s="4"/>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C348" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="349" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B349" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="C349" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="349" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B349" t="s">
-        <v>485</v>
-      </c>
-      <c r="C349" t="s">
-        <v>486</v>
-      </c>
+      <c r="E349" s="4"/>
     </row>
     <row r="350" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C350" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C351" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C352" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C353" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C354" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C355" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C356" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C357" t="s">
-        <v>502</v>
-      </c>
-      <c r="E357" s="4"/>
+        <v>498</v>
+      </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>687</v>
+        <v>499</v>
       </c>
       <c r="C358" t="s">
-        <v>19</v>
-      </c>
-      <c r="E358" s="4"/>
+        <v>500</v>
+      </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C359" t="s">
-        <v>19</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E359" s="4"/>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C360" t="s">
-        <v>505</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E360" s="4"/>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C361" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>506</v>
+        <v>688</v>
       </c>
       <c r="C362" t="s">
         <v>505</v>
@@ -6200,47 +6206,47 @@
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>689</v>
+        <v>504</v>
       </c>
       <c r="C363" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C364" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>509</v>
+        <v>689</v>
       </c>
       <c r="C365" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>690</v>
+        <v>507</v>
       </c>
       <c r="C366" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C367" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>513</v>
+        <v>690</v>
       </c>
       <c r="C368" t="s">
         <v>512</v>
@@ -6248,23 +6254,23 @@
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C369" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>691</v>
+        <v>513</v>
       </c>
       <c r="C370" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C371" t="s">
         <v>515</v>
@@ -6272,39 +6278,39 @@
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>517</v>
+        <v>691</v>
       </c>
       <c r="C372" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C373" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>722</v>
+        <v>517</v>
       </c>
       <c r="C374" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>692</v>
+        <v>519</v>
       </c>
       <c r="C375" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>693</v>
+        <v>722</v>
       </c>
       <c r="C376" t="s">
         <v>522</v>
@@ -6312,7 +6318,7 @@
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>521</v>
+        <v>692</v>
       </c>
       <c r="C377" t="s">
         <v>522</v>
@@ -6320,71 +6326,71 @@
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>523</v>
+        <v>693</v>
       </c>
       <c r="C378" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C379" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C380" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="C381" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C382" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C383" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>694</v>
+        <v>531</v>
       </c>
       <c r="C384" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C385" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>536</v>
+        <v>694</v>
       </c>
       <c r="C386" t="s">
         <v>535</v>
@@ -6392,18 +6398,15 @@
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C387" t="s">
         <v>535</v>
       </c>
-      <c r="D387" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C388" t="s">
         <v>535</v>
@@ -6411,47 +6414,50 @@
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C389" t="s">
-        <v>540</v>
+        <v>535</v>
+      </c>
+      <c r="D389" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>723</v>
+        <v>538</v>
       </c>
       <c r="C390" t="s">
-        <v>696</v>
+        <v>535</v>
       </c>
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B391" s="10" t="s">
-        <v>695</v>
+      <c r="B391" t="s">
+        <v>539</v>
       </c>
       <c r="C391" t="s">
-        <v>696</v>
+        <v>540</v>
       </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
+        <v>723</v>
+      </c>
+      <c r="C392" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B393" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="C393" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B394" t="s">
         <v>541</v>
-      </c>
-      <c r="C392" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B393" t="s">
-        <v>724</v>
-      </c>
-      <c r="C393" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="394" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B394" s="11" t="s">
-        <v>697</v>
       </c>
       <c r="C394" t="s">
         <v>542</v>
@@ -6459,263 +6465,263 @@
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>698</v>
+        <v>724</v>
       </c>
       <c r="C395" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B396" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="C396" s="1" t="s">
+    <row r="396" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B396" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="C396" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B397" s="10" t="s">
-        <v>700</v>
+      <c r="B397" t="s">
+        <v>698</v>
       </c>
       <c r="C397" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B398" s="4" t="s">
+      <c r="B398" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B399" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="C399" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B400" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C398" t="s">
+      <c r="C400" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B399" t="s">
-        <v>544</v>
-      </c>
-      <c r="C399" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B400" t="s">
-        <v>701</v>
-      </c>
-      <c r="C400" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C401" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>548</v>
+        <v>701</v>
       </c>
       <c r="C402" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C403" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C404" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>719</v>
+        <v>550</v>
       </c>
       <c r="C405" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C406" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>556</v>
+        <v>719</v>
       </c>
       <c r="C407" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C408" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C409" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C410" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C411" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B412" s="4" t="s">
-        <v>565</v>
+      <c r="B412" t="s">
+        <v>561</v>
       </c>
       <c r="C412" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C413" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B414" t="s">
-        <v>567</v>
+      <c r="B414" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C414" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C415" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C416" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C417" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>702</v>
+        <v>571</v>
       </c>
       <c r="C418" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C419" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>577</v>
+        <v>702</v>
       </c>
       <c r="C420" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B421" s="4" t="s">
-        <v>579</v>
+      <c r="B421" t="s">
+        <v>575</v>
       </c>
       <c r="C421" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C422" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B423" t="s">
-        <v>582</v>
+      <c r="B423" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C423" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C424" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>703</v>
+        <v>582</v>
       </c>
       <c r="C425" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>704</v>
+        <v>584</v>
       </c>
       <c r="C426" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>586</v>
+        <v>703</v>
       </c>
       <c r="C427" t="s">
         <v>587</v>
@@ -6723,7 +6729,7 @@
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>588</v>
+        <v>704</v>
       </c>
       <c r="C428" t="s">
         <v>587</v>
@@ -6731,31 +6737,31 @@
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C429" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B430" s="4" t="s">
-        <v>591</v>
+      <c r="B430" t="s">
+        <v>588</v>
       </c>
       <c r="C430" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C431" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B432" t="s">
-        <v>594</v>
+      <c r="B432" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C432" t="s">
         <v>592</v>
@@ -6763,119 +6769,119 @@
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C433" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="434" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B434" s="11" t="s">
-        <v>705</v>
+    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B434" t="s">
+        <v>594</v>
       </c>
       <c r="C434" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B435" s="10" t="s">
-        <v>706</v>
+      <c r="B435" t="s">
+        <v>595</v>
       </c>
       <c r="C435" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B436" t="s">
-        <v>596</v>
+    <row r="436" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B436" s="11" t="s">
+        <v>705</v>
       </c>
       <c r="C436" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" t="s">
-        <v>597</v>
+      <c r="B437" s="10" t="s">
+        <v>706</v>
       </c>
       <c r="C437" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C438" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C439" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C440" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>707</v>
+        <v>600</v>
       </c>
       <c r="C441" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C442" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>605</v>
+        <v>707</v>
       </c>
       <c r="C443" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B444" s="4" t="s">
-        <v>606</v>
+      <c r="B444" t="s">
+        <v>603</v>
       </c>
       <c r="C444" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" s="4" t="s">
+      <c r="B445" t="s">
+        <v>605</v>
+      </c>
+      <c r="C445" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B446" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C446" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B447" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="C445" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B446" t="s">
-        <v>709</v>
-      </c>
-      <c r="C446" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" t="s">
-        <v>607</v>
       </c>
       <c r="C447" t="s">
         <v>608</v>
@@ -6883,47 +6889,47 @@
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C448" t="s">
-        <v>712</v>
+        <v>608</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C449" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>611</v>
+        <v>711</v>
       </c>
       <c r="C450" t="s">
-        <v>612</v>
+        <v>712</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C451" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>710</v>
+        <v>611</v>
       </c>
       <c r="C452" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B453" s="4" t="s">
-        <v>615</v>
+      <c r="B453" t="s">
+        <v>613</v>
       </c>
       <c r="C453" t="s">
         <v>614</v>
@@ -6931,15 +6937,15 @@
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>616</v>
+        <v>710</v>
       </c>
       <c r="C454" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B455" t="s">
-        <v>617</v>
+      <c r="B455" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C455" t="s">
         <v>614</v>
@@ -6947,17 +6953,33 @@
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C456" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
+        <v>617</v>
+      </c>
+      <c r="C457" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B458" t="s">
+        <v>618</v>
+      </c>
+      <c r="C458" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B459" t="s">
         <v>620</v>
       </c>
-      <c r="C457" t="s">
+      <c r="C459" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added scaling for net migration data
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="733">
   <si>
     <t>Country Name</t>
   </si>
@@ -1967,9 +1967,6 @@
   </si>
   <si>
     <t>Falkland Islands</t>
-  </si>
-  <si>
-    <t>Polynesia</t>
   </si>
   <si>
     <t>Germany, Federal Republic of</t>
@@ -3290,10 +3287,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F459"/>
+  <dimension ref="A1:F458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="B459" sqref="B459"/>
+    <sheetView tabSelected="1" topLeftCell="A434" workbookViewId="0">
+      <selection activeCell="B458" sqref="B458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3437,7 +3434,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
@@ -3581,7 +3578,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -3797,7 +3794,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C63" t="s">
         <v>105</v>
@@ -3984,7 +3981,7 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C86" t="s">
         <v>131</v>
@@ -4128,7 +4125,7 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C104" t="s">
         <v>157</v>
@@ -4152,7 +4149,7 @@
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C107" t="s">
         <v>159</v>
@@ -4288,7 +4285,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>651</v>
+        <v>180</v>
       </c>
       <c r="C124" t="s">
         <v>181</v>
@@ -4296,31 +4293,31 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C125" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C126" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C127" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C128" t="s">
         <v>187</v>
@@ -4328,23 +4325,23 @@
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C129" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>189</v>
+        <v>651</v>
       </c>
       <c r="C130" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>652</v>
+        <v>191</v>
       </c>
       <c r="C131" t="s">
         <v>192</v>
@@ -4352,167 +4349,167 @@
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C132" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C133" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C134" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C135" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C136" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>201</v>
+        <v>652</v>
       </c>
       <c r="C137" t="s">
-        <v>202</v>
+        <v>653</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>653</v>
+        <v>203</v>
       </c>
       <c r="C138" t="s">
-        <v>654</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C139" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C141" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C142" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C143" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>213</v>
+      <c r="B144" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C144" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="5" t="s">
-        <v>215</v>
+      <c r="B145" t="s">
+        <v>216</v>
       </c>
       <c r="C145" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C146" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C147" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C148" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C149" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C150" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>226</v>
+        <v>716</v>
       </c>
       <c r="C151" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>717</v>
+        <v>654</v>
       </c>
       <c r="C152" t="s">
         <v>229</v>
@@ -4544,7 +4541,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>658</v>
+        <v>634</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4552,7 +4549,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>634</v>
+        <v>228</v>
       </c>
       <c r="C157" t="s">
         <v>229</v>
@@ -4560,7 +4557,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C158" t="s">
         <v>229</v>
@@ -4568,7 +4565,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4576,15 +4573,15 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>231</v>
+        <v>727</v>
       </c>
       <c r="C160" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>728</v>
+        <v>232</v>
       </c>
       <c r="C161" t="s">
         <v>233</v>
@@ -4592,23 +4589,23 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C162" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>234</v>
+      <c r="B163" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="C163" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164" s="6" t="s">
-        <v>236</v>
+      <c r="B164" t="s">
+        <v>238</v>
       </c>
       <c r="C164" t="s">
         <v>237</v>
@@ -4616,55 +4613,55 @@
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>238</v>
-      </c>
-      <c r="C165" t="s">
-        <v>237</v>
+        <v>658</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>659</v>
-      </c>
-      <c r="C166" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C166" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>239</v>
+        <v>732</v>
       </c>
       <c r="C167" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>733</v>
-      </c>
-      <c r="C168" t="s">
+        <v>659</v>
+      </c>
+      <c r="C168" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>660</v>
-      </c>
-      <c r="C169" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C169" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>241</v>
-      </c>
-      <c r="C170" t="s">
+        <v>660</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>661</v>
+        <v>635</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>242</v>
@@ -4672,23 +4669,23 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>635</v>
-      </c>
-      <c r="C172" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C172" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>243</v>
+    <row r="173" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B173" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C173" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="174" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B174" s="11" t="s">
-        <v>662</v>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>244</v>
       </c>
       <c r="C174" t="s">
         <v>242</v>
@@ -4696,79 +4693,79 @@
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C175" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C176" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
-        <v>247</v>
+      <c r="B177" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C177" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" s="4" t="s">
-        <v>249</v>
+      <c r="B178" t="s">
+        <v>250</v>
       </c>
       <c r="C178" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C179" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C180" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C181" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C182" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C183" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C184" t="s">
         <v>261</v>
@@ -4776,70 +4773,70 @@
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C185" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C186" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C188" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C189" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>271</v>
+        <v>662</v>
       </c>
       <c r="C190" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
-        <v>663</v>
+    <row r="191" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B191" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C191" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B192" s="11" t="s">
-        <v>713</v>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>663</v>
       </c>
       <c r="C192" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+      <c r="B193" s="10" t="s">
         <v>664</v>
       </c>
       <c r="C193" t="s">
@@ -4855,8 +4852,8 @@
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B195" s="10" t="s">
-        <v>666</v>
+      <c r="B195" t="s">
+        <v>273</v>
       </c>
       <c r="C195" t="s">
         <v>272</v>
@@ -4864,15 +4861,15 @@
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>273</v>
+        <v>731</v>
       </c>
       <c r="C196" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>732</v>
+        <v>666</v>
       </c>
       <c r="C197" t="s">
         <v>275</v>
@@ -4880,23 +4877,23 @@
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>667</v>
+        <v>717</v>
       </c>
       <c r="C198" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>718</v>
+      <c r="B199" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C199" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="4" t="s">
-        <v>274</v>
+      <c r="B200" t="s">
+        <v>667</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
@@ -4904,7 +4901,7 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>668</v>
+        <v>276</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4912,7 +4909,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>276</v>
+        <v>636</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
@@ -4920,7 +4917,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>636</v>
+        <v>277</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
@@ -4928,7 +4925,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4936,7 +4933,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>278</v>
+        <v>668</v>
       </c>
       <c r="C205" t="s">
         <v>275</v>
@@ -4952,31 +4949,31 @@
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>670</v>
+        <v>279</v>
       </c>
       <c r="C207" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C208" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>281</v>
+      <c r="B209" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="C209" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B210" s="4" t="s">
-        <v>283</v>
+      <c r="B210" t="s">
+        <v>285</v>
       </c>
       <c r="C210" t="s">
         <v>284</v>
@@ -4984,22 +4981,22 @@
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C211" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>286</v>
+        <v>670</v>
       </c>
       <c r="C212" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
+      <c r="B213" s="10" t="s">
         <v>671</v>
       </c>
       <c r="C213" t="s">
@@ -5007,8 +5004,8 @@
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="10" t="s">
-        <v>672</v>
+      <c r="B214" t="s">
+        <v>288</v>
       </c>
       <c r="C214" t="s">
         <v>287</v>
@@ -5016,7 +5013,7 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>288</v>
+        <v>672</v>
       </c>
       <c r="C215" t="s">
         <v>287</v>
@@ -5024,7 +5021,7 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>673</v>
+        <v>289</v>
       </c>
       <c r="C216" t="s">
         <v>287</v>
@@ -5032,15 +5029,15 @@
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>289</v>
+        <v>625</v>
       </c>
       <c r="C217" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>625</v>
+        <v>290</v>
       </c>
       <c r="C218" t="s">
         <v>291</v>
@@ -5048,15 +5045,15 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>290</v>
+        <v>626</v>
       </c>
       <c r="C219" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>626</v>
+        <v>292</v>
       </c>
       <c r="C220" t="s">
         <v>293</v>
@@ -5064,95 +5061,95 @@
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C221" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C222" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C223" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C224" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C225" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>302</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B226" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C226" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="227" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B227" s="11" t="s">
-        <v>714</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>304</v>
       </c>
       <c r="C227" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
-        <v>304</v>
+      <c r="B228" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C228" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" s="4" t="s">
-        <v>306</v>
+      <c r="B229" t="s">
+        <v>307</v>
       </c>
       <c r="C229" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C230" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>309</v>
+        <v>630</v>
       </c>
       <c r="C231" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>630</v>
+        <v>311</v>
       </c>
       <c r="C232" t="s">
         <v>312</v>
@@ -5160,31 +5157,31 @@
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C233" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C234" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>315</v>
+        <v>724</v>
       </c>
       <c r="C235" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>725</v>
+        <v>317</v>
       </c>
       <c r="C236" t="s">
         <v>318</v>
@@ -5192,10 +5189,10 @@
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>317</v>
+        <v>673</v>
       </c>
       <c r="C237" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
@@ -5208,7 +5205,7 @@
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>675</v>
+        <v>319</v>
       </c>
       <c r="C239" t="s">
         <v>320</v>
@@ -5216,7 +5213,7 @@
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>319</v>
+        <v>675</v>
       </c>
       <c r="C240" t="s">
         <v>320</v>
@@ -5224,7 +5221,7 @@
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>676</v>
+        <v>321</v>
       </c>
       <c r="C241" t="s">
         <v>320</v>
@@ -5232,47 +5229,47 @@
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C242" t="s">
         <v>320</v>
       </c>
+      <c r="E242" s="4"/>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C243" t="s">
         <v>320</v>
       </c>
-      <c r="E243" s="4"/>
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B244" t="s">
-        <v>323</v>
+      <c r="B244" s="4" t="s">
+        <v>324</v>
       </c>
       <c r="C244" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B245" s="4" t="s">
-        <v>324</v>
+        <v>676</v>
       </c>
       <c r="C245" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B246" s="4" t="s">
+    <row r="246" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B246" s="11" t="s">
         <v>677</v>
       </c>
       <c r="C246" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="247" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B247" s="11" t="s">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
         <v>678</v>
       </c>
       <c r="C247" t="s">
@@ -5281,7 +5278,7 @@
     </row>
     <row r="248" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>679</v>
+        <v>326</v>
       </c>
       <c r="C248" t="s">
         <v>325</v>
@@ -5289,7 +5286,7 @@
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C249" t="s">
         <v>325</v>
@@ -5297,7 +5294,7 @@
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C250" t="s">
         <v>325</v>
@@ -5305,111 +5302,111 @@
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C251" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C252" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C253" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C254" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C255" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C256" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C257" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C258" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C259" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C260" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C261" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C262" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C263" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C264" t="s">
         <v>354</v>
@@ -5417,49 +5414,49 @@
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>355</v>
+        <v>720</v>
       </c>
       <c r="C265" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B266" t="s">
-        <v>721</v>
+      <c r="B266" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C266" t="s">
         <v>354</v>
       </c>
+      <c r="F266" s="4"/>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B267" s="10" t="s">
-        <v>680</v>
+      <c r="B267" t="s">
+        <v>627</v>
       </c>
       <c r="C267" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F267" s="4"/>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>627</v>
+        <v>356</v>
       </c>
       <c r="C268" t="s">
         <v>357</v>
       </c>
-      <c r="F268" s="4"/>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>356</v>
+        <v>628</v>
       </c>
       <c r="C269" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>628</v>
+        <v>358</v>
       </c>
       <c r="C270" t="s">
         <v>359</v>
@@ -5467,23 +5464,23 @@
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C271" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>360</v>
+        <v>680</v>
       </c>
       <c r="C272" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>681</v>
+        <v>362</v>
       </c>
       <c r="C273" t="s">
         <v>363</v>
@@ -5491,127 +5488,127 @@
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>362</v>
+        <v>681</v>
       </c>
       <c r="C274" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B275" t="s">
-        <v>682</v>
+      <c r="B275" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C275" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B276" s="4" t="s">
-        <v>364</v>
+      <c r="B276" t="s">
+        <v>365</v>
       </c>
       <c r="C276" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C277" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C278" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C279" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C280" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C281" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C282" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C283" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C284" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C285" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C286" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C287" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B288" t="s">
-        <v>387</v>
+      <c r="B288" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C288" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B289" s="4" t="s">
-        <v>389</v>
+      <c r="B289" t="s">
+        <v>390</v>
       </c>
       <c r="C289" t="s">
         <v>388</v>
@@ -5619,63 +5616,63 @@
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C290" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C291" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C292" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C293" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C294" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C295" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C296" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C297" t="s">
         <v>404</v>
@@ -5683,23 +5680,23 @@
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C298" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C299" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C300" t="s">
         <v>409</v>
@@ -5707,79 +5704,79 @@
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C301" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C302" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C303" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C304" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C305" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C306" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C307" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C308" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>425</v>
+        <v>682</v>
       </c>
       <c r="C309" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>683</v>
+        <v>427</v>
       </c>
       <c r="C310" t="s">
         <v>428</v>
@@ -5787,7 +5784,7 @@
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>427</v>
+        <v>683</v>
       </c>
       <c r="C311" t="s">
         <v>428</v>
@@ -5795,31 +5792,31 @@
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>684</v>
+        <v>429</v>
       </c>
       <c r="C312" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B313" t="s">
-        <v>429</v>
+      <c r="B313" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C313" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="4" t="s">
-        <v>430</v>
+      <c r="B314" t="s">
+        <v>684</v>
       </c>
       <c r="C314" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>685</v>
+        <v>431</v>
       </c>
       <c r="C315" t="s">
         <v>432</v>
@@ -5827,63 +5824,63 @@
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C316" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C317" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C318" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C319" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C320" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C321" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>443</v>
+        <v>631</v>
       </c>
       <c r="C322" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>631</v>
+        <v>445</v>
       </c>
       <c r="C323" t="s">
         <v>446</v>
@@ -5891,39 +5888,39 @@
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C324" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C325" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C326" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C327" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C328" t="s">
         <v>454</v>
@@ -5931,39 +5928,39 @@
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C329" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C330" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C331" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>460</v>
+        <v>685</v>
       </c>
       <c r="C332" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>686</v>
+        <v>632</v>
       </c>
       <c r="C333" t="s">
         <v>463</v>
@@ -5971,7 +5968,7 @@
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>632</v>
+        <v>462</v>
       </c>
       <c r="C334" t="s">
         <v>463</v>
@@ -5979,7 +5976,7 @@
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C335" t="s">
         <v>463</v>
@@ -5987,7 +5984,7 @@
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C336" t="s">
         <v>463</v>
@@ -5995,210 +5992,210 @@
     </row>
     <row r="337" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C337" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C338" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="339" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B339" t="s">
-        <v>468</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="339" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B339" s="11" t="s">
+        <v>730</v>
       </c>
       <c r="C339" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="340" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B340" s="11" t="s">
-        <v>731</v>
+        <v>714</v>
       </c>
       <c r="C340" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="341" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B341" s="11" t="s">
-        <v>715</v>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
+        <v>470</v>
       </c>
       <c r="C341" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="342" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B342" t="s">
-        <v>470</v>
+      <c r="B342" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C342" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="343" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B343" s="4" t="s">
-        <v>472</v>
+      <c r="B343" t="s">
+        <v>473</v>
       </c>
       <c r="C343" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C344" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="345" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C345" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C346" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="347" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C347" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B348" t="s">
-        <v>481</v>
+      <c r="B348" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C348" t="s">
-        <v>480</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E348" s="4"/>
     </row>
     <row r="349" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B349" s="4" t="s">
-        <v>482</v>
+      <c r="B349" t="s">
+        <v>484</v>
       </c>
       <c r="C349" t="s">
         <v>483</v>
       </c>
-      <c r="E349" s="4"/>
     </row>
     <row r="350" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C350" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C351" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C352" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C353" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C354" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C355" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C356" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C357" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C358" t="s">
-        <v>500</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E358" s="4"/>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>501</v>
+        <v>686</v>
       </c>
       <c r="C359" t="s">
-        <v>502</v>
+        <v>19</v>
       </c>
       <c r="E359" s="4"/>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>687</v>
+        <v>503</v>
       </c>
       <c r="C360" t="s">
         <v>19</v>
       </c>
-      <c r="E360" s="4"/>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>503</v>
+        <v>687</v>
       </c>
       <c r="C361" t="s">
-        <v>19</v>
+        <v>505</v>
       </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>688</v>
+        <v>504</v>
       </c>
       <c r="C362" t="s">
         <v>505</v>
@@ -6206,7 +6203,7 @@
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C363" t="s">
         <v>505</v>
@@ -6214,15 +6211,15 @@
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>506</v>
+        <v>688</v>
       </c>
       <c r="C364" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>689</v>
+        <v>507</v>
       </c>
       <c r="C365" t="s">
         <v>508</v>
@@ -6230,23 +6227,23 @@
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C366" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>509</v>
+        <v>689</v>
       </c>
       <c r="C367" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>690</v>
+        <v>511</v>
       </c>
       <c r="C368" t="s">
         <v>512</v>
@@ -6254,7 +6251,7 @@
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C369" t="s">
         <v>512</v>
@@ -6262,15 +6259,15 @@
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C370" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>514</v>
+        <v>690</v>
       </c>
       <c r="C371" t="s">
         <v>515</v>
@@ -6278,7 +6275,7 @@
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>691</v>
+        <v>516</v>
       </c>
       <c r="C372" t="s">
         <v>515</v>
@@ -6286,31 +6283,31 @@
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C373" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C374" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>519</v>
+        <v>721</v>
       </c>
       <c r="C375" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>722</v>
+        <v>691</v>
       </c>
       <c r="C376" t="s">
         <v>522</v>
@@ -6326,7 +6323,7 @@
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>693</v>
+        <v>521</v>
       </c>
       <c r="C378" t="s">
         <v>522</v>
@@ -6334,47 +6331,47 @@
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C379" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C380" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C381" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C382" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C383" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C384" t="s">
         <v>532</v>
@@ -6382,15 +6379,15 @@
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>533</v>
+        <v>693</v>
       </c>
       <c r="C385" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>694</v>
+        <v>534</v>
       </c>
       <c r="C386" t="s">
         <v>535</v>
@@ -6398,7 +6395,7 @@
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C387" t="s">
         <v>535</v>
@@ -6406,73 +6403,73 @@
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C388" t="s">
         <v>535</v>
       </c>
+      <c r="D388" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C389" t="s">
         <v>535</v>
       </c>
-      <c r="D389" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C390" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>539</v>
+        <v>722</v>
       </c>
       <c r="C391" t="s">
-        <v>540</v>
+        <v>695</v>
       </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B392" t="s">
-        <v>723</v>
+      <c r="B392" s="10" t="s">
+        <v>694</v>
       </c>
       <c r="C392" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B393" s="10" t="s">
-        <v>695</v>
+      <c r="B393" t="s">
+        <v>541</v>
       </c>
       <c r="C393" t="s">
-        <v>696</v>
+        <v>542</v>
       </c>
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>541</v>
+        <v>723</v>
       </c>
       <c r="C394" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B395" t="s">
-        <v>724</v>
+    <row r="395" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B395" s="11" t="s">
+        <v>696</v>
       </c>
       <c r="C395" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="396" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B396" s="11" t="s">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B396" t="s">
         <v>697</v>
       </c>
       <c r="C396" t="s">
@@ -6480,48 +6477,48 @@
       </c>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B397" t="s">
+      <c r="B397" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C397" t="s">
+      <c r="C397" s="1" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B398" s="1" t="s">
+      <c r="B398" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="C398" s="1" t="s">
+      <c r="C398" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B399" s="10" t="s">
-        <v>700</v>
+      <c r="B399" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C399" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B400" s="4" t="s">
-        <v>543</v>
+      <c r="B400" t="s">
+        <v>544</v>
       </c>
       <c r="C400" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>544</v>
+        <v>700</v>
       </c>
       <c r="C401" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>701</v>
+        <v>546</v>
       </c>
       <c r="C402" t="s">
         <v>547</v>
@@ -6529,31 +6526,31 @@
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C403" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C404" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C405" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>552</v>
+        <v>718</v>
       </c>
       <c r="C406" t="s">
         <v>553</v>
@@ -6561,15 +6558,15 @@
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>719</v>
+        <v>554</v>
       </c>
       <c r="C407" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C408" t="s">
         <v>555</v>
@@ -6577,47 +6574,47 @@
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C409" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C410" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C411" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C412" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B413" t="s">
-        <v>563</v>
+      <c r="B413" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C413" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B414" s="4" t="s">
-        <v>565</v>
+      <c r="B414" t="s">
+        <v>566</v>
       </c>
       <c r="C414" t="s">
         <v>564</v>
@@ -6625,47 +6622,47 @@
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C415" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C416" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C417" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C418" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>573</v>
+        <v>701</v>
       </c>
       <c r="C419" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>702</v>
+        <v>575</v>
       </c>
       <c r="C420" t="s">
         <v>576</v>
@@ -6673,50 +6670,50 @@
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C421" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B422" t="s">
-        <v>577</v>
+      <c r="B422" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C422" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B423" s="4" t="s">
-        <v>579</v>
+      <c r="B423" t="s">
+        <v>580</v>
       </c>
       <c r="C423" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C424" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C425" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>584</v>
+        <v>702</v>
       </c>
       <c r="C426" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
@@ -6729,7 +6726,7 @@
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>704</v>
+        <v>586</v>
       </c>
       <c r="C428" t="s">
         <v>587</v>
@@ -6737,7 +6734,7 @@
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C429" t="s">
         <v>587</v>
@@ -6745,23 +6742,23 @@
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C430" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B431" t="s">
-        <v>589</v>
+      <c r="B431" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C431" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B432" s="4" t="s">
-        <v>591</v>
+      <c r="B432" t="s">
+        <v>593</v>
       </c>
       <c r="C432" t="s">
         <v>592</v>
@@ -6769,7 +6766,7 @@
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C433" t="s">
         <v>592</v>
@@ -6777,22 +6774,22 @@
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C434" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B435" t="s">
-        <v>595</v>
+    <row r="435" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B435" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C435" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="436" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B436" s="11" t="s">
+    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B436" s="10" t="s">
         <v>705</v>
       </c>
       <c r="C436" t="s">
@@ -6800,8 +6797,8 @@
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" s="10" t="s">
-        <v>706</v>
+      <c r="B437" t="s">
+        <v>596</v>
       </c>
       <c r="C437" t="s">
         <v>592</v>
@@ -6809,15 +6806,15 @@
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C438" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C439" t="s">
         <v>598</v>
@@ -6825,15 +6822,15 @@
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C440" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C441" t="s">
         <v>601</v>
@@ -6841,15 +6838,15 @@
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>602</v>
+        <v>706</v>
       </c>
       <c r="C442" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>707</v>
+        <v>603</v>
       </c>
       <c r="C443" t="s">
         <v>604</v>
@@ -6857,15 +6854,15 @@
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C444" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" t="s">
-        <v>605</v>
+      <c r="B445" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C445" t="s">
         <v>604</v>
@@ -6873,14 +6870,14 @@
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" s="4" t="s">
-        <v>606</v>
+        <v>707</v>
       </c>
       <c r="C446" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" s="4" t="s">
+      <c r="B447" t="s">
         <v>708</v>
       </c>
       <c r="C447" t="s">
@@ -6889,7 +6886,7 @@
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>709</v>
+        <v>607</v>
       </c>
       <c r="C448" t="s">
         <v>608</v>
@@ -6897,55 +6894,55 @@
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>607</v>
+        <v>710</v>
       </c>
       <c r="C449" t="s">
-        <v>608</v>
+        <v>711</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>711</v>
+        <v>609</v>
       </c>
       <c r="C450" t="s">
-        <v>712</v>
+        <v>610</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C451" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C452" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>613</v>
+        <v>709</v>
       </c>
       <c r="C453" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B454" t="s">
-        <v>710</v>
+      <c r="B454" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C454" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B455" s="4" t="s">
-        <v>615</v>
+      <c r="B455" t="s">
+        <v>616</v>
       </c>
       <c r="C455" t="s">
         <v>614</v>
@@ -6953,7 +6950,7 @@
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C456" t="s">
         <v>614</v>
@@ -6961,25 +6958,17 @@
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C457" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C458" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B459" t="s">
-        <v>620</v>
-      </c>
-      <c r="C459" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added first version of the ILO PDF converted data cleaning
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Country Code" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1" iterateCount="4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="736">
   <si>
     <t>Country Name</t>
   </si>
@@ -2216,6 +2216,12 @@
   </si>
   <si>
     <t>Dem. Rep. Congo</t>
+  </si>
+  <si>
+    <t>lao</t>
+  </si>
+  <si>
+    <t>Chinese Taipei</t>
   </si>
 </sst>
 </file>
@@ -3290,10 +3296,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F459"/>
+  <dimension ref="A1:F461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="C389" sqref="C389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5024,7 +5030,7 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>672</v>
+        <v>734</v>
       </c>
       <c r="C216" t="s">
         <v>287</v>
@@ -5032,7 +5038,7 @@
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>289</v>
+        <v>672</v>
       </c>
       <c r="C217" t="s">
         <v>287</v>
@@ -5040,15 +5046,15 @@
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>625</v>
+        <v>289</v>
       </c>
       <c r="C218" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>290</v>
+        <v>625</v>
       </c>
       <c r="C219" t="s">
         <v>291</v>
@@ -5056,15 +5062,15 @@
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>626</v>
+        <v>290</v>
       </c>
       <c r="C220" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>292</v>
+        <v>626</v>
       </c>
       <c r="C221" t="s">
         <v>293</v>
@@ -5072,95 +5078,95 @@
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C222" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C223" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C224" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C225" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
+        <v>300</v>
+      </c>
+      <c r="C226" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
         <v>302</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C227" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="227" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B227" s="11" t="s">
+    <row r="228" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B228" s="11" t="s">
         <v>713</v>
-      </c>
-      <c r="C227" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
-        <v>304</v>
       </c>
       <c r="C228" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" s="4" t="s">
-        <v>306</v>
+      <c r="B229" t="s">
+        <v>304</v>
       </c>
       <c r="C229" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B230" t="s">
-        <v>307</v>
+      <c r="B230" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C230" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C231" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>630</v>
+        <v>309</v>
       </c>
       <c r="C232" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>311</v>
+        <v>630</v>
       </c>
       <c r="C233" t="s">
         <v>312</v>
@@ -5168,31 +5174,31 @@
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C234" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C235" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>724</v>
+        <v>315</v>
       </c>
       <c r="C236" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>317</v>
+        <v>724</v>
       </c>
       <c r="C237" t="s">
         <v>318</v>
@@ -5200,15 +5206,15 @@
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>673</v>
+        <v>317</v>
       </c>
       <c r="C238" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C239" t="s">
         <v>320</v>
@@ -5216,7 +5222,7 @@
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>319</v>
+        <v>674</v>
       </c>
       <c r="C240" t="s">
         <v>320</v>
@@ -5224,7 +5230,7 @@
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>675</v>
+        <v>319</v>
       </c>
       <c r="C241" t="s">
         <v>320</v>
@@ -5232,7 +5238,7 @@
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>321</v>
+        <v>675</v>
       </c>
       <c r="C242" t="s">
         <v>320</v>
@@ -5240,48 +5246,48 @@
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C243" t="s">
         <v>320</v>
       </c>
-      <c r="E243" s="4"/>
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C244" t="s">
         <v>320</v>
       </c>
+      <c r="E244" s="4"/>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B245" s="4" t="s">
-        <v>324</v>
+      <c r="B245" t="s">
+        <v>323</v>
       </c>
       <c r="C245" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" s="4" t="s">
-        <v>676</v>
+        <v>324</v>
       </c>
       <c r="C246" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="247" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B247" s="11" t="s">
-        <v>677</v>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C247" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B248" t="s">
-        <v>678</v>
+    <row r="248" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B248" s="11" t="s">
+        <v>677</v>
       </c>
       <c r="C248" t="s">
         <v>325</v>
@@ -5289,7 +5295,7 @@
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>326</v>
+        <v>678</v>
       </c>
       <c r="C249" t="s">
         <v>325</v>
@@ -5297,7 +5303,7 @@
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C250" t="s">
         <v>325</v>
@@ -5305,7 +5311,7 @@
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C251" t="s">
         <v>325</v>
@@ -5313,111 +5319,111 @@
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C252" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C253" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C254" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C255" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C256" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C257" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C258" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C259" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C260" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C261" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C262" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C263" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C264" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C265" t="s">
         <v>354</v>
@@ -5425,49 +5431,49 @@
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>720</v>
+        <v>355</v>
       </c>
       <c r="C266" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B267" s="10" t="s">
-        <v>679</v>
+      <c r="B267" t="s">
+        <v>720</v>
       </c>
       <c r="C267" t="s">
         <v>354</v>
       </c>
-      <c r="F267" s="4"/>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B268" t="s">
-        <v>627</v>
+      <c r="B268" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C268" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F268" s="4"/>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>356</v>
+        <v>627</v>
       </c>
       <c r="C269" t="s">
         <v>357</v>
       </c>
+      <c r="F269" s="4"/>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>628</v>
+        <v>356</v>
       </c>
       <c r="C270" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>358</v>
+        <v>628</v>
       </c>
       <c r="C271" t="s">
         <v>359</v>
@@ -5475,23 +5481,23 @@
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C272" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>680</v>
+        <v>360</v>
       </c>
       <c r="C273" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>362</v>
+        <v>680</v>
       </c>
       <c r="C274" t="s">
         <v>363</v>
@@ -5499,127 +5505,127 @@
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>681</v>
+        <v>362</v>
       </c>
       <c r="C275" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B276" s="4" t="s">
-        <v>364</v>
+      <c r="B276" t="s">
+        <v>681</v>
       </c>
       <c r="C276" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B277" t="s">
-        <v>365</v>
+      <c r="B277" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C277" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C278" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C279" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C280" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C281" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C282" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C283" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C284" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C285" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C286" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C287" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
+        <v>385</v>
+      </c>
+      <c r="C288" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B289" t="s">
         <v>387</v>
-      </c>
-      <c r="C288" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B289" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="C289" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B290" t="s">
-        <v>390</v>
+      <c r="B290" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C290" t="s">
         <v>388</v>
@@ -5627,63 +5633,63 @@
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C291" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C292" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C293" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C294" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C295" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C296" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C297" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C298" t="s">
         <v>404</v>
@@ -5691,23 +5697,23 @@
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C299" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C300" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C301" t="s">
         <v>409</v>
@@ -5715,79 +5721,79 @@
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C302" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C303" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C304" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C305" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C306" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C307" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C308" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C309" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>682</v>
+        <v>425</v>
       </c>
       <c r="C310" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>427</v>
+        <v>682</v>
       </c>
       <c r="C311" t="s">
         <v>428</v>
@@ -5795,7 +5801,7 @@
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>683</v>
+        <v>427</v>
       </c>
       <c r="C312" t="s">
         <v>428</v>
@@ -5803,31 +5809,31 @@
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>429</v>
+        <v>683</v>
       </c>
       <c r="C313" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="4" t="s">
-        <v>430</v>
+      <c r="B314" t="s">
+        <v>429</v>
       </c>
       <c r="C314" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B315" t="s">
-        <v>684</v>
+      <c r="B315" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C315" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>431</v>
+        <v>684</v>
       </c>
       <c r="C316" t="s">
         <v>432</v>
@@ -5835,63 +5841,63 @@
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C317" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C318" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C319" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C320" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C321" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C322" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>631</v>
+        <v>443</v>
       </c>
       <c r="C323" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>445</v>
+        <v>631</v>
       </c>
       <c r="C324" t="s">
         <v>446</v>
@@ -5899,39 +5905,39 @@
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C325" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C326" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C327" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C328" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C329" t="s">
         <v>454</v>
@@ -5939,39 +5945,39 @@
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C330" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C331" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C332" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>685</v>
+        <v>460</v>
       </c>
       <c r="C333" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>632</v>
+        <v>685</v>
       </c>
       <c r="C334" t="s">
         <v>463</v>
@@ -5979,7 +5985,7 @@
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>462</v>
+        <v>632</v>
       </c>
       <c r="C335" t="s">
         <v>463</v>
@@ -5987,7 +5993,7 @@
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C336" t="s">
         <v>463</v>
@@ -5995,7 +6001,7 @@
     </row>
     <row r="337" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C337" t="s">
         <v>463</v>
@@ -6003,210 +6009,210 @@
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C338" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="339" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
+        <v>466</v>
+      </c>
+      <c r="C339" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="340" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
         <v>468</v>
       </c>
-      <c r="C339" t="s">
+      <c r="C340" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="340" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B340" s="11" t="s">
-        <v>730</v>
-      </c>
-      <c r="C340" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="341" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B341" s="11" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="C341" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="342" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B342" t="s">
-        <v>470</v>
+    <row r="342" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B342" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C342" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="343" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B343" s="4" t="s">
-        <v>472</v>
+      <c r="B343" t="s">
+        <v>470</v>
       </c>
       <c r="C343" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B344" t="s">
-        <v>473</v>
+      <c r="B344" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C344" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="345" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C345" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C346" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="347" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C347" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C348" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="349" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B349" s="4" t="s">
+      <c r="B349" t="s">
+        <v>481</v>
+      </c>
+      <c r="C349" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="350" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B350" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="C349" t="s">
-        <v>483</v>
-      </c>
-      <c r="E349" s="4"/>
-    </row>
-    <row r="350" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B350" t="s">
-        <v>484</v>
       </c>
       <c r="C350" t="s">
         <v>483</v>
       </c>
+      <c r="E350" s="4"/>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C351" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C352" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C353" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C354" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C355" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C356" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C357" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C358" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C359" t="s">
-        <v>502</v>
-      </c>
-      <c r="E359" s="4"/>
+        <v>500</v>
+      </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>686</v>
+        <v>501</v>
       </c>
       <c r="C360" t="s">
-        <v>19</v>
+        <v>502</v>
       </c>
       <c r="E360" s="4"/>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>503</v>
+        <v>686</v>
       </c>
       <c r="C361" t="s">
         <v>19</v>
       </c>
+      <c r="E361" s="4"/>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>687</v>
+        <v>503</v>
       </c>
       <c r="C362" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>504</v>
+        <v>687</v>
       </c>
       <c r="C363" t="s">
         <v>505</v>
@@ -6214,7 +6220,7 @@
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C364" t="s">
         <v>505</v>
@@ -6222,15 +6228,15 @@
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>688</v>
+        <v>506</v>
       </c>
       <c r="C365" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>507</v>
+        <v>688</v>
       </c>
       <c r="C366" t="s">
         <v>508</v>
@@ -6238,23 +6244,23 @@
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C367" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>689</v>
+        <v>509</v>
       </c>
       <c r="C368" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>511</v>
+        <v>689</v>
       </c>
       <c r="C369" t="s">
         <v>512</v>
@@ -6262,7 +6268,7 @@
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C370" t="s">
         <v>512</v>
@@ -6270,15 +6276,15 @@
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C371" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>690</v>
+        <v>514</v>
       </c>
       <c r="C372" t="s">
         <v>515</v>
@@ -6286,7 +6292,7 @@
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>516</v>
+        <v>690</v>
       </c>
       <c r="C373" t="s">
         <v>515</v>
@@ -6294,31 +6300,31 @@
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C374" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C375" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>721</v>
+        <v>519</v>
       </c>
       <c r="C376" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="C377" t="s">
         <v>522</v>
@@ -6326,7 +6332,7 @@
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C378" t="s">
         <v>522</v>
@@ -6334,7 +6340,7 @@
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>521</v>
+        <v>692</v>
       </c>
       <c r="C379" t="s">
         <v>522</v>
@@ -6342,47 +6348,47 @@
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C380" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C381" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C382" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C383" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C384" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C385" t="s">
         <v>532</v>
@@ -6390,15 +6396,15 @@
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>693</v>
+        <v>533</v>
       </c>
       <c r="C386" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>534</v>
+        <v>693</v>
       </c>
       <c r="C387" t="s">
         <v>535</v>
@@ -6406,7 +6412,7 @@
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>536</v>
+        <v>735</v>
       </c>
       <c r="C388" t="s">
         <v>535</v>
@@ -6414,18 +6420,15 @@
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C389" t="s">
         <v>535</v>
       </c>
-      <c r="D389" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C390" t="s">
         <v>535</v>
@@ -6433,47 +6436,50 @@
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C391" t="s">
-        <v>540</v>
+        <v>535</v>
+      </c>
+      <c r="D391" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>722</v>
+        <v>538</v>
       </c>
       <c r="C392" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B393" s="10" t="s">
-        <v>694</v>
+      <c r="B393" t="s">
+        <v>539</v>
       </c>
       <c r="C393" t="s">
-        <v>695</v>
+        <v>540</v>
       </c>
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
+        <v>722</v>
+      </c>
+      <c r="C394" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B395" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="C395" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B396" t="s">
         <v>541</v>
-      </c>
-      <c r="C394" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B395" t="s">
-        <v>723</v>
-      </c>
-      <c r="C395" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="396" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B396" s="11" t="s">
-        <v>696</v>
       </c>
       <c r="C396" t="s">
         <v>542</v>
@@ -6481,263 +6487,263 @@
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>697</v>
+        <v>723</v>
       </c>
       <c r="C397" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B398" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="C398" s="1" t="s">
+    <row r="398" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B398" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="C398" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B399" s="10" t="s">
-        <v>699</v>
+      <c r="B399" t="s">
+        <v>697</v>
       </c>
       <c r="C399" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B400" s="4" t="s">
+      <c r="B400" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="C401" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C400" t="s">
+      <c r="C402" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B401" t="s">
-        <v>544</v>
-      </c>
-      <c r="C401" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B402" t="s">
-        <v>700</v>
-      </c>
-      <c r="C402" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C403" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>548</v>
+        <v>700</v>
       </c>
       <c r="C404" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C405" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C406" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>718</v>
+        <v>550</v>
       </c>
       <c r="C407" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C408" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>556</v>
+        <v>718</v>
       </c>
       <c r="C409" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C410" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C411" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C412" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C413" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B414" s="4" t="s">
-        <v>565</v>
+      <c r="B414" t="s">
+        <v>561</v>
       </c>
       <c r="C414" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C415" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B416" t="s">
-        <v>567</v>
+      <c r="B416" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C416" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C417" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C418" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C419" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>701</v>
+        <v>571</v>
       </c>
       <c r="C420" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C421" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>577</v>
+        <v>701</v>
       </c>
       <c r="C422" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B423" s="4" t="s">
-        <v>579</v>
+      <c r="B423" t="s">
+        <v>575</v>
       </c>
       <c r="C423" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C424" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B425" t="s">
-        <v>582</v>
+      <c r="B425" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C425" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C426" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>702</v>
+        <v>582</v>
       </c>
       <c r="C427" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>703</v>
+        <v>584</v>
       </c>
       <c r="C428" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>586</v>
+        <v>702</v>
       </c>
       <c r="C429" t="s">
         <v>587</v>
@@ -6745,7 +6751,7 @@
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>588</v>
+        <v>703</v>
       </c>
       <c r="C430" t="s">
         <v>587</v>
@@ -6753,31 +6759,31 @@
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C431" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B432" s="4" t="s">
-        <v>591</v>
+      <c r="B432" t="s">
+        <v>588</v>
       </c>
       <c r="C432" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C433" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B434" t="s">
-        <v>594</v>
+      <c r="B434" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C434" t="s">
         <v>592</v>
@@ -6785,119 +6791,119 @@
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C435" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="436" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B436" s="11" t="s">
-        <v>704</v>
+    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B436" t="s">
+        <v>594</v>
       </c>
       <c r="C436" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" s="10" t="s">
-        <v>705</v>
+      <c r="B437" t="s">
+        <v>595</v>
       </c>
       <c r="C437" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B438" t="s">
-        <v>596</v>
+    <row r="438" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B438" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C438" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B439" t="s">
-        <v>597</v>
+      <c r="B439" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C439" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C440" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C441" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C442" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>706</v>
+        <v>600</v>
       </c>
       <c r="C443" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C444" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>605</v>
+        <v>706</v>
       </c>
       <c r="C445" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B446" s="4" t="s">
-        <v>606</v>
+      <c r="B446" t="s">
+        <v>603</v>
       </c>
       <c r="C446" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" s="4" t="s">
+      <c r="B447" t="s">
+        <v>605</v>
+      </c>
+      <c r="C447" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B448" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C448" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B449" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="C447" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B448" t="s">
-        <v>708</v>
-      </c>
-      <c r="C448" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B449" t="s">
-        <v>607</v>
       </c>
       <c r="C449" t="s">
         <v>608</v>
@@ -6905,47 +6911,47 @@
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C450" t="s">
-        <v>711</v>
+        <v>608</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C451" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>611</v>
+        <v>710</v>
       </c>
       <c r="C452" t="s">
-        <v>612</v>
+        <v>711</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C453" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>709</v>
+        <v>611</v>
       </c>
       <c r="C454" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B455" s="4" t="s">
-        <v>615</v>
+      <c r="B455" t="s">
+        <v>613</v>
       </c>
       <c r="C455" t="s">
         <v>614</v>
@@ -6953,15 +6959,15 @@
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>616</v>
+        <v>709</v>
       </c>
       <c r="C456" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B457" t="s">
-        <v>617</v>
+      <c r="B457" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C457" t="s">
         <v>614</v>
@@ -6969,17 +6975,33 @@
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C458" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
+        <v>617</v>
+      </c>
+      <c r="C459" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B460" t="s">
+        <v>618</v>
+      </c>
+      <c r="C460" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B461" t="s">
         <v>620</v>
       </c>
-      <c r="C459" t="s">
+      <c r="C461" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more data for PISA
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Country Code" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="740">
   <si>
     <t>Country Name</t>
   </si>
@@ -2228,6 +2228,12 @@
   </si>
   <si>
     <t>Utd. Arab Em.</t>
+  </si>
+  <si>
+    <t>dubai (uae)</t>
+  </si>
+  <si>
+    <t>cyprus1,2</t>
   </si>
 </sst>
 </file>
@@ -3302,10 +3308,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F463"/>
+  <dimension ref="A1:F465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="C421" sqref="C421"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3988,7 +3994,7 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>126</v>
+        <v>739</v>
       </c>
       <c r="C85" t="s">
         <v>127</v>
@@ -3996,23 +4002,23 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C86" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>728</v>
+        <v>128</v>
       </c>
       <c r="C87" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>130</v>
+        <v>728</v>
       </c>
       <c r="C88" t="s">
         <v>131</v>
@@ -4020,55 +4026,55 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C90" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C91" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C92" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
-        <v>139</v>
+      <c r="B93" t="s">
+        <v>138</v>
       </c>
       <c r="C93" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>622</v>
+      <c r="B94" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C95" t="s">
         <v>141</v>
@@ -4076,15 +4082,15 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C96" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C97" t="s">
         <v>143</v>
@@ -4092,23 +4098,23 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C99" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C100" t="s">
         <v>147</v>
@@ -4116,7 +4122,7 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C101" t="s">
         <v>147</v>
@@ -4124,55 +4130,55 @@
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C102" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C103" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C104" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>726</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>156</v>
+        <v>726</v>
       </c>
       <c r="C106" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="12" t="s">
+      <c r="B107" t="s">
+        <v>156</v>
+      </c>
+      <c r="C107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="12" t="s">
         <v>648</v>
-      </c>
-      <c r="C107" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>719</v>
       </c>
       <c r="C108" t="s">
         <v>159</v>
@@ -4180,7 +4186,7 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>649</v>
+        <v>719</v>
       </c>
       <c r="C109" t="s">
         <v>159</v>
@@ -4188,7 +4194,7 @@
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>158</v>
+        <v>649</v>
       </c>
       <c r="C110" t="s">
         <v>159</v>
@@ -4196,23 +4202,23 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C111" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>624</v>
+        <v>160</v>
       </c>
       <c r="C112" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>162</v>
+        <v>624</v>
       </c>
       <c r="C113" t="s">
         <v>163</v>
@@ -4220,15 +4226,15 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>629</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>164</v>
+        <v>629</v>
       </c>
       <c r="C115" t="s">
         <v>165</v>
@@ -4236,23 +4242,23 @@
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C116" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C117" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C118" t="s">
         <v>169</v>
@@ -4260,15 +4266,15 @@
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>650</v>
+        <v>170</v>
       </c>
       <c r="C119" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>171</v>
+        <v>650</v>
       </c>
       <c r="C120" t="s">
         <v>172</v>
@@ -4276,7 +4282,7 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C121" t="s">
         <v>172</v>
@@ -4284,63 +4290,63 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C122" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C123" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C124" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C125" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C126" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C127" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C128" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C129" t="s">
         <v>187</v>
@@ -4348,23 +4354,23 @@
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C130" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>651</v>
+        <v>189</v>
       </c>
       <c r="C131" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>191</v>
+        <v>651</v>
       </c>
       <c r="C132" t="s">
         <v>192</v>
@@ -4372,167 +4378,167 @@
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C133" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C134" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C135" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C136" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C137" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>652</v>
+        <v>201</v>
       </c>
       <c r="C138" t="s">
-        <v>653</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>203</v>
+        <v>652</v>
       </c>
       <c r="C139" t="s">
-        <v>204</v>
+        <v>653</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C140" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C141" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C142" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C143" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
+        <v>211</v>
+      </c>
+      <c r="C144" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
         <v>213</v>
-      </c>
-      <c r="C144" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C145" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>216</v>
+      <c r="B146" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C146" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C147" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C148" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C149" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C150" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C151" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>716</v>
+        <v>226</v>
       </c>
       <c r="C152" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>654</v>
+        <v>716</v>
       </c>
       <c r="C153" t="s">
         <v>229</v>
@@ -4540,7 +4546,7 @@
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C154" t="s">
         <v>229</v>
@@ -4548,7 +4554,7 @@
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C155" t="s">
         <v>229</v>
@@ -4556,7 +4562,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4564,7 +4570,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>634</v>
+        <v>657</v>
       </c>
       <c r="C157" t="s">
         <v>229</v>
@@ -4572,7 +4578,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>228</v>
+        <v>634</v>
       </c>
       <c r="C158" t="s">
         <v>229</v>
@@ -4580,7 +4586,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4588,7 +4594,7 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C160" t="s">
         <v>229</v>
@@ -4596,15 +4602,15 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>727</v>
+        <v>231</v>
       </c>
       <c r="C161" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>232</v>
+        <v>727</v>
       </c>
       <c r="C162" t="s">
         <v>233</v>
@@ -4612,23 +4618,23 @@
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
+        <v>232</v>
+      </c>
+      <c r="C163" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
         <v>234</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164" s="6" t="s">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="C164" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>238</v>
       </c>
       <c r="C165" t="s">
         <v>237</v>
@@ -4636,55 +4642,55 @@
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>658</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
+      </c>
+      <c r="C166" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>239</v>
-      </c>
-      <c r="C167" t="s">
+        <v>658</v>
+      </c>
+      <c r="C167" s="7" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>732</v>
+        <v>239</v>
       </c>
       <c r="C168" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>659</v>
-      </c>
-      <c r="C169" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="C169" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>241</v>
-      </c>
-      <c r="C170" t="s">
+        <v>659</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>660</v>
-      </c>
-      <c r="C171" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C171" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>635</v>
+        <v>660</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>242</v>
@@ -4692,23 +4698,23 @@
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
+        <v>635</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
         <v>243</v>
-      </c>
-      <c r="C173" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="174" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B174" s="11" t="s">
-        <v>661</v>
       </c>
       <c r="C174" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>244</v>
+    <row r="175" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B175" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C175" t="s">
         <v>242</v>
@@ -4716,79 +4722,79 @@
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C176" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
+        <v>245</v>
+      </c>
+      <c r="C177" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
         <v>247</v>
-      </c>
-      <c r="C177" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="C178" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>250</v>
+      <c r="B179" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C179" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C180" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C181" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C182" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C183" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C184" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C185" t="s">
         <v>261</v>
@@ -4796,71 +4802,71 @@
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C186" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C188" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C189" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C190" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>662</v>
+        <v>271</v>
       </c>
       <c r="C191" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B192" s="11" t="s">
-        <v>712</v>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>662</v>
       </c>
       <c r="C192" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>663</v>
+    <row r="193" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B193" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C193" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B194" s="10" t="s">
-        <v>664</v>
+      <c r="B194" t="s">
+        <v>663</v>
       </c>
       <c r="C194" t="s">
         <v>272</v>
@@ -4868,15 +4874,15 @@
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C195" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
-        <v>273</v>
+      <c r="B196" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C196" t="s">
         <v>272</v>
@@ -4884,15 +4890,15 @@
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>731</v>
+        <v>273</v>
       </c>
       <c r="C197" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>666</v>
+        <v>731</v>
       </c>
       <c r="C198" t="s">
         <v>275</v>
@@ -4900,23 +4906,23 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>717</v>
+        <v>666</v>
       </c>
       <c r="C199" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="4" t="s">
-        <v>274</v>
+      <c r="B200" t="s">
+        <v>717</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>667</v>
+      <c r="B201" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4924,7 +4930,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>276</v>
+        <v>667</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
@@ -4932,7 +4938,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>636</v>
+        <v>276</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
@@ -4940,7 +4946,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>277</v>
+        <v>636</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4948,7 +4954,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C205" t="s">
         <v>275</v>
@@ -4956,7 +4962,7 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>668</v>
+        <v>278</v>
       </c>
       <c r="C206" t="s">
         <v>275</v>
@@ -4964,7 +4970,7 @@
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C207" t="s">
         <v>275</v>
@@ -4972,31 +4978,31 @@
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>279</v>
+        <v>669</v>
       </c>
       <c r="C208" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
+        <v>279</v>
+      </c>
+      <c r="C209" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
         <v>281</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C210" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B210" s="4" t="s">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C210" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>285</v>
       </c>
       <c r="C211" t="s">
         <v>284</v>
@@ -5004,31 +5010,31 @@
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C212" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>670</v>
+        <v>286</v>
       </c>
       <c r="C213" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="10" t="s">
-        <v>671</v>
+      <c r="B214" t="s">
+        <v>670</v>
       </c>
       <c r="C214" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
-        <v>288</v>
+      <c r="B215" s="10" t="s">
+        <v>671</v>
       </c>
       <c r="C215" t="s">
         <v>287</v>
@@ -5036,7 +5042,7 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>734</v>
+        <v>288</v>
       </c>
       <c r="C216" t="s">
         <v>287</v>
@@ -5044,7 +5050,7 @@
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>672</v>
+        <v>734</v>
       </c>
       <c r="C217" t="s">
         <v>287</v>
@@ -5052,7 +5058,7 @@
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>289</v>
+        <v>672</v>
       </c>
       <c r="C218" t="s">
         <v>287</v>
@@ -5060,15 +5066,15 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>625</v>
+        <v>289</v>
       </c>
       <c r="C219" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>290</v>
+        <v>625</v>
       </c>
       <c r="C220" t="s">
         <v>291</v>
@@ -5076,15 +5082,15 @@
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>626</v>
+        <v>290</v>
       </c>
       <c r="C221" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>292</v>
+        <v>626</v>
       </c>
       <c r="C222" t="s">
         <v>293</v>
@@ -5092,95 +5098,95 @@
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C223" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C224" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C225" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C226" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
+        <v>300</v>
+      </c>
+      <c r="C227" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
         <v>302</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C228" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="228" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B228" s="11" t="s">
+    <row r="229" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B229" s="11" t="s">
         <v>713</v>
-      </c>
-      <c r="C228" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
-        <v>304</v>
       </c>
       <c r="C229" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B230" s="4" t="s">
-        <v>306</v>
+      <c r="B230" t="s">
+        <v>304</v>
       </c>
       <c r="C230" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
-        <v>307</v>
+      <c r="B231" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C231" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C232" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>630</v>
+        <v>309</v>
       </c>
       <c r="C233" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>311</v>
+        <v>630</v>
       </c>
       <c r="C234" t="s">
         <v>312</v>
@@ -5188,31 +5194,31 @@
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C235" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C236" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>724</v>
+        <v>315</v>
       </c>
       <c r="C237" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>317</v>
+        <v>724</v>
       </c>
       <c r="C238" t="s">
         <v>318</v>
@@ -5220,15 +5226,15 @@
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>673</v>
+        <v>317</v>
       </c>
       <c r="C239" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C240" t="s">
         <v>320</v>
@@ -5236,7 +5242,7 @@
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>319</v>
+        <v>674</v>
       </c>
       <c r="C241" t="s">
         <v>320</v>
@@ -5244,7 +5250,7 @@
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>675</v>
+        <v>319</v>
       </c>
       <c r="C242" t="s">
         <v>320</v>
@@ -5252,7 +5258,7 @@
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>321</v>
+        <v>675</v>
       </c>
       <c r="C243" t="s">
         <v>320</v>
@@ -5260,48 +5266,48 @@
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C244" t="s">
         <v>320</v>
       </c>
-      <c r="E244" s="4"/>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C245" t="s">
         <v>320</v>
       </c>
+      <c r="E245" s="4"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B246" s="4" t="s">
-        <v>324</v>
+      <c r="B246" t="s">
+        <v>323</v>
       </c>
       <c r="C246" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="247" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B247" s="4" t="s">
-        <v>676</v>
+        <v>324</v>
       </c>
       <c r="C247" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B248" s="11" t="s">
-        <v>677</v>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B248" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C248" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B249" t="s">
-        <v>678</v>
+    <row r="249" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B249" s="11" t="s">
+        <v>677</v>
       </c>
       <c r="C249" t="s">
         <v>325</v>
@@ -5309,7 +5315,7 @@
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>326</v>
+        <v>678</v>
       </c>
       <c r="C250" t="s">
         <v>325</v>
@@ -5317,7 +5323,7 @@
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C251" t="s">
         <v>325</v>
@@ -5325,7 +5331,7 @@
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C252" t="s">
         <v>325</v>
@@ -5333,111 +5339,111 @@
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C253" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C254" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C255" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C256" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C257" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C258" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C259" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C260" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C261" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C262" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C263" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C264" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C265" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C266" t="s">
         <v>354</v>
@@ -5445,49 +5451,49 @@
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>720</v>
+        <v>355</v>
       </c>
       <c r="C267" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B268" s="10" t="s">
-        <v>679</v>
+      <c r="B268" t="s">
+        <v>720</v>
       </c>
       <c r="C268" t="s">
         <v>354</v>
       </c>
-      <c r="F268" s="4"/>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B269" t="s">
-        <v>627</v>
+      <c r="B269" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C269" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F269" s="4"/>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>356</v>
+        <v>627</v>
       </c>
       <c r="C270" t="s">
         <v>357</v>
       </c>
+      <c r="F270" s="4"/>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>628</v>
+        <v>356</v>
       </c>
       <c r="C271" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>358</v>
+        <v>628</v>
       </c>
       <c r="C272" t="s">
         <v>359</v>
@@ -5495,23 +5501,23 @@
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C273" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>680</v>
+        <v>360</v>
       </c>
       <c r="C274" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>362</v>
+        <v>680</v>
       </c>
       <c r="C275" t="s">
         <v>363</v>
@@ -5519,127 +5525,127 @@
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>681</v>
+        <v>362</v>
       </c>
       <c r="C276" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B277" s="4" t="s">
-        <v>364</v>
+      <c r="B277" t="s">
+        <v>681</v>
       </c>
       <c r="C277" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B278" t="s">
-        <v>365</v>
+      <c r="B278" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C278" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C279" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C280" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C281" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C282" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C283" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C284" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C285" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C286" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C287" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C288" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
+        <v>385</v>
+      </c>
+      <c r="C289" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B290" t="s">
         <v>387</v>
-      </c>
-      <c r="C289" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B290" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="C290" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B291" t="s">
-        <v>390</v>
+      <c r="B291" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C291" t="s">
         <v>388</v>
@@ -5647,63 +5653,63 @@
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C292" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C293" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C294" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C295" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C296" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C297" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C298" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C299" t="s">
         <v>404</v>
@@ -5711,23 +5717,23 @@
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C300" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C301" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C302" t="s">
         <v>409</v>
@@ -5735,79 +5741,79 @@
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C303" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C304" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C305" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C306" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C307" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C308" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C309" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C310" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>682</v>
+        <v>425</v>
       </c>
       <c r="C311" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>427</v>
+        <v>682</v>
       </c>
       <c r="C312" t="s">
         <v>428</v>
@@ -5815,7 +5821,7 @@
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>683</v>
+        <v>427</v>
       </c>
       <c r="C313" t="s">
         <v>428</v>
@@ -5823,31 +5829,31 @@
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>429</v>
+        <v>683</v>
       </c>
       <c r="C314" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B315" s="4" t="s">
-        <v>430</v>
+      <c r="B315" t="s">
+        <v>429</v>
       </c>
       <c r="C315" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B316" t="s">
-        <v>684</v>
+      <c r="B316" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C316" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>431</v>
+        <v>684</v>
       </c>
       <c r="C317" t="s">
         <v>432</v>
@@ -5855,63 +5861,63 @@
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C318" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C319" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C320" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C321" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C322" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C323" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>631</v>
+        <v>443</v>
       </c>
       <c r="C324" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>445</v>
+        <v>631</v>
       </c>
       <c r="C325" t="s">
         <v>446</v>
@@ -5919,39 +5925,39 @@
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C326" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C327" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C328" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C329" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C330" t="s">
         <v>454</v>
@@ -5959,39 +5965,39 @@
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C331" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C332" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C333" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>685</v>
+        <v>460</v>
       </c>
       <c r="C334" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>632</v>
+        <v>685</v>
       </c>
       <c r="C335" t="s">
         <v>463</v>
@@ -5999,7 +6005,7 @@
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>462</v>
+        <v>632</v>
       </c>
       <c r="C336" t="s">
         <v>463</v>
@@ -6007,7 +6013,7 @@
     </row>
     <row r="337" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C337" t="s">
         <v>463</v>
@@ -6015,7 +6021,7 @@
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C338" t="s">
         <v>463</v>
@@ -6023,210 +6029,210 @@
     </row>
     <row r="339" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C339" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="340" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
+        <v>466</v>
+      </c>
+      <c r="C340" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
         <v>468</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C341" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="341" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B341" s="11" t="s">
-        <v>730</v>
-      </c>
-      <c r="C341" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="342" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B342" s="11" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="C342" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="343" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B343" t="s">
-        <v>470</v>
+    <row r="343" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B343" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C343" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="344" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B344" s="4" t="s">
-        <v>472</v>
+      <c r="B344" t="s">
+        <v>470</v>
       </c>
       <c r="C344" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="345" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B345" t="s">
-        <v>473</v>
+      <c r="B345" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C345" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="346" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C346" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="347" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C347" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="348" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C348" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="349" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C349" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="350" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B350" s="4" t="s">
+      <c r="B350" t="s">
+        <v>481</v>
+      </c>
+      <c r="C350" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="351" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B351" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="C350" t="s">
-        <v>483</v>
-      </c>
-      <c r="E350" s="4"/>
-    </row>
-    <row r="351" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B351" t="s">
-        <v>484</v>
       </c>
       <c r="C351" t="s">
         <v>483</v>
       </c>
+      <c r="E351" s="4"/>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C352" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C353" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C354" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C355" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C356" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C357" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C358" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C359" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C360" t="s">
-        <v>502</v>
-      </c>
-      <c r="E360" s="4"/>
+        <v>500</v>
+      </c>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>686</v>
+        <v>501</v>
       </c>
       <c r="C361" t="s">
-        <v>19</v>
+        <v>502</v>
       </c>
       <c r="E361" s="4"/>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>503</v>
+        <v>686</v>
       </c>
       <c r="C362" t="s">
         <v>19</v>
       </c>
+      <c r="E362" s="4"/>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>687</v>
+        <v>503</v>
       </c>
       <c r="C363" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>504</v>
+        <v>687</v>
       </c>
       <c r="C364" t="s">
         <v>505</v>
@@ -6234,7 +6240,7 @@
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C365" t="s">
         <v>505</v>
@@ -6242,15 +6248,15 @@
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>688</v>
+        <v>506</v>
       </c>
       <c r="C366" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>507</v>
+        <v>688</v>
       </c>
       <c r="C367" t="s">
         <v>508</v>
@@ -6258,23 +6264,23 @@
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C368" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>689</v>
+        <v>509</v>
       </c>
       <c r="C369" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>511</v>
+        <v>689</v>
       </c>
       <c r="C370" t="s">
         <v>512</v>
@@ -6282,7 +6288,7 @@
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C371" t="s">
         <v>512</v>
@@ -6290,15 +6296,15 @@
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C372" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>690</v>
+        <v>514</v>
       </c>
       <c r="C373" t="s">
         <v>515</v>
@@ -6306,7 +6312,7 @@
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>516</v>
+        <v>690</v>
       </c>
       <c r="C374" t="s">
         <v>515</v>
@@ -6314,31 +6320,31 @@
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C375" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C376" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>721</v>
+        <v>519</v>
       </c>
       <c r="C377" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="C378" t="s">
         <v>522</v>
@@ -6346,7 +6352,7 @@
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C379" t="s">
         <v>522</v>
@@ -6354,7 +6360,7 @@
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>521</v>
+        <v>692</v>
       </c>
       <c r="C380" t="s">
         <v>522</v>
@@ -6362,47 +6368,47 @@
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C381" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C382" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C383" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C384" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C385" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C386" t="s">
         <v>532</v>
@@ -6410,15 +6416,15 @@
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>693</v>
+        <v>533</v>
       </c>
       <c r="C387" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>735</v>
+        <v>693</v>
       </c>
       <c r="C388" t="s">
         <v>535</v>
@@ -6426,7 +6432,7 @@
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>534</v>
+        <v>735</v>
       </c>
       <c r="C389" t="s">
         <v>535</v>
@@ -6434,7 +6440,7 @@
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C390" t="s">
         <v>535</v>
@@ -6442,122 +6448,122 @@
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C391" t="s">
         <v>535</v>
       </c>
-      <c r="D391" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C392" t="s">
         <v>535</v>
       </c>
+      <c r="D392" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C393" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
+        <v>539</v>
+      </c>
+      <c r="C394" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B395" t="s">
         <v>722</v>
-      </c>
-      <c r="C394" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B395" s="10" t="s">
-        <v>694</v>
       </c>
       <c r="C395" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B396" t="s">
-        <v>541</v>
+      <c r="B396" s="10" t="s">
+        <v>694</v>
       </c>
       <c r="C396" t="s">
-        <v>542</v>
+        <v>695</v>
       </c>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>723</v>
+        <v>541</v>
       </c>
       <c r="C397" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="398" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B398" s="11" t="s">
-        <v>696</v>
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B398" t="s">
+        <v>723</v>
       </c>
       <c r="C398" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B399" t="s">
-        <v>697</v>
+    <row r="399" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B399" s="11" t="s">
+        <v>696</v>
       </c>
       <c r="C399" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B400" s="1" t="s">
+      <c r="B400" t="s">
+        <v>697</v>
+      </c>
+      <c r="C400" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C400" s="1" t="s">
+      <c r="C401" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B401" s="10" t="s">
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402" s="10" t="s">
         <v>699</v>
-      </c>
-      <c r="C401" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B402" s="4" t="s">
-        <v>543</v>
       </c>
       <c r="C402" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B403" t="s">
-        <v>544</v>
+      <c r="B403" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C403" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>700</v>
+        <v>544</v>
       </c>
       <c r="C404" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>546</v>
+        <v>700</v>
       </c>
       <c r="C405" t="s">
         <v>547</v>
@@ -6565,31 +6571,31 @@
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C406" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C407" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C408" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>718</v>
+        <v>552</v>
       </c>
       <c r="C409" t="s">
         <v>553</v>
@@ -6597,15 +6603,15 @@
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>554</v>
+        <v>718</v>
       </c>
       <c r="C410" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C411" t="s">
         <v>555</v>
@@ -6613,47 +6619,47 @@
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C412" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C413" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C414" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
+        <v>561</v>
+      </c>
+      <c r="C415" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B416" t="s">
         <v>563</v>
-      </c>
-      <c r="C415" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B416" s="4" t="s">
-        <v>565</v>
       </c>
       <c r="C416" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B417" t="s">
-        <v>566</v>
+      <c r="B417" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C417" t="s">
         <v>564</v>
@@ -6661,39 +6667,39 @@
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C418" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C419" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C420" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>737</v>
+        <v>571</v>
       </c>
       <c r="C421" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>573</v>
+        <v>738</v>
       </c>
       <c r="C422" t="s">
         <v>574</v>
@@ -6701,79 +6707,79 @@
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>701</v>
+        <v>737</v>
       </c>
       <c r="C423" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C424" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>577</v>
+        <v>701</v>
       </c>
       <c r="C425" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B426" s="4" t="s">
-        <v>579</v>
+      <c r="B426" t="s">
+        <v>575</v>
       </c>
       <c r="C426" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C427" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B428" t="s">
-        <v>582</v>
+      <c r="B428" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C428" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C429" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>702</v>
+        <v>582</v>
       </c>
       <c r="C430" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>703</v>
+        <v>584</v>
       </c>
       <c r="C431" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>586</v>
+        <v>702</v>
       </c>
       <c r="C432" t="s">
         <v>587</v>
@@ -6781,7 +6787,7 @@
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>588</v>
+        <v>703</v>
       </c>
       <c r="C433" t="s">
         <v>587</v>
@@ -6789,31 +6795,31 @@
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C434" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B435" s="4" t="s">
-        <v>591</v>
+      <c r="B435" t="s">
+        <v>588</v>
       </c>
       <c r="C435" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C436" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" t="s">
-        <v>594</v>
+      <c r="B437" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C437" t="s">
         <v>592</v>
@@ -6821,71 +6827,71 @@
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C438" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="439" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B439" s="11" t="s">
-        <v>704</v>
+    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B439" t="s">
+        <v>594</v>
       </c>
       <c r="C439" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B440" s="10" t="s">
-        <v>705</v>
+      <c r="B440" t="s">
+        <v>595</v>
       </c>
       <c r="C440" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B441" t="s">
-        <v>596</v>
+    <row r="441" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B441" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C441" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" t="s">
-        <v>597</v>
+      <c r="B442" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C442" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C443" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>736</v>
+        <v>597</v>
       </c>
       <c r="C444" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C445" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>602</v>
+        <v>736</v>
       </c>
       <c r="C446" t="s">
         <v>601</v>
@@ -6893,55 +6899,55 @@
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>706</v>
+        <v>600</v>
       </c>
       <c r="C447" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C448" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>605</v>
+        <v>706</v>
       </c>
       <c r="C449" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B450" s="4" t="s">
-        <v>606</v>
+      <c r="B450" t="s">
+        <v>603</v>
       </c>
       <c r="C450" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B451" s="4" t="s">
+      <c r="B451" t="s">
+        <v>605</v>
+      </c>
+      <c r="C451" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B452" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C452" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B453" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="C451" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B452" t="s">
-        <v>708</v>
-      </c>
-      <c r="C452" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B453" t="s">
-        <v>607</v>
       </c>
       <c r="C453" t="s">
         <v>608</v>
@@ -6949,47 +6955,47 @@
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C454" t="s">
-        <v>711</v>
+        <v>608</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C455" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>611</v>
+        <v>710</v>
       </c>
       <c r="C456" t="s">
-        <v>612</v>
+        <v>711</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C457" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>709</v>
+        <v>611</v>
       </c>
       <c r="C458" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B459" s="4" t="s">
-        <v>615</v>
+      <c r="B459" t="s">
+        <v>613</v>
       </c>
       <c r="C459" t="s">
         <v>614</v>
@@ -6997,15 +7003,15 @@
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>616</v>
+        <v>709</v>
       </c>
       <c r="C460" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B461" t="s">
-        <v>617</v>
+      <c r="B461" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C461" t="s">
         <v>614</v>
@@ -7013,17 +7019,33 @@
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C462" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
+        <v>617</v>
+      </c>
+      <c r="C463" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B464" t="s">
+        <v>618</v>
+      </c>
+      <c r="C464" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="465" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B465" t="s">
         <v>620</v>
       </c>
-      <c r="C463" t="s">
+      <c r="C465" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added PDF export function
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="743">
   <si>
     <t>Country Name</t>
   </si>
@@ -2234,6 +2234,15 @@
   </si>
   <si>
     <t>cyprus1,2</t>
+  </si>
+  <si>
+    <t>hong kong-china</t>
+  </si>
+  <si>
+    <t>macao-china</t>
+  </si>
+  <si>
+    <t>shanghai-china</t>
   </si>
 </sst>
 </file>
@@ -3308,10 +3317,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F465"/>
+  <dimension ref="A1:F468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,23 +3776,23 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>640</v>
+        <v>742</v>
       </c>
       <c r="C57" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>641</v>
+      <c r="B58" t="s">
+        <v>640</v>
       </c>
       <c r="C58" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>96</v>
+      <c r="B59" s="10" t="s">
+        <v>641</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -3791,71 +3800,71 @@
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>733</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="C64" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
-        <v>642</v>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>729</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>643</v>
+    <row r="66" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="11" t="s">
+        <v>642</v>
       </c>
       <c r="C66" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
-        <v>644</v>
+      <c r="B67" t="s">
+        <v>643</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>104</v>
+      <c r="B68" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3863,7 +3872,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C69" t="s">
         <v>105</v>
@@ -3871,7 +3880,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>105</v>
@@ -3879,7 +3888,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>645</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
         <v>105</v>
@@ -3887,26 +3896,26 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>108</v>
+        <v>645</v>
       </c>
       <c r="C72" t="s">
         <v>105</v>
       </c>
-      <c r="D72" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="D73" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
         <v>111</v>
@@ -3914,31 +3923,31 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C77" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>633</v>
+        <v>117</v>
       </c>
       <c r="C78" t="s">
         <v>118</v>
@@ -3946,7 +3955,7 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C79" t="s">
         <v>118</v>
@@ -3954,7 +3963,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C80" t="s">
         <v>118</v>
@@ -3962,31 +3971,31 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C83" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C84" t="s">
         <v>125</v>
@@ -3994,15 +4003,15 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>739</v>
+        <v>124</v>
       </c>
       <c r="C85" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>126</v>
+        <v>739</v>
       </c>
       <c r="C86" t="s">
         <v>127</v>
@@ -4010,23 +4019,23 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>728</v>
+        <v>128</v>
       </c>
       <c r="C88" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>130</v>
+        <v>728</v>
       </c>
       <c r="C89" t="s">
         <v>131</v>
@@ -4034,55 +4043,55 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C90" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C92" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C93" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
-        <v>139</v>
+      <c r="B94" t="s">
+        <v>138</v>
       </c>
       <c r="C94" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>622</v>
+      <c r="B95" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C96" t="s">
         <v>141</v>
@@ -4090,15 +4099,15 @@
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C97" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C98" t="s">
         <v>143</v>
@@ -4106,23 +4115,23 @@
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C101" t="s">
         <v>147</v>
@@ -4130,7 +4139,7 @@
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C102" t="s">
         <v>147</v>
@@ -4138,55 +4147,55 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C103" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C104" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C105" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>726</v>
+        <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>156</v>
+        <v>726</v>
       </c>
       <c r="C107" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="12" t="s">
+      <c r="B108" t="s">
+        <v>156</v>
+      </c>
+      <c r="C108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="12" t="s">
         <v>648</v>
-      </c>
-      <c r="C108" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>719</v>
       </c>
       <c r="C109" t="s">
         <v>159</v>
@@ -4194,7 +4203,7 @@
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>649</v>
+        <v>719</v>
       </c>
       <c r="C110" t="s">
         <v>159</v>
@@ -4202,7 +4211,7 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>158</v>
+        <v>649</v>
       </c>
       <c r="C111" t="s">
         <v>159</v>
@@ -4210,23 +4219,23 @@
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>624</v>
+        <v>160</v>
       </c>
       <c r="C113" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>162</v>
+        <v>624</v>
       </c>
       <c r="C114" t="s">
         <v>163</v>
@@ -4234,15 +4243,15 @@
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>629</v>
+        <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>164</v>
+        <v>629</v>
       </c>
       <c r="C116" t="s">
         <v>165</v>
@@ -4250,23 +4259,23 @@
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C117" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C118" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C119" t="s">
         <v>169</v>
@@ -4274,15 +4283,15 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>650</v>
+        <v>170</v>
       </c>
       <c r="C120" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>171</v>
+        <v>650</v>
       </c>
       <c r="C121" t="s">
         <v>172</v>
@@ -4290,7 +4299,7 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C122" t="s">
         <v>172</v>
@@ -4298,63 +4307,63 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C124" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C125" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C126" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C127" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C128" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C129" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C130" t="s">
         <v>187</v>
@@ -4362,23 +4371,23 @@
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C131" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>651</v>
+        <v>189</v>
       </c>
       <c r="C132" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>191</v>
+        <v>651</v>
       </c>
       <c r="C133" t="s">
         <v>192</v>
@@ -4386,167 +4395,167 @@
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C134" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C135" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C136" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C137" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C138" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>652</v>
+        <v>201</v>
       </c>
       <c r="C139" t="s">
-        <v>653</v>
+        <v>202</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>203</v>
+        <v>652</v>
       </c>
       <c r="C140" t="s">
-        <v>204</v>
+        <v>653</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C141" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C142" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C143" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C144" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
+        <v>211</v>
+      </c>
+      <c r="C145" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
         <v>213</v>
-      </c>
-      <c r="C145" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C146" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" t="s">
-        <v>216</v>
+      <c r="B147" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C147" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C148" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C149" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C150" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C151" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C152" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>716</v>
+        <v>226</v>
       </c>
       <c r="C153" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>654</v>
+        <v>740</v>
       </c>
       <c r="C154" t="s">
         <v>229</v>
@@ -4554,7 +4563,7 @@
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>655</v>
+        <v>716</v>
       </c>
       <c r="C155" t="s">
         <v>229</v>
@@ -4562,7 +4571,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4570,7 +4579,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C157" t="s">
         <v>229</v>
@@ -4578,7 +4587,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>634</v>
+        <v>656</v>
       </c>
       <c r="C158" t="s">
         <v>229</v>
@@ -4586,7 +4595,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>228</v>
+        <v>657</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4594,7 +4603,7 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>230</v>
+        <v>634</v>
       </c>
       <c r="C160" t="s">
         <v>229</v>
@@ -4602,7 +4611,7 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C161" t="s">
         <v>229</v>
@@ -4610,79 +4619,79 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>727</v>
+        <v>230</v>
       </c>
       <c r="C162" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C163" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>234</v>
+        <v>727</v>
       </c>
       <c r="C164" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B165" s="6" t="s">
-        <v>236</v>
+      <c r="B165" t="s">
+        <v>232</v>
       </c>
       <c r="C165" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C166" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C167" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
-        <v>658</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C168" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>732</v>
-      </c>
-      <c r="C169" t="s">
-        <v>242</v>
+        <v>658</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>659</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="C170" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>241</v>
+        <v>732</v>
       </c>
       <c r="C171" t="s">
         <v>242</v>
@@ -4690,7 +4699,7 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>242</v>
@@ -4698,167 +4707,167 @@
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>635</v>
-      </c>
-      <c r="C173" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C173" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>243</v>
-      </c>
-      <c r="C174" t="s">
+        <v>660</v>
+      </c>
+      <c r="C174" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="175" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B175" s="11" t="s">
-        <v>661</v>
-      </c>
-      <c r="C175" t="s">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>635</v>
+      </c>
+      <c r="C175" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C176" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
-        <v>245</v>
+    <row r="177" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B177" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C177" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C178" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
-        <v>249</v>
+      <c r="B179" t="s">
+        <v>245</v>
       </c>
       <c r="C179" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C180" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>252</v>
+      <c r="B181" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C181" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C182" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C183" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C184" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C185" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C186" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C187" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C188" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C189" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C190" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C191" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>662</v>
+        <v>269</v>
       </c>
       <c r="C192" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="193" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B193" s="11" t="s">
-        <v>712</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>271</v>
       </c>
       <c r="C193" t="s">
         <v>272</v>
@@ -4866,63 +4875,63 @@
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C194" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B195" s="10" t="s">
-        <v>664</v>
+    <row r="195" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B195" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C195" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" s="10" t="s">
-        <v>665</v>
+      <c r="B196" t="s">
+        <v>663</v>
       </c>
       <c r="C196" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>273</v>
+      <c r="B197" s="10" t="s">
+        <v>664</v>
       </c>
       <c r="C197" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>731</v>
+      <c r="B198" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C198" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>666</v>
+        <v>273</v>
       </c>
       <c r="C199" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>717</v>
+        <v>731</v>
       </c>
       <c r="C200" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="4" t="s">
-        <v>274</v>
+      <c r="B201" t="s">
+        <v>666</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4930,15 +4939,15 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>667</v>
+        <v>717</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>276</v>
+      <c r="B203" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
@@ -4946,7 +4955,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>636</v>
+        <v>667</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4954,7 +4963,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C205" t="s">
         <v>275</v>
@@ -4962,7 +4971,7 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>278</v>
+        <v>636</v>
       </c>
       <c r="C206" t="s">
         <v>275</v>
@@ -4970,7 +4979,7 @@
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>668</v>
+        <v>277</v>
       </c>
       <c r="C207" t="s">
         <v>275</v>
@@ -4978,7 +4987,7 @@
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>669</v>
+        <v>278</v>
       </c>
       <c r="C208" t="s">
         <v>275</v>
@@ -4986,55 +4995,55 @@
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>279</v>
+        <v>668</v>
       </c>
       <c r="C209" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>281</v>
+        <v>669</v>
       </c>
       <c r="C210" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" s="4" t="s">
-        <v>283</v>
+      <c r="B211" t="s">
+        <v>279</v>
       </c>
       <c r="C211" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C212" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C213" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>286</v>
-      </c>
-      <c r="C213" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>670</v>
+        <v>285</v>
       </c>
       <c r="C214" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="10" t="s">
-        <v>671</v>
+      <c r="B215" t="s">
+        <v>286</v>
       </c>
       <c r="C215" t="s">
         <v>287</v>
@@ -5042,15 +5051,15 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>288</v>
+        <v>670</v>
       </c>
       <c r="C216" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>734</v>
+      <c r="B217" s="10" t="s">
+        <v>671</v>
       </c>
       <c r="C217" t="s">
         <v>287</v>
@@ -5058,7 +5067,7 @@
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>672</v>
+        <v>288</v>
       </c>
       <c r="C218" t="s">
         <v>287</v>
@@ -5066,7 +5075,7 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>289</v>
+        <v>734</v>
       </c>
       <c r="C219" t="s">
         <v>287</v>
@@ -5074,95 +5083,95 @@
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>625</v>
+        <v>672</v>
       </c>
       <c r="C220" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C221" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C222" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C223" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>294</v>
+        <v>626</v>
       </c>
       <c r="C224" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C225" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C226" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C227" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C228" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="229" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B229" s="11" t="s">
-        <v>713</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>300</v>
       </c>
       <c r="C229" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C230" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B231" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C231" t="s">
         <v>305</v>
@@ -5170,87 +5179,87 @@
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C232" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B233" t="s">
-        <v>309</v>
+      <c r="B233" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C233" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>630</v>
+        <v>307</v>
       </c>
       <c r="C234" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C235" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>313</v>
+        <v>630</v>
       </c>
       <c r="C236" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C237" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>724</v>
+        <v>313</v>
       </c>
       <c r="C238" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C239" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>673</v>
+        <v>724</v>
       </c>
       <c r="C240" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>674</v>
+        <v>317</v>
       </c>
       <c r="C241" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>319</v>
+        <v>741</v>
       </c>
       <c r="C242" t="s">
         <v>320</v>
@@ -5258,7 +5267,7 @@
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C243" t="s">
         <v>320</v>
@@ -5266,7 +5275,7 @@
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>321</v>
+        <v>674</v>
       </c>
       <c r="C244" t="s">
         <v>320</v>
@@ -5274,64 +5283,64 @@
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C245" t="s">
         <v>320</v>
       </c>
-      <c r="E245" s="4"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>323</v>
+        <v>675</v>
       </c>
       <c r="C246" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="247" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B247" s="4" t="s">
+      <c r="B247" t="s">
+        <v>321</v>
+      </c>
+      <c r="C247" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>322</v>
+      </c>
+      <c r="C248" t="s">
+        <v>320</v>
+      </c>
+      <c r="E248" s="4"/>
+    </row>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>323</v>
+      </c>
+      <c r="C249" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B250" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="C247" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B248" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C248" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="249" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B249" s="11" t="s">
-        <v>677</v>
-      </c>
-      <c r="C249" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B250" t="s">
-        <v>678</v>
       </c>
       <c r="C250" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
-        <v>326</v>
+      <c r="B251" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C251" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B252" t="s">
-        <v>327</v>
+    <row r="252" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B252" s="11" t="s">
+        <v>677</v>
       </c>
       <c r="C252" t="s">
         <v>325</v>
@@ -5339,7 +5348,7 @@
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>328</v>
+        <v>678</v>
       </c>
       <c r="C253" t="s">
         <v>325</v>
@@ -5347,505 +5356,505 @@
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C254" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C255" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C256" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C257" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C258" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C259" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C260" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C261" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C262" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C263" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C264" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C265" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C266" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C267" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>720</v>
+        <v>351</v>
       </c>
       <c r="C268" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B269" s="10" t="s">
-        <v>679</v>
+      <c r="B269" t="s">
+        <v>353</v>
       </c>
       <c r="C269" t="s">
         <v>354</v>
       </c>
-      <c r="F269" s="4"/>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>627</v>
+        <v>355</v>
       </c>
       <c r="C270" t="s">
-        <v>357</v>
-      </c>
-      <c r="F270" s="4"/>
+        <v>354</v>
+      </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
+        <v>720</v>
+      </c>
+      <c r="C271" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B272" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="C272" t="s">
+        <v>354</v>
+      </c>
+      <c r="F272" s="4"/>
+    </row>
+    <row r="273" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>627</v>
+      </c>
+      <c r="C273" t="s">
+        <v>357</v>
+      </c>
+      <c r="F273" s="4"/>
+    </row>
+    <row r="274" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
         <v>356</v>
       </c>
-      <c r="C271" t="s">
+      <c r="C274" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B272" t="s">
+    <row r="275" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
         <v>628</v>
       </c>
-      <c r="C272" t="s">
+      <c r="C275" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B273" t="s">
+    <row r="276" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
         <v>358</v>
       </c>
-      <c r="C273" t="s">
+      <c r="C276" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B274" t="s">
+    <row r="277" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
         <v>360</v>
       </c>
-      <c r="C274" t="s">
+      <c r="C277" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B275" t="s">
+    <row r="278" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
         <v>680</v>
-      </c>
-      <c r="C275" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B276" t="s">
-        <v>362</v>
-      </c>
-      <c r="C276" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B277" t="s">
-        <v>681</v>
-      </c>
-      <c r="C277" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B278" s="4" t="s">
-        <v>364</v>
       </c>
       <c r="C278" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
+        <v>362</v>
+      </c>
+      <c r="C279" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="280" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>681</v>
+      </c>
+      <c r="C280" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="281" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B281" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C281" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="282" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
         <v>365</v>
       </c>
-      <c r="C279" t="s">
+      <c r="C282" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B280" t="s">
+    <row r="283" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
         <v>367</v>
       </c>
-      <c r="C280" t="s">
+      <c r="C283" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B281" t="s">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
         <v>369</v>
       </c>
-      <c r="C281" t="s">
+      <c r="C284" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B282" t="s">
+    <row r="285" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
         <v>371</v>
       </c>
-      <c r="C282" t="s">
+      <c r="C285" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B283" t="s">
+    <row r="286" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
         <v>373</v>
       </c>
-      <c r="C283" t="s">
+      <c r="C286" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B284" t="s">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
         <v>375</v>
       </c>
-      <c r="C284" t="s">
+      <c r="C287" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B285" t="s">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
         <v>377</v>
       </c>
-      <c r="C285" t="s">
+      <c r="C288" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B286" t="s">
-        <v>379</v>
-      </c>
-      <c r="C286" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B287" t="s">
-        <v>381</v>
-      </c>
-      <c r="C287" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B288" t="s">
-        <v>383</v>
-      </c>
-      <c r="C288" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C289" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C290" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B291" s="4" t="s">
-        <v>389</v>
+      <c r="B291" t="s">
+        <v>383</v>
       </c>
       <c r="C291" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C292" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C293" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B294" t="s">
-        <v>393</v>
+      <c r="B294" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C294" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C295" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C296" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C297" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C298" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C299" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C300" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C301" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C302" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C303" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C304" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C305" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C306" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C307" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C308" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C309" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C310" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C311" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>682</v>
+        <v>421</v>
       </c>
       <c r="C312" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C313" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>683</v>
+        <v>425</v>
       </c>
       <c r="C314" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>429</v>
+        <v>682</v>
       </c>
       <c r="C315" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B316" s="4" t="s">
-        <v>430</v>
+      <c r="B316" t="s">
+        <v>427</v>
       </c>
       <c r="C316" t="s">
         <v>428</v>
@@ -5853,522 +5862,522 @@
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C317" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C318" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B319" t="s">
-        <v>433</v>
+      <c r="B319" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C319" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>435</v>
+        <v>684</v>
       </c>
       <c r="C320" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C321" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C322" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C323" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C324" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>631</v>
+        <v>439</v>
       </c>
       <c r="C325" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C326" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C327" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>449</v>
+        <v>631</v>
       </c>
       <c r="C328" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C329" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C330" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C331" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C332" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C333" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C334" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>685</v>
+        <v>456</v>
       </c>
       <c r="C335" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>632</v>
+        <v>458</v>
       </c>
       <c r="C336" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="337" spans="2:5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C337" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="338" spans="2:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>464</v>
+        <v>685</v>
       </c>
       <c r="C338" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="339" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>465</v>
+        <v>632</v>
       </c>
       <c r="C339" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="340" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
+        <v>462</v>
+      </c>
+      <c r="C340" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
+        <v>464</v>
+      </c>
+      <c r="C341" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B342" t="s">
+        <v>465</v>
+      </c>
+      <c r="C342" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
         <v>466</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C343" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="341" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B341" t="s">
+    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
         <v>468</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C344" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="342" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B342" s="11" t="s">
+    <row r="345" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B345" s="11" t="s">
         <v>730</v>
-      </c>
-      <c r="C342" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="343" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B343" s="11" t="s">
-        <v>714</v>
-      </c>
-      <c r="C343" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="344" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B344" t="s">
-        <v>470</v>
-      </c>
-      <c r="C344" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="345" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B345" s="4" t="s">
-        <v>472</v>
       </c>
       <c r="C345" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="346" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B346" t="s">
+    <row r="346" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B346" s="11" t="s">
+        <v>714</v>
+      </c>
+      <c r="C346" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>470</v>
+      </c>
+      <c r="C347" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B348" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C348" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B349" t="s">
         <v>473</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C349" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B347" t="s">
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
         <v>475</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C350" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="348" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B348" t="s">
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
         <v>477</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C351" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="349" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B349" t="s">
+    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B352" t="s">
         <v>479</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C352" t="s">
         <v>480</v>
-      </c>
-    </row>
-    <row r="350" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B350" t="s">
-        <v>481</v>
-      </c>
-      <c r="C350" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="351" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B351" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C351" t="s">
-        <v>483</v>
-      </c>
-      <c r="E351" s="4"/>
-    </row>
-    <row r="352" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B352" t="s">
-        <v>484</v>
-      </c>
-      <c r="C352" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C353" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B354" t="s">
-        <v>487</v>
+      <c r="B354" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C354" t="s">
-        <v>488</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E354" s="4"/>
     </row>
     <row r="355" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C355" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C356" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="C357" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="C358" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C359" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C360" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C361" t="s">
-        <v>502</v>
-      </c>
-      <c r="E361" s="4"/>
+        <v>496</v>
+      </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>686</v>
+        <v>497</v>
       </c>
       <c r="C362" t="s">
-        <v>19</v>
-      </c>
-      <c r="E362" s="4"/>
+        <v>498</v>
+      </c>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C363" t="s">
-        <v>19</v>
+        <v>500</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>687</v>
+        <v>501</v>
       </c>
       <c r="C364" t="s">
-        <v>505</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E364" s="4"/>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>504</v>
+        <v>686</v>
       </c>
       <c r="C365" t="s">
-        <v>505</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E365" s="4"/>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C366" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C367" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C368" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C369" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C370" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C371" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C372" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>514</v>
+        <v>689</v>
       </c>
       <c r="C373" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>690</v>
+        <v>511</v>
       </c>
       <c r="C374" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C375" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C376" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>519</v>
+        <v>690</v>
       </c>
       <c r="C377" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>721</v>
+        <v>516</v>
       </c>
       <c r="C378" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>691</v>
+        <v>517</v>
       </c>
       <c r="C379" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>692</v>
+        <v>519</v>
       </c>
       <c r="C380" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>521</v>
+        <v>721</v>
       </c>
       <c r="C381" t="s">
         <v>522</v>
@@ -6376,79 +6385,79 @@
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>523</v>
+        <v>691</v>
       </c>
       <c r="C382" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>525</v>
+        <v>692</v>
       </c>
       <c r="C383" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C384" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C385" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C386" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C387" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>693</v>
+        <v>529</v>
       </c>
       <c r="C388" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>735</v>
+        <v>531</v>
       </c>
       <c r="C389" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C390" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>536</v>
+        <v>693</v>
       </c>
       <c r="C391" t="s">
         <v>535</v>
@@ -6456,18 +6465,15 @@
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>537</v>
+        <v>735</v>
       </c>
       <c r="C392" t="s">
         <v>535</v>
       </c>
-      <c r="D392" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C393" t="s">
         <v>535</v>
@@ -6475,335 +6481,338 @@
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C394" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>722</v>
+        <v>537</v>
       </c>
       <c r="C395" t="s">
-        <v>695</v>
+        <v>535</v>
+      </c>
+      <c r="D395" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B396" s="10" t="s">
-        <v>694</v>
+      <c r="B396" t="s">
+        <v>538</v>
       </c>
       <c r="C396" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C397" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C398" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="399" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B399" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
+      </c>
+    </row>
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B399" s="10" t="s">
+        <v>694</v>
       </c>
       <c r="C399" t="s">
-        <v>542</v>
+        <v>695</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>697</v>
+        <v>541</v>
       </c>
       <c r="C400" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B401" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="C401" s="1" t="s">
+      <c r="B401" t="s">
+        <v>723</v>
+      </c>
+      <c r="C401" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B402" s="10" t="s">
-        <v>699</v>
+    <row r="402" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B402" s="11" t="s">
+        <v>696</v>
       </c>
       <c r="C402" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B403" s="4" t="s">
-        <v>543</v>
+      <c r="B403" t="s">
+        <v>697</v>
       </c>
       <c r="C403" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B404" t="s">
-        <v>544</v>
-      </c>
-      <c r="C404" t="s">
-        <v>545</v>
+      <c r="B404" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B405" t="s">
-        <v>700</v>
+      <c r="B405" s="10" t="s">
+        <v>699</v>
       </c>
       <c r="C405" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B406" t="s">
-        <v>546</v>
+      <c r="B406" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C406" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C407" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="C408" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="C409" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>718</v>
+        <v>548</v>
       </c>
       <c r="C410" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C411" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C412" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>557</v>
+        <v>718</v>
       </c>
       <c r="C413" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="C414" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="C415" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C416" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B417" s="4" t="s">
-        <v>565</v>
+      <c r="B417" t="s">
+        <v>559</v>
       </c>
       <c r="C417" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C418" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C419" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B420" t="s">
-        <v>569</v>
+      <c r="B420" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C420" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="C421" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>738</v>
+        <v>567</v>
       </c>
       <c r="C422" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>737</v>
+        <v>569</v>
       </c>
       <c r="C423" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C424" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>701</v>
+        <v>738</v>
       </c>
       <c r="C425" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>575</v>
+        <v>737</v>
       </c>
       <c r="C426" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C427" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B428" s="4" t="s">
-        <v>579</v>
+      <c r="B428" t="s">
+        <v>701</v>
       </c>
       <c r="C428" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="C429" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="C430" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B431" t="s">
-        <v>584</v>
+      <c r="B431" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C431" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>702</v>
+        <v>580</v>
       </c>
       <c r="C432" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>703</v>
+        <v>582</v>
       </c>
       <c r="C433" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C434" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>588</v>
+        <v>702</v>
       </c>
       <c r="C435" t="s">
         <v>587</v>
@@ -6811,55 +6820,55 @@
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>589</v>
+        <v>703</v>
       </c>
       <c r="C436" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" s="4" t="s">
-        <v>591</v>
+      <c r="B437" t="s">
+        <v>586</v>
       </c>
       <c r="C437" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="C438" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="C439" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B440" t="s">
-        <v>595</v>
+      <c r="B440" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C440" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="441" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B441" s="11" t="s">
-        <v>704</v>
+    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B441" t="s">
+        <v>593</v>
       </c>
       <c r="C441" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" s="10" t="s">
-        <v>705</v>
+      <c r="B442" t="s">
+        <v>594</v>
       </c>
       <c r="C442" t="s">
         <v>592</v>
@@ -6867,159 +6876,159 @@
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C443" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B444" t="s">
-        <v>597</v>
+    <row r="444" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B444" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C444" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" t="s">
-        <v>599</v>
+      <c r="B445" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C445" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>736</v>
+        <v>596</v>
       </c>
       <c r="C446" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C447" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C448" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>706</v>
+        <v>736</v>
       </c>
       <c r="C449" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C450" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C451" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B452" s="4" t="s">
-        <v>606</v>
+      <c r="B452" t="s">
+        <v>706</v>
       </c>
       <c r="C452" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B453" s="4" t="s">
-        <v>707</v>
+      <c r="B453" t="s">
+        <v>603</v>
       </c>
       <c r="C453" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>708</v>
+        <v>605</v>
       </c>
       <c r="C454" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B455" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C455" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B456" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="C456" t="s">
         <v>608</v>
-      </c>
-    </row>
-    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B455" t="s">
-        <v>607</v>
-      </c>
-      <c r="C455" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B456" t="s">
-        <v>710</v>
-      </c>
-      <c r="C456" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>609</v>
+        <v>708</v>
       </c>
       <c r="C457" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C458" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>613</v>
+        <v>710</v>
       </c>
       <c r="C459" t="s">
-        <v>614</v>
+        <v>711</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>709</v>
+        <v>609</v>
       </c>
       <c r="C460" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B461" s="4" t="s">
-        <v>615</v>
+      <c r="B461" t="s">
+        <v>611</v>
       </c>
       <c r="C461" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C462" t="s">
         <v>614</v>
@@ -7027,25 +7036,49 @@
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
-        <v>617</v>
+        <v>709</v>
       </c>
       <c r="C463" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B464" t="s">
-        <v>618</v>
+      <c r="B464" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C464" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
+        <v>616</v>
+      </c>
+      <c r="C465" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="466" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B466" t="s">
+        <v>617</v>
+      </c>
+      <c r="C466" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="467" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B467" t="s">
+        <v>618</v>
+      </c>
+      <c r="C467" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="468" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B468" t="s">
         <v>620</v>
       </c>
-      <c r="C465" t="s">
+      <c r="C468" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISO3 file updated to include TWN and COG for venture capital data
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Country Code" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="745">
   <si>
     <t>Country Name</t>
   </si>
@@ -2243,6 +2243,12 @@
   </si>
   <si>
     <t>shanghai-china</t>
+  </si>
+  <si>
+    <t>Republic of Congo</t>
+  </si>
+  <si>
+    <t>Taiwan Province of China</t>
   </si>
 </sst>
 </file>
@@ -3317,10 +3323,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F468"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
+      <selection activeCell="C394" sqref="C394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3923,7 +3929,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>112</v>
+        <v>743</v>
       </c>
       <c r="C75" t="s">
         <v>111</v>
@@ -3931,31 +3937,31 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>633</v>
+        <v>117</v>
       </c>
       <c r="C79" t="s">
         <v>118</v>
@@ -3963,7 +3969,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C80" t="s">
         <v>118</v>
@@ -3971,7 +3977,7 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C81" t="s">
         <v>118</v>
@@ -3979,31 +3985,31 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C82" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C83" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C85" t="s">
         <v>125</v>
@@ -4011,15 +4017,15 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>739</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>126</v>
+        <v>739</v>
       </c>
       <c r="C87" t="s">
         <v>127</v>
@@ -4027,23 +4033,23 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>728</v>
+        <v>128</v>
       </c>
       <c r="C89" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>130</v>
+        <v>728</v>
       </c>
       <c r="C90" t="s">
         <v>131</v>
@@ -4051,55 +4057,55 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C91" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C92" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C93" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C94" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
-        <v>139</v>
+      <c r="B95" t="s">
+        <v>138</v>
       </c>
       <c r="C95" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>622</v>
+      <c r="B96" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C96" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C97" t="s">
         <v>141</v>
@@ -4107,15 +4113,15 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C98" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C99" t="s">
         <v>143</v>
@@ -4123,23 +4129,23 @@
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C101" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C102" t="s">
         <v>147</v>
@@ -4147,7 +4153,7 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C103" t="s">
         <v>147</v>
@@ -4155,55 +4161,55 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C104" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C105" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>726</v>
+        <v>154</v>
       </c>
       <c r="C107" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>156</v>
+        <v>726</v>
       </c>
       <c r="C108" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="12" t="s">
+      <c r="B109" t="s">
+        <v>156</v>
+      </c>
+      <c r="C109" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="12" t="s">
         <v>648</v>
-      </c>
-      <c r="C109" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>719</v>
       </c>
       <c r="C110" t="s">
         <v>159</v>
@@ -4211,7 +4217,7 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>649</v>
+        <v>719</v>
       </c>
       <c r="C111" t="s">
         <v>159</v>
@@ -4219,7 +4225,7 @@
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>158</v>
+        <v>649</v>
       </c>
       <c r="C112" t="s">
         <v>159</v>
@@ -4227,23 +4233,23 @@
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C113" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>624</v>
+        <v>160</v>
       </c>
       <c r="C114" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>162</v>
+        <v>624</v>
       </c>
       <c r="C115" t="s">
         <v>163</v>
@@ -4251,15 +4257,15 @@
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>629</v>
+        <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>164</v>
+        <v>629</v>
       </c>
       <c r="C117" t="s">
         <v>165</v>
@@ -4267,23 +4273,23 @@
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C118" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C119" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C120" t="s">
         <v>169</v>
@@ -4291,15 +4297,15 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>650</v>
+        <v>170</v>
       </c>
       <c r="C121" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>171</v>
+        <v>650</v>
       </c>
       <c r="C122" t="s">
         <v>172</v>
@@ -4307,7 +4313,7 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C123" t="s">
         <v>172</v>
@@ -4315,63 +4321,63 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C124" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C125" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C126" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C127" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C128" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C129" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C130" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C131" t="s">
         <v>187</v>
@@ -4379,23 +4385,23 @@
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C132" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>651</v>
+        <v>189</v>
       </c>
       <c r="C133" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>191</v>
+        <v>651</v>
       </c>
       <c r="C134" t="s">
         <v>192</v>
@@ -4403,167 +4409,167 @@
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C135" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C136" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C137" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C138" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C139" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>652</v>
+        <v>201</v>
       </c>
       <c r="C140" t="s">
-        <v>653</v>
+        <v>202</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>203</v>
+        <v>652</v>
       </c>
       <c r="C141" t="s">
-        <v>204</v>
+        <v>653</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C142" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C143" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C144" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C145" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
+        <v>211</v>
+      </c>
+      <c r="C146" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
         <v>213</v>
-      </c>
-      <c r="C146" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C147" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>216</v>
+      <c r="B148" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C148" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C149" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C150" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C151" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C152" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C153" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>740</v>
+        <v>226</v>
       </c>
       <c r="C154" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>716</v>
+        <v>740</v>
       </c>
       <c r="C155" t="s">
         <v>229</v>
@@ -4571,7 +4577,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>654</v>
+        <v>716</v>
       </c>
       <c r="C156" t="s">
         <v>229</v>
@@ -4579,7 +4585,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C157" t="s">
         <v>229</v>
@@ -4587,7 +4593,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C158" t="s">
         <v>229</v>
@@ -4595,7 +4601,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4603,7 +4609,7 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>634</v>
+        <v>657</v>
       </c>
       <c r="C160" t="s">
         <v>229</v>
@@ -4611,7 +4617,7 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>228</v>
+        <v>634</v>
       </c>
       <c r="C161" t="s">
         <v>229</v>
@@ -4619,7 +4625,7 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C162" t="s">
         <v>229</v>
@@ -4627,7 +4633,7 @@
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C163" t="s">
         <v>229</v>
@@ -4635,15 +4641,15 @@
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>727</v>
+        <v>231</v>
       </c>
       <c r="C164" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>232</v>
+        <v>727</v>
       </c>
       <c r="C165" t="s">
         <v>233</v>
@@ -4651,23 +4657,23 @@
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
+        <v>232</v>
+      </c>
+      <c r="C166" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
         <v>234</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C167" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B167" s="6" t="s">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="C167" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>238</v>
       </c>
       <c r="C168" t="s">
         <v>237</v>
@@ -4675,55 +4681,55 @@
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>658</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
+      </c>
+      <c r="C169" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>239</v>
-      </c>
-      <c r="C170" t="s">
+        <v>658</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>732</v>
+        <v>239</v>
       </c>
       <c r="C171" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>659</v>
-      </c>
-      <c r="C172" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="C172" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>241</v>
-      </c>
-      <c r="C173" t="s">
+        <v>659</v>
+      </c>
+      <c r="C173" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>660</v>
-      </c>
-      <c r="C174" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C174" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>635</v>
+        <v>660</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>242</v>
@@ -4731,23 +4737,23 @@
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
+        <v>635</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
         <v>243</v>
-      </c>
-      <c r="C176" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="177" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B177" s="11" t="s">
-        <v>661</v>
       </c>
       <c r="C177" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>244</v>
+    <row r="178" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B178" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C178" t="s">
         <v>242</v>
@@ -4755,79 +4761,79 @@
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C179" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
+        <v>245</v>
+      </c>
+      <c r="C180" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>247</v>
-      </c>
-      <c r="C180" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="C181" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>250</v>
+      <c r="B182" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C182" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C183" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C184" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C185" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C186" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C187" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C188" t="s">
         <v>261</v>
@@ -4835,71 +4841,71 @@
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C189" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C190" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C191" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C192" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C193" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>662</v>
+        <v>271</v>
       </c>
       <c r="C194" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="195" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B195" s="11" t="s">
-        <v>712</v>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>662</v>
       </c>
       <c r="C195" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
-        <v>663</v>
+    <row r="196" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B196" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C196" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="10" t="s">
-        <v>664</v>
+      <c r="B197" t="s">
+        <v>663</v>
       </c>
       <c r="C197" t="s">
         <v>272</v>
@@ -4907,15 +4913,15 @@
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C198" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>273</v>
+      <c r="B199" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C199" t="s">
         <v>272</v>
@@ -4923,15 +4929,15 @@
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>731</v>
+        <v>273</v>
       </c>
       <c r="C200" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>666</v>
+        <v>731</v>
       </c>
       <c r="C201" t="s">
         <v>275</v>
@@ -4939,23 +4945,23 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>717</v>
+        <v>666</v>
       </c>
       <c r="C202" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>274</v>
+      <c r="B203" t="s">
+        <v>717</v>
       </c>
       <c r="C203" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>667</v>
+      <c r="B204" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C204" t="s">
         <v>275</v>
@@ -4963,7 +4969,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>276</v>
+        <v>667</v>
       </c>
       <c r="C205" t="s">
         <v>275</v>
@@ -4971,7 +4977,7 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>636</v>
+        <v>276</v>
       </c>
       <c r="C206" t="s">
         <v>275</v>
@@ -4979,7 +4985,7 @@
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>277</v>
+        <v>636</v>
       </c>
       <c r="C207" t="s">
         <v>275</v>
@@ -4987,7 +4993,7 @@
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C208" t="s">
         <v>275</v>
@@ -4995,7 +5001,7 @@
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>668</v>
+        <v>278</v>
       </c>
       <c r="C209" t="s">
         <v>275</v>
@@ -5003,7 +5009,7 @@
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C210" t="s">
         <v>275</v>
@@ -5011,31 +5017,31 @@
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>279</v>
+        <v>669</v>
       </c>
       <c r="C211" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
+        <v>279</v>
+      </c>
+      <c r="C212" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
         <v>281</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C213" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="4" t="s">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C213" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>285</v>
       </c>
       <c r="C214" t="s">
         <v>284</v>
@@ -5043,31 +5049,31 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C215" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>670</v>
+        <v>286</v>
       </c>
       <c r="C216" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" s="10" t="s">
-        <v>671</v>
+      <c r="B217" t="s">
+        <v>670</v>
       </c>
       <c r="C217" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
-        <v>288</v>
+      <c r="B218" s="10" t="s">
+        <v>671</v>
       </c>
       <c r="C218" t="s">
         <v>287</v>
@@ -5075,7 +5081,7 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>734</v>
+        <v>288</v>
       </c>
       <c r="C219" t="s">
         <v>287</v>
@@ -5083,7 +5089,7 @@
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>672</v>
+        <v>734</v>
       </c>
       <c r="C220" t="s">
         <v>287</v>
@@ -5091,7 +5097,7 @@
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>289</v>
+        <v>672</v>
       </c>
       <c r="C221" t="s">
         <v>287</v>
@@ -5099,15 +5105,15 @@
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>625</v>
+        <v>289</v>
       </c>
       <c r="C222" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>290</v>
+        <v>625</v>
       </c>
       <c r="C223" t="s">
         <v>291</v>
@@ -5115,15 +5121,15 @@
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>626</v>
+        <v>290</v>
       </c>
       <c r="C224" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>292</v>
+        <v>626</v>
       </c>
       <c r="C225" t="s">
         <v>293</v>
@@ -5131,95 +5137,95 @@
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C226" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C227" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C228" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C229" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
+        <v>300</v>
+      </c>
+      <c r="C230" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
         <v>302</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C231" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="231" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B231" s="11" t="s">
+    <row r="232" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B232" s="11" t="s">
         <v>713</v>
-      </c>
-      <c r="C231" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
-        <v>304</v>
       </c>
       <c r="C232" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B233" s="4" t="s">
-        <v>306</v>
+      <c r="B233" t="s">
+        <v>304</v>
       </c>
       <c r="C233" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B234" t="s">
-        <v>307</v>
+      <c r="B234" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C234" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C235" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>630</v>
+        <v>309</v>
       </c>
       <c r="C236" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>311</v>
+        <v>630</v>
       </c>
       <c r="C237" t="s">
         <v>312</v>
@@ -5227,31 +5233,31 @@
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C238" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C239" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>724</v>
+        <v>315</v>
       </c>
       <c r="C240" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>317</v>
+        <v>724</v>
       </c>
       <c r="C241" t="s">
         <v>318</v>
@@ -5259,15 +5265,15 @@
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>741</v>
+        <v>317</v>
       </c>
       <c r="C242" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>673</v>
+        <v>741</v>
       </c>
       <c r="C243" t="s">
         <v>320</v>
@@ -5275,7 +5281,7 @@
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C244" t="s">
         <v>320</v>
@@ -5283,7 +5289,7 @@
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>319</v>
+        <v>674</v>
       </c>
       <c r="C245" t="s">
         <v>320</v>
@@ -5291,7 +5297,7 @@
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>675</v>
+        <v>319</v>
       </c>
       <c r="C246" t="s">
         <v>320</v>
@@ -5299,7 +5305,7 @@
     </row>
     <row r="247" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>321</v>
+        <v>675</v>
       </c>
       <c r="C247" t="s">
         <v>320</v>
@@ -5307,48 +5313,48 @@
     </row>
     <row r="248" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C248" t="s">
         <v>320</v>
       </c>
-      <c r="E248" s="4"/>
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C249" t="s">
         <v>320</v>
       </c>
+      <c r="E249" s="4"/>
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B250" s="4" t="s">
-        <v>324</v>
+      <c r="B250" t="s">
+        <v>323</v>
       </c>
       <c r="C250" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" s="4" t="s">
-        <v>676</v>
+        <v>324</v>
       </c>
       <c r="C251" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="252" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B252" s="11" t="s">
-        <v>677</v>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C252" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B253" t="s">
-        <v>678</v>
+    <row r="253" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B253" s="11" t="s">
+        <v>677</v>
       </c>
       <c r="C253" t="s">
         <v>325</v>
@@ -5356,7 +5362,7 @@
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>326</v>
+        <v>678</v>
       </c>
       <c r="C254" t="s">
         <v>325</v>
@@ -5364,7 +5370,7 @@
     </row>
     <row r="255" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C255" t="s">
         <v>325</v>
@@ -5372,169 +5378,169 @@
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C256" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
+        <v>328</v>
+      </c>
+      <c r="C257" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
         <v>329</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C258" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B258" t="s">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
         <v>331</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C259" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="259" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B259" t="s">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
         <v>333</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C260" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="260" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
         <v>335</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C261" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="261" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B261" t="s">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
         <v>337</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C262" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="262" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B262" t="s">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
         <v>339</v>
       </c>
-      <c r="C262" t="s">
+      <c r="C263" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="263" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B263" t="s">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
         <v>341</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C264" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="264" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B264" t="s">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
         <v>343</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C265" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="265" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B265" t="s">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B266" t="s">
         <v>345</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C266" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="266" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B266" t="s">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
         <v>347</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C267" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="267" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B267" t="s">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
         <v>349</v>
       </c>
-      <c r="C267" t="s">
+      <c r="C268" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="268" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B268" t="s">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
         <v>351</v>
       </c>
-      <c r="C268" t="s">
+      <c r="C269" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="269" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B269" t="s">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
         <v>353</v>
-      </c>
-      <c r="C269" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="270" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B270" t="s">
-        <v>355</v>
       </c>
       <c r="C270" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="271" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>720</v>
+        <v>355</v>
       </c>
       <c r="C271" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B272" s="10" t="s">
-        <v>679</v>
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>720</v>
       </c>
       <c r="C272" t="s">
         <v>354</v>
       </c>
-      <c r="F272" s="4"/>
     </row>
     <row r="273" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B273" t="s">
-        <v>627</v>
+      <c r="B273" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C273" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F273" s="4"/>
     </row>
     <row r="274" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>356</v>
+        <v>627</v>
       </c>
       <c r="C274" t="s">
         <v>357</v>
       </c>
+      <c r="F274" s="4"/>
     </row>
     <row r="275" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>628</v>
+        <v>356</v>
       </c>
       <c r="C275" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="276" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>358</v>
+        <v>628</v>
       </c>
       <c r="C276" t="s">
         <v>359</v>
@@ -5542,23 +5548,23 @@
     </row>
     <row r="277" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C277" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="278" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>680</v>
+        <v>360</v>
       </c>
       <c r="C278" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="279" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>362</v>
+        <v>680</v>
       </c>
       <c r="C279" t="s">
         <v>363</v>
@@ -5566,127 +5572,127 @@
     </row>
     <row r="280" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>681</v>
+        <v>362</v>
       </c>
       <c r="C280" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="281" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B281" s="4" t="s">
-        <v>364</v>
+      <c r="B281" t="s">
+        <v>681</v>
       </c>
       <c r="C281" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="282" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B282" t="s">
-        <v>365</v>
+      <c r="B282" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C282" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="283" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C283" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="284" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C284" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="285" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C285" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="286" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C286" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="287" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C287" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="288" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C288" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C289" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C290" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C291" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C292" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
+        <v>385</v>
+      </c>
+      <c r="C293" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B294" t="s">
         <v>387</v>
-      </c>
-      <c r="C293" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B294" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="C294" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B295" t="s">
-        <v>390</v>
+      <c r="B295" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C295" t="s">
         <v>388</v>
@@ -5694,63 +5700,63 @@
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C296" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C297" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C298" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C299" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C300" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C301" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C302" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C303" t="s">
         <v>404</v>
@@ -5758,23 +5764,23 @@
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C304" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C305" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C306" t="s">
         <v>409</v>
@@ -5782,79 +5788,79 @@
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C307" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C308" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C309" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C310" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C311" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C312" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C313" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C314" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>682</v>
+        <v>425</v>
       </c>
       <c r="C315" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>427</v>
+        <v>682</v>
       </c>
       <c r="C316" t="s">
         <v>428</v>
@@ -5862,7 +5868,7 @@
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>683</v>
+        <v>427</v>
       </c>
       <c r="C317" t="s">
         <v>428</v>
@@ -5870,31 +5876,31 @@
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>429</v>
+        <v>683</v>
       </c>
       <c r="C318" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B319" s="4" t="s">
-        <v>430</v>
+      <c r="B319" t="s">
+        <v>429</v>
       </c>
       <c r="C319" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B320" t="s">
-        <v>684</v>
+      <c r="B320" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C320" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>431</v>
+        <v>684</v>
       </c>
       <c r="C321" t="s">
         <v>432</v>
@@ -5902,63 +5908,63 @@
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C322" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C323" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C324" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C325" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C326" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C327" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>631</v>
+        <v>443</v>
       </c>
       <c r="C328" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>445</v>
+        <v>631</v>
       </c>
       <c r="C329" t="s">
         <v>446</v>
@@ -5966,39 +5972,39 @@
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C330" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C331" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C332" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C333" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C334" t="s">
         <v>454</v>
@@ -6006,39 +6012,39 @@
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C335" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C336" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C337" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>685</v>
+        <v>460</v>
       </c>
       <c r="C338" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>632</v>
+        <v>685</v>
       </c>
       <c r="C339" t="s">
         <v>463</v>
@@ -6046,7 +6052,7 @@
     </row>
     <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>462</v>
+        <v>632</v>
       </c>
       <c r="C340" t="s">
         <v>463</v>
@@ -6054,7 +6060,7 @@
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C341" t="s">
         <v>463</v>
@@ -6062,7 +6068,7 @@
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C342" t="s">
         <v>463</v>
@@ -6070,210 +6076,210 @@
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C343" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
+        <v>466</v>
+      </c>
+      <c r="C344" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
         <v>468</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C345" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="345" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B345" s="11" t="s">
-        <v>730</v>
-      </c>
-      <c r="C345" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="346" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B346" s="11" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="C346" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B347" t="s">
-        <v>470</v>
+    <row r="347" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B347" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C347" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="348" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B348" s="4" t="s">
-        <v>472</v>
+      <c r="B348" t="s">
+        <v>470</v>
       </c>
       <c r="C348" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="349" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B349" t="s">
-        <v>473</v>
+      <c r="B349" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C349" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="350" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C350" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="351" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C351" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C352" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C353" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B354" s="4" t="s">
+      <c r="B354" t="s">
+        <v>481</v>
+      </c>
+      <c r="C354" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="355" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B355" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="C354" t="s">
-        <v>483</v>
-      </c>
-      <c r="E354" s="4"/>
-    </row>
-    <row r="355" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B355" t="s">
-        <v>484</v>
       </c>
       <c r="C355" t="s">
         <v>483</v>
       </c>
+      <c r="E355" s="4"/>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C356" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C357" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C358" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C359" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C360" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C361" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C362" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C363" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C364" t="s">
-        <v>502</v>
-      </c>
-      <c r="E364" s="4"/>
+        <v>500</v>
+      </c>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>686</v>
+        <v>501</v>
       </c>
       <c r="C365" t="s">
-        <v>19</v>
+        <v>502</v>
       </c>
       <c r="E365" s="4"/>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>503</v>
+        <v>686</v>
       </c>
       <c r="C366" t="s">
         <v>19</v>
       </c>
+      <c r="E366" s="4"/>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>687</v>
+        <v>503</v>
       </c>
       <c r="C367" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>504</v>
+        <v>687</v>
       </c>
       <c r="C368" t="s">
         <v>505</v>
@@ -6281,7 +6287,7 @@
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C369" t="s">
         <v>505</v>
@@ -6289,15 +6295,15 @@
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>688</v>
+        <v>506</v>
       </c>
       <c r="C370" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>507</v>
+        <v>688</v>
       </c>
       <c r="C371" t="s">
         <v>508</v>
@@ -6305,23 +6311,23 @@
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C372" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>689</v>
+        <v>509</v>
       </c>
       <c r="C373" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>511</v>
+        <v>689</v>
       </c>
       <c r="C374" t="s">
         <v>512</v>
@@ -6329,7 +6335,7 @@
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C375" t="s">
         <v>512</v>
@@ -6337,15 +6343,15 @@
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C376" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>690</v>
+        <v>514</v>
       </c>
       <c r="C377" t="s">
         <v>515</v>
@@ -6353,7 +6359,7 @@
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>516</v>
+        <v>690</v>
       </c>
       <c r="C378" t="s">
         <v>515</v>
@@ -6361,31 +6367,31 @@
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C379" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C380" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>721</v>
+        <v>519</v>
       </c>
       <c r="C381" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="C382" t="s">
         <v>522</v>
@@ -6393,7 +6399,7 @@
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C383" t="s">
         <v>522</v>
@@ -6401,7 +6407,7 @@
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>521</v>
+        <v>692</v>
       </c>
       <c r="C384" t="s">
         <v>522</v>
@@ -6409,47 +6415,47 @@
     </row>
     <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C385" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C386" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C387" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C388" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C389" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C390" t="s">
         <v>532</v>
@@ -6457,15 +6463,15 @@
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>693</v>
+        <v>533</v>
       </c>
       <c r="C391" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>735</v>
+        <v>693</v>
       </c>
       <c r="C392" t="s">
         <v>535</v>
@@ -6473,7 +6479,7 @@
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>534</v>
+        <v>744</v>
       </c>
       <c r="C393" t="s">
         <v>535</v>
@@ -6481,7 +6487,7 @@
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>536</v>
+        <v>735</v>
       </c>
       <c r="C394" t="s">
         <v>535</v>
@@ -6489,18 +6495,15 @@
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C395" t="s">
         <v>535</v>
       </c>
-      <c r="D395" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C396" t="s">
         <v>535</v>
@@ -6508,47 +6511,50 @@
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C397" t="s">
-        <v>540</v>
+        <v>535</v>
+      </c>
+      <c r="D397" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>722</v>
+        <v>538</v>
       </c>
       <c r="C398" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B399" s="10" t="s">
-        <v>694</v>
+      <c r="B399" t="s">
+        <v>539</v>
       </c>
       <c r="C399" t="s">
-        <v>695</v>
+        <v>540</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
+        <v>722</v>
+      </c>
+      <c r="C400" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="C401" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402" t="s">
         <v>541</v>
-      </c>
-      <c r="C400" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B401" t="s">
-        <v>723</v>
-      </c>
-      <c r="C401" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="402" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B402" s="11" t="s">
-        <v>696</v>
       </c>
       <c r="C402" t="s">
         <v>542</v>
@@ -6556,199 +6562,199 @@
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>697</v>
+        <v>723</v>
       </c>
       <c r="C403" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B404" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="C404" s="1" t="s">
+    <row r="404" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B404" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="C404" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B405" s="10" t="s">
-        <v>699</v>
+      <c r="B405" t="s">
+        <v>697</v>
       </c>
       <c r="C405" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B406" s="4" t="s">
+      <c r="B406" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B407" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="C407" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B408" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C406" t="s">
+      <c r="C408" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B407" t="s">
-        <v>544</v>
-      </c>
-      <c r="C407" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B408" t="s">
-        <v>700</v>
-      </c>
-      <c r="C408" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C409" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>548</v>
+        <v>700</v>
       </c>
       <c r="C410" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C411" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C412" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>718</v>
+        <v>550</v>
       </c>
       <c r="C413" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C414" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>556</v>
+        <v>718</v>
       </c>
       <c r="C415" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C416" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C417" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C418" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C419" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B420" s="4" t="s">
-        <v>565</v>
+      <c r="B420" t="s">
+        <v>561</v>
       </c>
       <c r="C420" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C421" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B422" t="s">
-        <v>567</v>
+      <c r="B422" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C422" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C423" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C424" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>738</v>
+        <v>569</v>
       </c>
       <c r="C425" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>737</v>
+        <v>571</v>
       </c>
       <c r="C426" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>573</v>
+        <v>738</v>
       </c>
       <c r="C427" t="s">
         <v>574</v>
@@ -6756,79 +6762,79 @@
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>701</v>
+        <v>737</v>
       </c>
       <c r="C428" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C429" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>577</v>
+        <v>701</v>
       </c>
       <c r="C430" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B431" s="4" t="s">
-        <v>579</v>
+      <c r="B431" t="s">
+        <v>575</v>
       </c>
       <c r="C431" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C432" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B433" t="s">
-        <v>582</v>
+      <c r="B433" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C433" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C434" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>702</v>
+        <v>582</v>
       </c>
       <c r="C435" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>703</v>
+        <v>584</v>
       </c>
       <c r="C436" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>586</v>
+        <v>702</v>
       </c>
       <c r="C437" t="s">
         <v>587</v>
@@ -6836,7 +6842,7 @@
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>588</v>
+        <v>703</v>
       </c>
       <c r="C438" t="s">
         <v>587</v>
@@ -6844,31 +6850,31 @@
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C439" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B440" s="4" t="s">
-        <v>591</v>
+      <c r="B440" t="s">
+        <v>588</v>
       </c>
       <c r="C440" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C441" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" t="s">
-        <v>594</v>
+      <c r="B442" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C442" t="s">
         <v>592</v>
@@ -6876,71 +6882,71 @@
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C443" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="444" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B444" s="11" t="s">
-        <v>704</v>
+    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B444" t="s">
+        <v>594</v>
       </c>
       <c r="C444" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" s="10" t="s">
-        <v>705</v>
+      <c r="B445" t="s">
+        <v>595</v>
       </c>
       <c r="C445" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B446" t="s">
-        <v>596</v>
+    <row r="446" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B446" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C446" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" t="s">
-        <v>597</v>
+      <c r="B447" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C447" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C448" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>736</v>
+        <v>597</v>
       </c>
       <c r="C449" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C450" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>602</v>
+        <v>736</v>
       </c>
       <c r="C451" t="s">
         <v>601</v>
@@ -6948,55 +6954,55 @@
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>706</v>
+        <v>600</v>
       </c>
       <c r="C452" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C453" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>605</v>
+        <v>706</v>
       </c>
       <c r="C454" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B455" s="4" t="s">
-        <v>606</v>
+      <c r="B455" t="s">
+        <v>603</v>
       </c>
       <c r="C455" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B456" s="4" t="s">
+      <c r="B456" t="s">
+        <v>605</v>
+      </c>
+      <c r="C456" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B457" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C457" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B458" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="C456" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B457" t="s">
-        <v>708</v>
-      </c>
-      <c r="C457" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B458" t="s">
-        <v>607</v>
       </c>
       <c r="C458" t="s">
         <v>608</v>
@@ -7004,47 +7010,47 @@
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C459" t="s">
-        <v>711</v>
+        <v>608</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C460" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>611</v>
+        <v>710</v>
       </c>
       <c r="C461" t="s">
-        <v>612</v>
+        <v>711</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C462" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
-        <v>709</v>
+        <v>611</v>
       </c>
       <c r="C463" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B464" s="4" t="s">
-        <v>615</v>
+      <c r="B464" t="s">
+        <v>613</v>
       </c>
       <c r="C464" t="s">
         <v>614</v>
@@ -7052,15 +7058,15 @@
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>616</v>
+        <v>709</v>
       </c>
       <c r="C465" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B466" t="s">
-        <v>617</v>
+      <c r="B466" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C466" t="s">
         <v>614</v>
@@ -7068,17 +7074,33 @@
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C467" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
+        <v>617</v>
+      </c>
+      <c r="C468" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="469" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B469" t="s">
+        <v>618</v>
+      </c>
+      <c r="C469" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="470" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B470" t="s">
         <v>620</v>
       </c>
-      <c r="C468" t="s">
+      <c r="C470" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Trade Data WITS exports and codes
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="756">
   <si>
     <t>Country Name</t>
   </si>
@@ -2277,6 +2277,24 @@
   </si>
   <si>
     <t>Korea (North)</t>
+  </si>
+  <si>
+    <t>anguila</t>
+  </si>
+  <si>
+    <t>turks and caicos isl.</t>
+  </si>
+  <si>
+    <t>occ.pal.terr</t>
+  </si>
+  <si>
+    <t>macao</t>
+  </si>
+  <si>
+    <t>ethiopia(excludes eritrea)</t>
+  </si>
+  <si>
+    <t>yugoslavia</t>
   </si>
 </sst>
 </file>
@@ -2479,6 +2497,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="46">
@@ -3387,10 +3406,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F475"/>
+  <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C202" sqref="C202"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="E260" sqref="E260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,35 +3485,35 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>15</v>
+      <c r="B10" t="s">
+        <v>750</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -3502,47 +3521,47 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>725</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>725</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
@@ -3550,127 +3569,127 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>40</v>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>637</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>59</v>
+        <v>637</v>
       </c>
       <c r="C35" t="s">
         <v>60</v>
@@ -3678,15 +3697,15 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>715</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>61</v>
+        <v>715</v>
       </c>
       <c r="C37" t="s">
         <v>62</v>
@@ -3694,31 +3713,31 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>65</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
         <v>638</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>67</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
@@ -3726,63 +3745,63 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>639</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>81</v>
+        <v>639</v>
       </c>
       <c r="C49" t="s">
         <v>82</v>
@@ -3790,31 +3809,31 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
         <v>88</v>
@@ -3822,55 +3841,55 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>742</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>640</v>
+        <v>742</v>
       </c>
       <c r="C58" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="10" t="s">
-        <v>641</v>
+      <c r="B59" t="s">
+        <v>640</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>96</v>
+      <c r="B60" s="10" t="s">
+        <v>641</v>
       </c>
       <c r="C60" t="s">
         <v>97</v>
@@ -3878,71 +3897,71 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>733</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B66" s="11" t="s">
-        <v>642</v>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>729</v>
       </c>
       <c r="C66" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>643</v>
+    <row r="67" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="11" t="s">
+        <v>642</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
-        <v>644</v>
+      <c r="B68" t="s">
+        <v>643</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>104</v>
+      <c r="B69" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="C69" t="s">
         <v>105</v>
@@ -3950,7 +3969,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C70" t="s">
         <v>105</v>
@@ -3958,7 +3977,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
         <v>105</v>
@@ -3966,7 +3985,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>645</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
         <v>105</v>
@@ -3974,34 +3993,34 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>108</v>
+        <v>645</v>
       </c>
       <c r="C73" t="s">
         <v>105</v>
       </c>
-      <c r="D73" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>110</v>
-      </c>
-      <c r="C74" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="14" t="s">
-        <v>748</v>
       </c>
       <c r="C75" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>743</v>
+      <c r="B76" s="14" t="s">
+        <v>748</v>
       </c>
       <c r="C76" t="s">
         <v>111</v>
@@ -4009,7 +4028,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>112</v>
+        <v>743</v>
       </c>
       <c r="C77" t="s">
         <v>111</v>
@@ -4017,39 +4036,39 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>117</v>
-      </c>
-      <c r="C80" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="14" t="s">
-        <v>747</v>
       </c>
       <c r="C81" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>633</v>
+      <c r="B82" s="14" t="s">
+        <v>747</v>
       </c>
       <c r="C82" t="s">
         <v>118</v>
@@ -4057,7 +4076,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C83" t="s">
         <v>118</v>
@@ -4065,7 +4084,7 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C84" t="s">
         <v>118</v>
@@ -4073,31 +4092,31 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C85" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C86" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C87" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C88" t="s">
         <v>125</v>
@@ -4105,15 +4124,15 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>739</v>
+        <v>124</v>
       </c>
       <c r="C89" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>126</v>
+        <v>739</v>
       </c>
       <c r="C90" t="s">
         <v>127</v>
@@ -4121,23 +4140,23 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C91" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>728</v>
+        <v>128</v>
       </c>
       <c r="C92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>130</v>
+        <v>728</v>
       </c>
       <c r="C93" t="s">
         <v>131</v>
@@ -4145,55 +4164,55 @@
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C94" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C95" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C96" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C97" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
-        <v>139</v>
+      <c r="B98" t="s">
+        <v>138</v>
       </c>
       <c r="C98" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>622</v>
+      <c r="B99" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C100" t="s">
         <v>141</v>
@@ -4201,15 +4220,15 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C101" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C102" t="s">
         <v>143</v>
@@ -4217,23 +4236,23 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C103" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C104" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C105" t="s">
         <v>147</v>
@@ -4241,7 +4260,7 @@
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C106" t="s">
         <v>147</v>
@@ -4249,63 +4268,63 @@
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C109" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>726</v>
+        <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>156</v>
+        <v>726</v>
       </c>
       <c r="C111" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="12" t="s">
-        <v>648</v>
+      <c r="B112" t="s">
+        <v>156</v>
       </c>
       <c r="C112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>719</v>
+        <v>754</v>
       </c>
       <c r="C113" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>649</v>
+      <c r="B114" s="12" t="s">
+        <v>648</v>
       </c>
       <c r="C114" t="s">
         <v>159</v>
@@ -4313,7 +4332,7 @@
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>158</v>
+        <v>719</v>
       </c>
       <c r="C115" t="s">
         <v>159</v>
@@ -4321,87 +4340,87 @@
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>160</v>
+        <v>649</v>
       </c>
       <c r="C116" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>624</v>
+        <v>158</v>
       </c>
       <c r="C117" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C118" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="C119" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C120" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>166</v>
+        <v>629</v>
       </c>
       <c r="C121" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C122" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C123" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>650</v>
+        <v>168</v>
       </c>
       <c r="C124" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C125" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>173</v>
+        <v>650</v>
       </c>
       <c r="C126" t="s">
         <v>172</v>
@@ -4409,263 +4428,263 @@
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C127" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C128" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C129" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C130" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C131" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C132" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C133" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C134" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C135" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>651</v>
+        <v>188</v>
       </c>
       <c r="C136" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C137" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>193</v>
+        <v>651</v>
       </c>
       <c r="C138" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C139" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C140" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C141" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C142" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>652</v>
+        <v>199</v>
       </c>
       <c r="C143" t="s">
-        <v>653</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C144" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>205</v>
+        <v>652</v>
       </c>
       <c r="C145" t="s">
-        <v>206</v>
+        <v>653</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C146" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C147" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C148" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C149" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="5" t="s">
-        <v>215</v>
+      <c r="B150" t="s">
+        <v>211</v>
       </c>
       <c r="C150" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C151" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>218</v>
+      <c r="B152" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C152" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C153" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C154" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C155" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C156" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>740</v>
+        <v>224</v>
       </c>
       <c r="C157" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>716</v>
+        <v>226</v>
       </c>
       <c r="C158" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>654</v>
+        <v>740</v>
       </c>
       <c r="C159" t="s">
         <v>229</v>
@@ -4673,7 +4692,7 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>655</v>
+        <v>716</v>
       </c>
       <c r="C160" t="s">
         <v>229</v>
@@ -4681,7 +4700,7 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C161" t="s">
         <v>229</v>
@@ -4689,7 +4708,7 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C162" t="s">
         <v>229</v>
@@ -4697,7 +4716,7 @@
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>634</v>
+        <v>656</v>
       </c>
       <c r="C163" t="s">
         <v>229</v>
@@ -4705,7 +4724,7 @@
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>228</v>
+        <v>657</v>
       </c>
       <c r="C164" t="s">
         <v>229</v>
@@ -4713,7 +4732,7 @@
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>230</v>
+        <v>634</v>
       </c>
       <c r="C165" t="s">
         <v>229</v>
@@ -4721,7 +4740,7 @@
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C166" t="s">
         <v>229</v>
@@ -4729,79 +4748,79 @@
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>727</v>
+        <v>230</v>
       </c>
       <c r="C167" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C168" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>234</v>
+        <v>727</v>
       </c>
       <c r="C169" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B170" s="6" t="s">
-        <v>236</v>
+      <c r="B170" t="s">
+        <v>232</v>
       </c>
       <c r="C170" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C171" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C172" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>658</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C173" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>732</v>
-      </c>
-      <c r="C174" t="s">
-        <v>242</v>
+        <v>658</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>659</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="C175" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>241</v>
+        <v>732</v>
       </c>
       <c r="C176" t="s">
         <v>242</v>
@@ -4809,7 +4828,7 @@
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>242</v>
@@ -4817,167 +4836,167 @@
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>635</v>
-      </c>
-      <c r="C178" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C178" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>243</v>
-      </c>
-      <c r="C179" t="s">
+        <v>660</v>
+      </c>
+      <c r="C179" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="180" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B180" s="11" t="s">
-        <v>661</v>
-      </c>
-      <c r="C180" t="s">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>635</v>
+      </c>
+      <c r="C180" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C181" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>245</v>
+    <row r="182" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B182" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C182" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C183" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B184" s="4" t="s">
-        <v>249</v>
+      <c r="B184" t="s">
+        <v>245</v>
       </c>
       <c r="C184" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C185" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
-        <v>252</v>
+      <c r="B186" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C186" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C187" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C188" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C189" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C190" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C191" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C192" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C193" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C194" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C195" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C196" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>662</v>
+        <v>269</v>
       </c>
       <c r="C197" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="198" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B198" s="11" t="s">
-        <v>712</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>271</v>
       </c>
       <c r="C198" t="s">
         <v>272</v>
@@ -4985,23 +5004,23 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C199" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="10" t="s">
-        <v>664</v>
+    <row r="200" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B200" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C200" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="10" t="s">
-        <v>749</v>
+      <c r="B201" t="s">
+        <v>663</v>
       </c>
       <c r="C201" t="s">
         <v>272</v>
@@ -5009,47 +5028,47 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C202" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>273</v>
+      <c r="B203" s="10" t="s">
+        <v>749</v>
       </c>
       <c r="C203" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>731</v>
+      <c r="B204" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C204" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>666</v>
+        <v>273</v>
       </c>
       <c r="C205" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>717</v>
+        <v>731</v>
       </c>
       <c r="C206" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="4" t="s">
-        <v>274</v>
+      <c r="B207" t="s">
+        <v>666</v>
       </c>
       <c r="C207" t="s">
         <v>275</v>
@@ -5057,15 +5076,15 @@
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>667</v>
+        <v>717</v>
       </c>
       <c r="C208" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>276</v>
+      <c r="B209" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C209" t="s">
         <v>275</v>
@@ -5073,7 +5092,7 @@
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>636</v>
+        <v>667</v>
       </c>
       <c r="C210" t="s">
         <v>275</v>
@@ -5081,7 +5100,7 @@
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C211" t="s">
         <v>275</v>
@@ -5089,7 +5108,7 @@
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>278</v>
+        <v>636</v>
       </c>
       <c r="C212" t="s">
         <v>275</v>
@@ -5097,7 +5116,7 @@
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>668</v>
+        <v>277</v>
       </c>
       <c r="C213" t="s">
         <v>275</v>
@@ -5105,7 +5124,7 @@
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>669</v>
+        <v>278</v>
       </c>
       <c r="C214" t="s">
         <v>275</v>
@@ -5113,55 +5132,55 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>279</v>
+        <v>668</v>
       </c>
       <c r="C215" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>281</v>
+        <v>669</v>
       </c>
       <c r="C216" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" s="4" t="s">
-        <v>283</v>
+      <c r="B217" t="s">
+        <v>279</v>
       </c>
       <c r="C217" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C218" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C219" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
-        <v>286</v>
-      </c>
-      <c r="C219" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>670</v>
+        <v>285</v>
       </c>
       <c r="C220" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B221" s="10" t="s">
-        <v>671</v>
+      <c r="B221" t="s">
+        <v>286</v>
       </c>
       <c r="C221" t="s">
         <v>287</v>
@@ -5169,15 +5188,15 @@
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>288</v>
+        <v>670</v>
       </c>
       <c r="C222" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
-        <v>734</v>
+      <c r="B223" s="10" t="s">
+        <v>671</v>
       </c>
       <c r="C223" t="s">
         <v>287</v>
@@ -5185,7 +5204,7 @@
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>672</v>
+        <v>288</v>
       </c>
       <c r="C224" t="s">
         <v>287</v>
@@ -5193,7 +5212,7 @@
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>289</v>
+        <v>734</v>
       </c>
       <c r="C225" t="s">
         <v>287</v>
@@ -5201,95 +5220,95 @@
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>625</v>
+        <v>672</v>
       </c>
       <c r="C226" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C227" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C228" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C229" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>294</v>
+        <v>626</v>
       </c>
       <c r="C230" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C231" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C232" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C233" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C234" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="235" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B235" s="11" t="s">
-        <v>713</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>300</v>
       </c>
       <c r="C235" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C236" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B237" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B237" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C237" t="s">
         <v>305</v>
@@ -5297,87 +5316,87 @@
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C238" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B239" t="s">
-        <v>309</v>
+      <c r="B239" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="C239" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>630</v>
+        <v>307</v>
       </c>
       <c r="C240" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C241" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="242" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>313</v>
+        <v>630</v>
       </c>
       <c r="C242" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C243" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>724</v>
+        <v>313</v>
       </c>
       <c r="C244" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C245" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>741</v>
+        <v>724</v>
       </c>
       <c r="C246" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="247" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>673</v>
+        <v>317</v>
       </c>
       <c r="C247" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="248" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>674</v>
+        <v>753</v>
       </c>
       <c r="C248" t="s">
         <v>320</v>
@@ -5385,7 +5404,7 @@
     </row>
     <row r="249" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>319</v>
+        <v>741</v>
       </c>
       <c r="C249" t="s">
         <v>320</v>
@@ -5393,7 +5412,7 @@
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C250" t="s">
         <v>320</v>
@@ -5401,7 +5420,7 @@
     </row>
     <row r="251" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>321</v>
+        <v>674</v>
       </c>
       <c r="C251" t="s">
         <v>320</v>
@@ -5409,72 +5428,72 @@
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C252" t="s">
         <v>320</v>
       </c>
-      <c r="E252" s="4"/>
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>323</v>
+        <v>675</v>
       </c>
       <c r="C253" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B254" s="4" t="s">
+      <c r="B254" t="s">
+        <v>321</v>
+      </c>
+      <c r="C254" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
+        <v>322</v>
+      </c>
+      <c r="C255" t="s">
+        <v>320</v>
+      </c>
+      <c r="E255" s="4"/>
+    </row>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
+        <v>323</v>
+      </c>
+      <c r="C256" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B257" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="C254" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="255" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B255" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C255" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="256" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B256" s="11" t="s">
-        <v>677</v>
-      </c>
-      <c r="C256" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B257" t="s">
-        <v>678</v>
       </c>
       <c r="C257" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="258" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B258" t="s">
-        <v>326</v>
+      <c r="B258" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C258" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="259" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B259" t="s">
-        <v>327</v>
+      <c r="B259" s="4" t="s">
+        <v>755</v>
       </c>
       <c r="C259" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
-        <v>328</v>
+    <row r="260" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B260" s="11" t="s">
+        <v>677</v>
       </c>
       <c r="C260" t="s">
         <v>325</v>
@@ -5482,513 +5501,513 @@
     </row>
     <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>329</v>
+        <v>678</v>
       </c>
       <c r="C261" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C262" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C263" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C264" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C265" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C266" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C267" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C268" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="269" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C269" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="270" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C270" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="271" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C271" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="272" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C272" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="273" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C273" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="274" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C274" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="275" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>720</v>
+        <v>349</v>
       </c>
       <c r="C275" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="276" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B276" s="10" t="s">
-        <v>679</v>
+      <c r="B276" t="s">
+        <v>351</v>
       </c>
       <c r="C276" t="s">
-        <v>354</v>
-      </c>
-      <c r="F276" s="4"/>
+        <v>352</v>
+      </c>
     </row>
     <row r="277" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>627</v>
+        <v>353</v>
       </c>
       <c r="C277" t="s">
-        <v>357</v>
-      </c>
-      <c r="F277" s="4"/>
+        <v>354</v>
+      </c>
     </row>
     <row r="278" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C278" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="279" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>628</v>
+        <v>720</v>
       </c>
       <c r="C279" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="280" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B280" t="s">
-        <v>358</v>
+      <c r="B280" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C280" t="s">
-        <v>359</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="F280" s="4"/>
     </row>
     <row r="281" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>360</v>
+        <v>627</v>
       </c>
       <c r="C281" t="s">
-        <v>361</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="F281" s="4"/>
     </row>
     <row r="282" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>680</v>
+        <v>356</v>
       </c>
       <c r="C282" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="283" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>362</v>
+        <v>628</v>
       </c>
       <c r="C283" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="284" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>681</v>
+        <v>358</v>
       </c>
       <c r="C284" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="285" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B285" s="4" t="s">
-        <v>364</v>
+      <c r="B285" t="s">
+        <v>360</v>
       </c>
       <c r="C285" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="286" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>365</v>
+        <v>680</v>
       </c>
       <c r="C286" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="287" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C287" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="288" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>369</v>
+        <v>681</v>
       </c>
       <c r="C288" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B289" t="s">
-        <v>371</v>
+      <c r="B289" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C289" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C290" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="C291" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C292" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C293" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C294" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C295" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B296" s="13" t="s">
-        <v>746</v>
+      <c r="B296" t="s">
+        <v>377</v>
       </c>
       <c r="C296" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C297" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C298" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B299" s="4" t="s">
-        <v>389</v>
+      <c r="B299" t="s">
+        <v>383</v>
       </c>
       <c r="C299" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B300" t="s">
-        <v>390</v>
+      <c r="B300" s="13" t="s">
+        <v>746</v>
       </c>
       <c r="C300" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C301" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C302" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B303" t="s">
-        <v>395</v>
+      <c r="B303" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C303" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C304" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C305" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C306" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C307" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C308" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C309" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C310" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C311" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C312" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C313" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C314" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C315" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C316" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="C317" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C318" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C319" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>682</v>
+        <v>419</v>
       </c>
       <c r="C320" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C321" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>683</v>
+        <v>423</v>
       </c>
       <c r="C322" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C323" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B324" s="4" t="s">
-        <v>430</v>
+      <c r="B324" t="s">
+        <v>682</v>
       </c>
       <c r="C324" t="s">
         <v>428</v>
@@ -5996,637 +6015,634 @@
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>684</v>
+        <v>427</v>
       </c>
       <c r="C325" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>431</v>
+        <v>752</v>
       </c>
       <c r="C326" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>433</v>
+        <v>683</v>
       </c>
       <c r="C327" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C328" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B329" t="s">
-        <v>437</v>
+      <c r="B329" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C329" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>439</v>
+        <v>684</v>
       </c>
       <c r="C330" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C331" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="C332" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>631</v>
+        <v>435</v>
       </c>
       <c r="C333" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C334" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C335" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C336" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C337" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>453</v>
+        <v>631</v>
       </c>
       <c r="C338" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="C339" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C340" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C341" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="C342" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>685</v>
+        <v>453</v>
       </c>
       <c r="C343" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>632</v>
+        <v>455</v>
       </c>
       <c r="C344" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="345" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C345" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="346" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C346" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="347" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C347" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="348" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>466</v>
+        <v>685</v>
       </c>
       <c r="C348" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="349" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>468</v>
+        <v>632</v>
       </c>
       <c r="C349" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="350" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B350" s="11" t="s">
-        <v>730</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
+        <v>462</v>
       </c>
       <c r="C350" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="351" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B351" s="11" t="s">
-        <v>714</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
+        <v>464</v>
       </c>
       <c r="C351" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C352" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B353" s="4" t="s">
-        <v>472</v>
+      <c r="B353" t="s">
+        <v>466</v>
       </c>
       <c r="C353" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="354" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C354" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="355" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B355" t="s">
-        <v>475</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="355" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B355" s="11" t="s">
+        <v>730</v>
       </c>
       <c r="C355" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="356" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B356" t="s">
-        <v>477</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="356" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B356" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C356" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="C357" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="358" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B358" t="s">
-        <v>481</v>
+      <c r="B358" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C358" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B359" s="4" t="s">
-        <v>482</v>
+      <c r="B359" t="s">
+        <v>473</v>
       </c>
       <c r="C359" t="s">
-        <v>483</v>
-      </c>
-      <c r="E359" s="4"/>
+        <v>474</v>
+      </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="C360" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="361" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="C361" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="362" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C362" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="363" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="C363" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
     </row>
     <row r="364" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B364" t="s">
-        <v>491</v>
+      <c r="B364" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C364" t="s">
-        <v>492</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E364" s="4"/>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="C365" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="C366" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="C367" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="C368" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
     </row>
     <row r="369" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="C369" t="s">
-        <v>502</v>
-      </c>
-      <c r="E369" s="4"/>
+        <v>492</v>
+      </c>
     </row>
     <row r="370" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>686</v>
+        <v>493</v>
       </c>
       <c r="C370" t="s">
-        <v>19</v>
-      </c>
-      <c r="E370" s="4"/>
+        <v>494</v>
+      </c>
     </row>
     <row r="371" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="C371" t="s">
-        <v>19</v>
+        <v>496</v>
       </c>
     </row>
     <row r="372" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>687</v>
+        <v>497</v>
       </c>
       <c r="C372" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="373" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C373" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="374" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C374" t="s">
-        <v>505</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E374" s="4"/>
     </row>
     <row r="375" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C375" t="s">
-        <v>508</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E375" s="4"/>
     </row>
     <row r="376" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C376" t="s">
-        <v>508</v>
+        <v>19</v>
       </c>
     </row>
     <row r="377" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>509</v>
+        <v>687</v>
       </c>
       <c r="C377" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="378" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>689</v>
+        <v>504</v>
       </c>
       <c r="C378" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="379" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="C379" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="380" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>513</v>
+        <v>688</v>
       </c>
       <c r="C380" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="381" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="C381" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="382" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>690</v>
+        <v>509</v>
       </c>
       <c r="C382" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="383" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>516</v>
+        <v>689</v>
       </c>
       <c r="C383" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="384" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C384" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="385" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C385" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="386" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>721</v>
+        <v>514</v>
       </c>
       <c r="C386" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="387" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C387" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="388" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>692</v>
+        <v>516</v>
       </c>
       <c r="C388" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="389" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C389" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="390" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C390" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="391" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>525</v>
+        <v>721</v>
       </c>
       <c r="C391" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="392" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>527</v>
+        <v>691</v>
       </c>
       <c r="C392" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="393" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>529</v>
+        <v>692</v>
       </c>
       <c r="C393" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="394" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C394" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C395" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="396" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>693</v>
+        <v>525</v>
       </c>
       <c r="C396" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="397" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B397" s="13" t="s">
-        <v>745</v>
+      <c r="B397" t="s">
+        <v>527</v>
       </c>
       <c r="C397" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="398" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>744</v>
+        <v>529</v>
       </c>
       <c r="C398" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="399" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>735</v>
+        <v>531</v>
       </c>
       <c r="C399" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="400" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C400" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="401" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>536</v>
+        <v>693</v>
       </c>
       <c r="C401" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="402" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B402" t="s">
-        <v>537</v>
+      <c r="B402" s="13" t="s">
+        <v>745</v>
       </c>
       <c r="C402" t="s">
         <v>535</v>
       </c>
-      <c r="D402" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="403" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>538</v>
+        <v>744</v>
       </c>
       <c r="C403" t="s">
         <v>535</v>
@@ -6634,399 +6650,402 @@
     </row>
     <row r="404" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>539</v>
+        <v>735</v>
       </c>
       <c r="C404" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="405" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>722</v>
+        <v>534</v>
       </c>
       <c r="C405" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="406" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B406" s="10" t="s">
-        <v>694</v>
+      <c r="B406" t="s">
+        <v>536</v>
       </c>
       <c r="C406" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="407" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="C407" t="s">
-        <v>542</v>
+        <v>535</v>
+      </c>
+      <c r="D407" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="408" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>723</v>
+        <v>538</v>
       </c>
       <c r="C408" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="409" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B409" s="11" t="s">
-        <v>696</v>
+        <v>535</v>
+      </c>
+    </row>
+    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B409" t="s">
+        <v>539</v>
       </c>
       <c r="C409" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="410" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>697</v>
+        <v>722</v>
       </c>
       <c r="C410" t="s">
-        <v>542</v>
+        <v>695</v>
       </c>
     </row>
     <row r="411" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B411" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="C411" s="1" t="s">
-        <v>542</v>
+      <c r="B411" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="C411" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="412" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B412" s="10" t="s">
-        <v>699</v>
+      <c r="B412" t="s">
+        <v>541</v>
       </c>
       <c r="C412" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="413" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B413" s="4" t="s">
-        <v>543</v>
+      <c r="B413" t="s">
+        <v>723</v>
       </c>
       <c r="C413" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B414" t="s">
-        <v>544</v>
+    <row r="414" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B414" s="11" t="s">
+        <v>696</v>
       </c>
       <c r="C414" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="415" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C415" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="416" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B416" t="s">
-        <v>546</v>
-      </c>
-      <c r="C416" t="s">
-        <v>547</v>
+      <c r="B416" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B417" t="s">
-        <v>548</v>
+      <c r="B417" s="10" t="s">
+        <v>699</v>
       </c>
       <c r="C417" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B418" t="s">
-        <v>550</v>
+      <c r="B418" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C418" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="C419" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>718</v>
+        <v>700</v>
       </c>
       <c r="C420" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C421" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="C422" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C423" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C424" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>561</v>
+        <v>718</v>
       </c>
       <c r="C425" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="C426" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B427" s="4" t="s">
-        <v>565</v>
+      <c r="B427" t="s">
+        <v>556</v>
       </c>
       <c r="C427" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="C428" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="C429" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C430" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>571</v>
+        <v>751</v>
       </c>
       <c r="C431" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>738</v>
+        <v>563</v>
       </c>
       <c r="C432" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B433" t="s">
-        <v>737</v>
+      <c r="B433" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C433" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C434" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>701</v>
+        <v>567</v>
       </c>
       <c r="C435" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C436" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C437" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B438" s="4" t="s">
-        <v>579</v>
+      <c r="B438" t="s">
+        <v>738</v>
       </c>
       <c r="C438" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>580</v>
+        <v>737</v>
       </c>
       <c r="C439" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="C440" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>584</v>
+        <v>701</v>
       </c>
       <c r="C441" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>702</v>
+        <v>575</v>
       </c>
       <c r="C442" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>703</v>
+        <v>577</v>
       </c>
       <c r="C443" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B444" t="s">
-        <v>586</v>
+      <c r="B444" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C444" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="C445" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="C446" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" s="4" t="s">
-        <v>591</v>
+      <c r="B447" t="s">
+        <v>584</v>
       </c>
       <c r="C447" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>593</v>
+        <v>702</v>
       </c>
       <c r="C448" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>594</v>
+        <v>703</v>
       </c>
       <c r="C449" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="C450" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="451" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B451" s="11" t="s">
-        <v>704</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B451" t="s">
+        <v>588</v>
       </c>
       <c r="C451" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B452" s="10" t="s">
-        <v>705</v>
+      <c r="B452" t="s">
+        <v>589</v>
       </c>
       <c r="C452" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B453" t="s">
-        <v>596</v>
+      <c r="B453" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C453" t="s">
         <v>592</v>
@@ -7034,177 +7053,225 @@
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C454" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="C455" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>736</v>
+        <v>595</v>
       </c>
       <c r="C456" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B457" t="s">
-        <v>600</v>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="457" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B457" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C457" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B458" t="s">
-        <v>602</v>
+      <c r="B458" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C458" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>706</v>
+        <v>596</v>
       </c>
       <c r="C459" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C460" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="C461" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B462" s="4" t="s">
-        <v>606</v>
+      <c r="B462" t="s">
+        <v>736</v>
       </c>
       <c r="C462" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B463" s="4" t="s">
-        <v>707</v>
+      <c r="B463" t="s">
+        <v>600</v>
       </c>
       <c r="C463" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
-        <v>708</v>
+        <v>602</v>
       </c>
       <c r="C464" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>607</v>
+        <v>706</v>
       </c>
       <c r="C465" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>710</v>
+        <v>603</v>
       </c>
       <c r="C466" t="s">
-        <v>711</v>
+        <v>604</v>
       </c>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C467" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B468" t="s">
-        <v>611</v>
+      <c r="B468" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C468" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B469" t="s">
-        <v>613</v>
+      <c r="B469" s="4" t="s">
+        <v>707</v>
       </c>
       <c r="C469" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="470" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C470" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="471" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B471" s="4" t="s">
-        <v>615</v>
+      <c r="B471" t="s">
+        <v>607</v>
       </c>
       <c r="C471" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="472" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>616</v>
+        <v>710</v>
       </c>
       <c r="C472" t="s">
-        <v>614</v>
+        <v>711</v>
       </c>
     </row>
     <row r="473" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C473" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="474" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="C474" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
+        <v>613</v>
+      </c>
+      <c r="C475" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B476" t="s">
+        <v>709</v>
+      </c>
+      <c r="C476" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="477" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B477" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C477" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="478" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B478" t="s">
+        <v>616</v>
+      </c>
+      <c r="C478" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B479" t="s">
+        <v>617</v>
+      </c>
+      <c r="C479" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="480" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B480" t="s">
+        <v>618</v>
+      </c>
+      <c r="C480" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="481" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B481" t="s">
         <v>620</v>
       </c>
-      <c r="C475" t="s">
+      <c r="C481" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added cleaning codes for linkedin users and journals
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="781">
   <si>
     <t>Country Name</t>
   </si>
@@ -2349,6 +2349,27 @@
   </si>
   <si>
     <t>rep of georgia</t>
+  </si>
+  <si>
+    <t>Sao Tome Prin</t>
+  </si>
+  <si>
+    <t>serbia monteneg</t>
+  </si>
+  <si>
+    <t>st kitts nevi</t>
+  </si>
+  <si>
+    <t>st lucia</t>
+  </si>
+  <si>
+    <t>Surinam</t>
+  </si>
+  <si>
+    <t>u arab emirates</t>
+  </si>
+  <si>
+    <t>Western samoa</t>
   </si>
 </sst>
 </file>
@@ -3460,10 +3481,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F500"/>
+  <dimension ref="A1:F507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" topLeftCell="A483" workbookViewId="0">
+      <selection activeCell="B507" sqref="B507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6365,7 +6386,7 @@
     </row>
     <row r="362" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>458</v>
+        <v>780</v>
       </c>
       <c r="C362" t="s">
         <v>459</v>
@@ -6373,23 +6394,23 @@
     </row>
     <row r="363" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C363" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="364" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>685</v>
+        <v>460</v>
       </c>
       <c r="C364" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="365" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>632</v>
+        <v>685</v>
       </c>
       <c r="C365" t="s">
         <v>463</v>
@@ -6397,7 +6418,7 @@
     </row>
     <row r="366" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>462</v>
+        <v>632</v>
       </c>
       <c r="C366" t="s">
         <v>463</v>
@@ -6405,7 +6426,7 @@
     </row>
     <row r="367" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C367" t="s">
         <v>463</v>
@@ -6413,7 +6434,7 @@
     </row>
     <row r="368" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C368" t="s">
         <v>463</v>
@@ -6421,453 +6442,450 @@
     </row>
     <row r="369" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>466</v>
+        <v>774</v>
       </c>
       <c r="C369" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="370" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
+        <v>465</v>
+      </c>
+      <c r="C370" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="371" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>466</v>
+      </c>
+      <c r="C371" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="372" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
         <v>468</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C372" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="371" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B371" s="11" t="s">
-        <v>730</v>
-      </c>
-      <c r="C371" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="372" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B372" s="11" t="s">
-        <v>714</v>
-      </c>
-      <c r="C372" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="373" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>470</v>
+        <v>775</v>
       </c>
       <c r="C373" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="374" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B374" s="4" t="s">
-        <v>472</v>
+    <row r="374" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B374" s="11" t="s">
+        <v>730</v>
       </c>
       <c r="C374" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="375" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B375" t="s">
-        <v>473</v>
+    <row r="375" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B375" s="11" t="s">
+        <v>714</v>
       </c>
       <c r="C375" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="376" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C376" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="377" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B377" t="s">
-        <v>477</v>
+      <c r="B377" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C377" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="378" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C378" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="379" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C379" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="380" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B380" s="4" t="s">
-        <v>482</v>
+      <c r="B380" t="s">
+        <v>477</v>
       </c>
       <c r="C380" t="s">
-        <v>483</v>
-      </c>
-      <c r="E380" s="4"/>
+        <v>478</v>
+      </c>
     </row>
     <row r="381" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C381" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="382" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C382" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="383" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B383" t="s">
-        <v>487</v>
+      <c r="B383" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C383" t="s">
-        <v>488</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E383" s="4"/>
     </row>
     <row r="384" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C384" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="385" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C385" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="386" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="C386" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="387" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="C387" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="388" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C388" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="389" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C389" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="390" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C390" t="s">
-        <v>502</v>
-      </c>
-      <c r="E390" s="4"/>
+        <v>496</v>
+      </c>
     </row>
     <row r="391" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>686</v>
+        <v>497</v>
       </c>
       <c r="C391" t="s">
-        <v>19</v>
-      </c>
-      <c r="E391" s="4"/>
+        <v>498</v>
+      </c>
     </row>
     <row r="392" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C392" t="s">
-        <v>19</v>
+        <v>500</v>
       </c>
     </row>
     <row r="393" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>687</v>
+        <v>501</v>
       </c>
       <c r="C393" t="s">
-        <v>505</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E393" s="4"/>
     </row>
     <row r="394" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>504</v>
+        <v>686</v>
       </c>
       <c r="C394" t="s">
-        <v>505</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E394" s="4"/>
     </row>
     <row r="395" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C395" t="s">
-        <v>505</v>
+        <v>19</v>
       </c>
     </row>
     <row r="396" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>688</v>
+        <v>776</v>
       </c>
       <c r="C396" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="397" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>507</v>
+        <v>687</v>
       </c>
       <c r="C397" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="398" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C398" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="399" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>689</v>
+        <v>506</v>
       </c>
       <c r="C399" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="400" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>511</v>
+        <v>777</v>
       </c>
       <c r="C400" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>513</v>
+        <v>688</v>
       </c>
       <c r="C401" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="C402" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>690</v>
+        <v>509</v>
       </c>
       <c r="C403" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>516</v>
+        <v>689</v>
       </c>
       <c r="C404" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C405" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C406" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>721</v>
+        <v>514</v>
       </c>
       <c r="C407" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C408" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>692</v>
+        <v>516</v>
       </c>
       <c r="C409" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C410" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C411" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>525</v>
+        <v>721</v>
       </c>
       <c r="C412" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>527</v>
+        <v>691</v>
       </c>
       <c r="C413" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>529</v>
+        <v>692</v>
       </c>
       <c r="C414" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C415" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>533</v>
+        <v>778</v>
       </c>
       <c r="C416" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="417" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>693</v>
+        <v>523</v>
       </c>
       <c r="C417" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
     </row>
     <row r="418" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B418" s="13" t="s">
-        <v>745</v>
+      <c r="B418" t="s">
+        <v>525</v>
       </c>
       <c r="C418" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="419" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>744</v>
+        <v>527</v>
       </c>
       <c r="C419" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="420" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>735</v>
+        <v>529</v>
       </c>
       <c r="C420" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="421" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C421" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="422" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C422" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="423" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>537</v>
+        <v>693</v>
       </c>
       <c r="C423" t="s">
         <v>535</v>
       </c>
-      <c r="D423" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="424" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B424" t="s">
-        <v>538</v>
+      <c r="B424" s="13" t="s">
+        <v>745</v>
       </c>
       <c r="C424" t="s">
         <v>535</v>
@@ -6875,79 +6893,82 @@
     </row>
     <row r="425" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>539</v>
+        <v>744</v>
       </c>
       <c r="C425" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="426" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="C426" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="427" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B427" s="10" t="s">
-        <v>694</v>
+      <c r="B427" t="s">
+        <v>534</v>
       </c>
       <c r="C427" t="s">
-        <v>695</v>
+        <v>535</v>
       </c>
     </row>
     <row r="428" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="C428" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
     </row>
     <row r="429" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>723</v>
+        <v>537</v>
       </c>
       <c r="C429" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="430" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B430" s="11" t="s">
-        <v>696</v>
+        <v>535</v>
+      </c>
+      <c r="D429" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="430" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B430" t="s">
+        <v>538</v>
       </c>
       <c r="C430" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
     </row>
     <row r="431" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>697</v>
+        <v>539</v>
       </c>
       <c r="C431" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="432" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B432" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="C432" s="1" t="s">
-        <v>542</v>
+      <c r="B432" t="s">
+        <v>722</v>
+      </c>
+      <c r="C432" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" s="10" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="C433" t="s">
-        <v>542</v>
+        <v>695</v>
       </c>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B434" s="4" t="s">
-        <v>543</v>
+      <c r="B434" t="s">
+        <v>541</v>
       </c>
       <c r="C434" t="s">
         <v>542</v>
@@ -6955,529 +6976,585 @@
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>544</v>
+        <v>723</v>
       </c>
       <c r="C435" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B436" t="s">
-        <v>700</v>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="436" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B436" s="11" t="s">
+        <v>696</v>
       </c>
       <c r="C436" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>546</v>
+        <v>697</v>
       </c>
       <c r="C437" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B438" t="s">
-        <v>548</v>
-      </c>
-      <c r="C438" t="s">
-        <v>549</v>
+      <c r="B438" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B439" t="s">
-        <v>550</v>
+      <c r="B439" s="10" t="s">
+        <v>699</v>
       </c>
       <c r="C439" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B440" t="s">
-        <v>552</v>
+      <c r="B440" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C440" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>718</v>
+        <v>544</v>
       </c>
       <c r="C441" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>756</v>
+        <v>700</v>
       </c>
       <c r="C442" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C443" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="C444" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C445" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C446" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>561</v>
+        <v>718</v>
       </c>
       <c r="C447" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="C448" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="C449" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B450" s="4" t="s">
-        <v>565</v>
+      <c r="B450" t="s">
+        <v>556</v>
       </c>
       <c r="C450" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="C451" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="C452" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C453" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>571</v>
+        <v>751</v>
       </c>
       <c r="C454" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>738</v>
+        <v>563</v>
       </c>
       <c r="C455" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B456" t="s">
-        <v>737</v>
+      <c r="B456" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C456" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C457" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>701</v>
+        <v>567</v>
       </c>
       <c r="C458" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>763</v>
+        <v>569</v>
       </c>
       <c r="C459" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C460" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>578</v>
+        <v>738</v>
       </c>
       <c r="C461" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>577</v>
+        <v>779</v>
       </c>
       <c r="C462" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B463" s="4" t="s">
-        <v>579</v>
+      <c r="B463" t="s">
+        <v>737</v>
       </c>
       <c r="C463" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="C464" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>582</v>
+        <v>701</v>
       </c>
       <c r="C465" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>584</v>
+        <v>763</v>
       </c>
       <c r="C466" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>702</v>
+        <v>575</v>
       </c>
       <c r="C467" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
-        <v>703</v>
+        <v>578</v>
       </c>
       <c r="C468" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="C469" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="470" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B470" t="s">
-        <v>588</v>
+      <c r="B470" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C470" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="471" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="C471" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
     </row>
     <row r="472" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B472" s="4" t="s">
-        <v>591</v>
+      <c r="B472" t="s">
+        <v>582</v>
       </c>
       <c r="C472" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
     </row>
     <row r="473" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="C473" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="474" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>594</v>
+        <v>702</v>
       </c>
       <c r="C474" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>595</v>
+        <v>703</v>
       </c>
       <c r="C475" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="476" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B476" s="11" t="s">
-        <v>704</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B476" t="s">
+        <v>586</v>
       </c>
       <c r="C476" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="477" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B477" s="10" t="s">
-        <v>705</v>
+      <c r="B477" t="s">
+        <v>588</v>
       </c>
       <c r="C477" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="478" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C478" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B479" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C479" t="s">
         <v>592</v>
-      </c>
-    </row>
-    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B479" t="s">
-        <v>597</v>
-      </c>
-      <c r="C479" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="480" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C480" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="481" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
-        <v>736</v>
+        <v>594</v>
       </c>
       <c r="C481" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="482" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="C482" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B483" t="s">
-        <v>602</v>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="483" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B483" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C483" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="484" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B484" t="s">
-        <v>706</v>
+      <c r="B484" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C484" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="485" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="C485" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="486" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C486" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="487" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B487" s="4" t="s">
-        <v>606</v>
+      <c r="B487" t="s">
+        <v>599</v>
       </c>
       <c r="C487" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="488" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B488" s="4" t="s">
-        <v>707</v>
+      <c r="B488" t="s">
+        <v>736</v>
       </c>
       <c r="C488" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="489" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B489" t="s">
-        <v>708</v>
+        <v>600</v>
       </c>
       <c r="C489" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="490" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B490" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="C490" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="491" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="C491" t="s">
-        <v>711</v>
+        <v>604</v>
       </c>
     </row>
     <row r="492" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C492" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="493" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="C493" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="494" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B494" t="s">
-        <v>613</v>
+      <c r="B494" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C494" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
     </row>
     <row r="495" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B495" t="s">
-        <v>709</v>
+      <c r="B495" s="4" t="s">
+        <v>707</v>
       </c>
       <c r="C495" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="496" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B496" s="4" t="s">
-        <v>615</v>
+      <c r="B496" t="s">
+        <v>708</v>
       </c>
       <c r="C496" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="C497" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="498" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>617</v>
+        <v>710</v>
       </c>
       <c r="C498" t="s">
-        <v>614</v>
+        <v>711</v>
       </c>
     </row>
     <row r="499" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="C499" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
     </row>
     <row r="500" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
+        <v>611</v>
+      </c>
+      <c r="C500" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="501" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B501" t="s">
+        <v>613</v>
+      </c>
+      <c r="C501" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="502" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B502" t="s">
+        <v>709</v>
+      </c>
+      <c r="C502" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="503" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B503" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C503" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="504" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B504" t="s">
+        <v>616</v>
+      </c>
+      <c r="C504" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="505" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B505" t="s">
+        <v>617</v>
+      </c>
+      <c r="C505" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="506" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B506" t="s">
+        <v>618</v>
+      </c>
+      <c r="C506" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="507" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B507" t="s">
         <v>620</v>
       </c>
-      <c r="C500" t="s">
+      <c r="C507" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added codes for RPI
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="788">
   <si>
     <t>Country Name</t>
   </si>
@@ -2370,6 +2370,27 @@
   </si>
   <si>
     <t>Western samoa</t>
+  </si>
+  <si>
+    <t>china  hong kong sar</t>
+  </si>
+  <si>
+    <t>china  macao sar</t>
+  </si>
+  <si>
+    <t>democratic republic of congo</t>
+  </si>
+  <si>
+    <t>iran  islamic republic of</t>
+  </si>
+  <si>
+    <t>korea  democratic people's rep. of</t>
+  </si>
+  <si>
+    <t>korea  republic of</t>
+  </si>
+  <si>
+    <t>the former yugoslav rep. of macedonia</t>
   </si>
 </sst>
 </file>
@@ -3481,10 +3502,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F507"/>
+  <dimension ref="A1:F514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A483" workbookViewId="0">
-      <selection activeCell="B507" sqref="B507"/>
+    <sheetView tabSelected="1" topLeftCell="A490" workbookViewId="0">
+      <selection activeCell="B514" sqref="B514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4075,16 +4096,16 @@
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
-        <v>644</v>
+      <c r="B74" t="s">
+        <v>783</v>
       </c>
       <c r="C74" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>104</v>
+      <c r="B75" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="C75" t="s">
         <v>105</v>
@@ -4092,7 +4113,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C76" t="s">
         <v>105</v>
@@ -4100,7 +4121,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
         <v>105</v>
@@ -4108,7 +4129,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>645</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
         <v>105</v>
@@ -4116,34 +4137,34 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>108</v>
+        <v>645</v>
       </c>
       <c r="C79" t="s">
         <v>105</v>
       </c>
-      <c r="D79" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>108</v>
+      </c>
+      <c r="C80" t="s">
+        <v>105</v>
+      </c>
+      <c r="D80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>110</v>
-      </c>
-      <c r="C80" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="14" t="s">
-        <v>748</v>
       </c>
       <c r="C81" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>743</v>
+      <c r="B82" s="14" t="s">
+        <v>748</v>
       </c>
       <c r="C82" t="s">
         <v>111</v>
@@ -4151,7 +4172,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>112</v>
+        <v>743</v>
       </c>
       <c r="C83" t="s">
         <v>111</v>
@@ -4159,47 +4180,47 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C85" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>761</v>
+        <v>115</v>
       </c>
       <c r="C86" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>117</v>
+        <v>761</v>
       </c>
       <c r="C87" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="14" t="s">
-        <v>747</v>
+      <c r="B88" t="s">
+        <v>117</v>
       </c>
       <c r="C88" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>633</v>
+      <c r="B89" s="14" t="s">
+        <v>747</v>
       </c>
       <c r="C89" t="s">
         <v>118</v>
@@ -4207,7 +4228,7 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="C90" t="s">
         <v>118</v>
@@ -4215,7 +4236,7 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="C91" t="s">
         <v>118</v>
@@ -4223,31 +4244,31 @@
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C92" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>647</v>
+        <v>122</v>
       </c>
       <c r="C94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>124</v>
+        <v>647</v>
       </c>
       <c r="C95" t="s">
         <v>125</v>
@@ -4255,15 +4276,15 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>739</v>
+        <v>124</v>
       </c>
       <c r="C96" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>126</v>
+        <v>739</v>
       </c>
       <c r="C97" t="s">
         <v>127</v>
@@ -4271,23 +4292,23 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C98" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>728</v>
+        <v>128</v>
       </c>
       <c r="C99" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>130</v>
+        <v>728</v>
       </c>
       <c r="C100" t="s">
         <v>131</v>
@@ -4295,31 +4316,31 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C101" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C102" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>762</v>
+        <v>134</v>
       </c>
       <c r="C103" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>136</v>
+        <v>762</v>
       </c>
       <c r="C104" t="s">
         <v>137</v>
@@ -4327,31 +4348,31 @@
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C105" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
-        <v>139</v>
+      <c r="B106" t="s">
+        <v>138</v>
       </c>
       <c r="C106" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>622</v>
+      <c r="B107" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C107" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>140</v>
+        <v>622</v>
       </c>
       <c r="C108" t="s">
         <v>141</v>
@@ -4359,15 +4380,15 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>623</v>
+        <v>140</v>
       </c>
       <c r="C109" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>142</v>
+        <v>623</v>
       </c>
       <c r="C110" t="s">
         <v>143</v>
@@ -4375,23 +4396,23 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C111" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C112" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C113" t="s">
         <v>147</v>
@@ -4399,7 +4420,7 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C114" t="s">
         <v>147</v>
@@ -4407,23 +4428,23 @@
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>764</v>
+        <v>150</v>
       </c>
       <c r="C116" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>152</v>
+        <v>764</v>
       </c>
       <c r="C117" t="s">
         <v>153</v>
@@ -4431,23 +4452,23 @@
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>726</v>
+        <v>154</v>
       </c>
       <c r="C119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>156</v>
+        <v>726</v>
       </c>
       <c r="C120" t="s">
         <v>157</v>
@@ -4455,23 +4476,23 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
+        <v>156</v>
+      </c>
+      <c r="C121" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
         <v>754</v>
-      </c>
-      <c r="C121" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="12" t="s">
-        <v>648</v>
       </c>
       <c r="C122" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>719</v>
+      <c r="B123" s="12" t="s">
+        <v>648</v>
       </c>
       <c r="C123" t="s">
         <v>159</v>
@@ -4479,7 +4500,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>649</v>
+        <v>719</v>
       </c>
       <c r="C124" t="s">
         <v>159</v>
@@ -4487,7 +4508,7 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>158</v>
+        <v>649</v>
       </c>
       <c r="C125" t="s">
         <v>159</v>
@@ -4495,23 +4516,23 @@
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C126" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>624</v>
+        <v>160</v>
       </c>
       <c r="C127" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>162</v>
+        <v>624</v>
       </c>
       <c r="C128" t="s">
         <v>163</v>
@@ -4519,15 +4540,15 @@
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>629</v>
+        <v>162</v>
       </c>
       <c r="C129" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>164</v>
+        <v>629</v>
       </c>
       <c r="C130" t="s">
         <v>165</v>
@@ -4535,23 +4556,23 @@
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C131" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C132" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C133" t="s">
         <v>169</v>
@@ -4559,15 +4580,15 @@
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>650</v>
+        <v>170</v>
       </c>
       <c r="C134" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>171</v>
+        <v>650</v>
       </c>
       <c r="C135" t="s">
         <v>172</v>
@@ -4575,7 +4596,7 @@
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C136" t="s">
         <v>172</v>
@@ -4583,39 +4604,39 @@
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C137" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C138" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C139" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>765</v>
+        <v>178</v>
       </c>
       <c r="C140" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>180</v>
+        <v>765</v>
       </c>
       <c r="C141" t="s">
         <v>181</v>
@@ -4623,31 +4644,31 @@
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C142" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C143" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C144" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C145" t="s">
         <v>187</v>
@@ -4655,15 +4676,15 @@
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>773</v>
+        <v>188</v>
       </c>
       <c r="C146" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>189</v>
+        <v>773</v>
       </c>
       <c r="C147" t="s">
         <v>190</v>
@@ -4671,15 +4692,15 @@
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>651</v>
+        <v>189</v>
       </c>
       <c r="C148" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>191</v>
+        <v>651</v>
       </c>
       <c r="C149" t="s">
         <v>192</v>
@@ -4687,95 +4708,95 @@
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C150" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C151" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C152" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C153" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C154" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>652</v>
+        <v>201</v>
       </c>
       <c r="C155" t="s">
-        <v>653</v>
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>203</v>
+        <v>652</v>
       </c>
       <c r="C156" t="s">
-        <v>204</v>
+        <v>653</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C157" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C158" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C159" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>766</v>
+        <v>209</v>
       </c>
       <c r="C160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>211</v>
+        <v>766</v>
       </c>
       <c r="C161" t="s">
         <v>212</v>
@@ -4783,79 +4804,79 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
+        <v>211</v>
+      </c>
+      <c r="C162" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>213</v>
-      </c>
-      <c r="C162" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C163" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>216</v>
+      <c r="B164" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C164" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C165" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C166" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C167" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C168" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C169" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>740</v>
+        <v>226</v>
       </c>
       <c r="C170" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>716</v>
+        <v>740</v>
       </c>
       <c r="C171" t="s">
         <v>229</v>
@@ -4863,7 +4884,7 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>654</v>
+        <v>781</v>
       </c>
       <c r="C172" t="s">
         <v>229</v>
@@ -4871,7 +4892,7 @@
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>655</v>
+        <v>716</v>
       </c>
       <c r="C173" t="s">
         <v>229</v>
@@ -4879,7 +4900,7 @@
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C174" t="s">
         <v>229</v>
@@ -4887,7 +4908,7 @@
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C175" t="s">
         <v>229</v>
@@ -4895,7 +4916,7 @@
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>634</v>
+        <v>656</v>
       </c>
       <c r="C176" t="s">
         <v>229</v>
@@ -4903,7 +4924,7 @@
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>228</v>
+        <v>657</v>
       </c>
       <c r="C177" t="s">
         <v>229</v>
@@ -4911,7 +4932,7 @@
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>230</v>
+        <v>634</v>
       </c>
       <c r="C178" t="s">
         <v>229</v>
@@ -4919,7 +4940,7 @@
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C179" t="s">
         <v>229</v>
@@ -4927,79 +4948,79 @@
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>727</v>
+        <v>230</v>
       </c>
       <c r="C180" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C181" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>234</v>
+        <v>727</v>
       </c>
       <c r="C182" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B183" s="6" t="s">
-        <v>236</v>
+      <c r="B183" t="s">
+        <v>232</v>
       </c>
       <c r="C183" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C184" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C185" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>658</v>
-      </c>
-      <c r="C185" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C186" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>732</v>
-      </c>
-      <c r="C187" t="s">
-        <v>242</v>
+        <v>658</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>659</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="C188" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>241</v>
+        <v>784</v>
       </c>
       <c r="C189" t="s">
         <v>242</v>
@@ -5007,15 +5028,15 @@
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>660</v>
-      </c>
-      <c r="C190" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="C190" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>635</v>
+        <v>659</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>242</v>
@@ -5023,247 +5044,247 @@
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C192" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B193" s="11" t="s">
-        <v>661</v>
-      </c>
-      <c r="C193" t="s">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>660</v>
+      </c>
+      <c r="C193" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>244</v>
-      </c>
-      <c r="C194" t="s">
+        <v>635</v>
+      </c>
+      <c r="C194" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C195" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
-        <v>247</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B196" s="11" t="s">
+        <v>661</v>
       </c>
       <c r="C196" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="4" t="s">
-        <v>249</v>
+      <c r="B197" t="s">
+        <v>244</v>
       </c>
       <c r="C197" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C198" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C199" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>254</v>
+      <c r="B200" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C200" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C201" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C202" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C203" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C204" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C205" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C206" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C207" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C208" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C209" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>662</v>
+        <v>267</v>
       </c>
       <c r="C210" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="211" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B211" s="11" t="s">
-        <v>712</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>269</v>
       </c>
       <c r="C211" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>663</v>
+        <v>271</v>
       </c>
       <c r="C212" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="10" t="s">
-        <v>664</v>
+      <c r="B213" t="s">
+        <v>662</v>
       </c>
       <c r="C213" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="10" t="s">
-        <v>749</v>
+    <row r="214" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B214" s="11" t="s">
+        <v>712</v>
       </c>
       <c r="C214" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="10" t="s">
-        <v>770</v>
+    <row r="215" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B215" s="11" t="s">
+        <v>785</v>
       </c>
       <c r="C215" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B216" s="10" t="s">
-        <v>665</v>
+      <c r="B216" t="s">
+        <v>663</v>
       </c>
       <c r="C216" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>273</v>
+      <c r="B217" s="10" t="s">
+        <v>664</v>
       </c>
       <c r="C217" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
-        <v>731</v>
+      <c r="B218" s="10" t="s">
+        <v>749</v>
       </c>
       <c r="C218" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
-        <v>666</v>
+      <c r="B219" s="10" t="s">
+        <v>770</v>
       </c>
       <c r="C219" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
-        <v>717</v>
+      <c r="B220" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="C220" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B221" s="4" t="s">
-        <v>274</v>
+      <c r="B221" t="s">
+        <v>273</v>
       </c>
       <c r="C221" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>667</v>
+        <v>731</v>
       </c>
       <c r="C222" t="s">
         <v>275</v>
@@ -5271,7 +5292,7 @@
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>276</v>
+        <v>666</v>
       </c>
       <c r="C223" t="s">
         <v>275</v>
@@ -5279,23 +5300,23 @@
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>636</v>
+        <v>717</v>
       </c>
       <c r="C224" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B225" t="s">
-        <v>277</v>
+      <c r="B225" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C225" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>278</v>
+      <c r="B226" s="4" t="s">
+        <v>786</v>
       </c>
       <c r="C226" t="s">
         <v>275</v>
@@ -5303,7 +5324,7 @@
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C227" t="s">
         <v>275</v>
@@ -5311,7 +5332,7 @@
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>669</v>
+        <v>276</v>
       </c>
       <c r="C228" t="s">
         <v>275</v>
@@ -5319,79 +5340,79 @@
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>279</v>
+        <v>636</v>
       </c>
       <c r="C229" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C230" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" s="4" t="s">
-        <v>283</v>
+      <c r="B231" t="s">
+        <v>278</v>
       </c>
       <c r="C231" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>285</v>
+        <v>668</v>
       </c>
       <c r="C232" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>286</v>
+        <v>669</v>
       </c>
       <c r="C233" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>670</v>
+        <v>279</v>
       </c>
       <c r="C234" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B235" s="10" t="s">
-        <v>671</v>
+      <c r="B235" t="s">
+        <v>281</v>
       </c>
       <c r="C235" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B236" t="s">
-        <v>288</v>
+      <c r="B236" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="C236" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>734</v>
+        <v>285</v>
       </c>
       <c r="C237" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>672</v>
+        <v>286</v>
       </c>
       <c r="C238" t="s">
         <v>287</v>
@@ -5399,2162 +5420,2218 @@
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>289</v>
+        <v>670</v>
       </c>
       <c r="C239" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B240" t="s">
-        <v>625</v>
+      <c r="B240" s="10" t="s">
+        <v>671</v>
       </c>
       <c r="C240" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C241" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>626</v>
+        <v>734</v>
       </c>
       <c r="C242" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="243" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>292</v>
+        <v>672</v>
       </c>
       <c r="C243" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="244" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C244" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>296</v>
+        <v>625</v>
       </c>
       <c r="C245" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C246" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>300</v>
+        <v>626</v>
       </c>
       <c r="C247" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C248" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="249" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B249" s="11" t="s">
-        <v>713</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>294</v>
       </c>
       <c r="C249" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C250" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="251" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B251" s="4" t="s">
-        <v>306</v>
+      <c r="B251" t="s">
+        <v>298</v>
       </c>
       <c r="C251" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="252" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C252" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="253" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C253" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B254" t="s">
-        <v>630</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="254" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B254" s="11" t="s">
+        <v>713</v>
       </c>
       <c r="C254" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="255" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
+        <v>304</v>
+      </c>
+      <c r="C255" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B256" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C256" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>307</v>
+      </c>
+      <c r="C257" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>309</v>
+      </c>
+      <c r="C258" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>630</v>
+      </c>
+      <c r="C259" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
         <v>311</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C260" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
         <v>313</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C261" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="257" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B257" t="s">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
         <v>315</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C262" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="258" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B258" t="s">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
         <v>724</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C263" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B259" t="s">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
         <v>317</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C264" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
-        <v>753</v>
-      </c>
-      <c r="C260" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="261" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B261" t="s">
-        <v>741</v>
-      </c>
-      <c r="C261" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B262" t="s">
-        <v>673</v>
-      </c>
-      <c r="C262" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B263" t="s">
-        <v>674</v>
-      </c>
-      <c r="C263" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="264" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B264" t="s">
-        <v>319</v>
-      </c>
-      <c r="C264" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>675</v>
+        <v>782</v>
       </c>
       <c r="C265" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>321</v>
+        <v>753</v>
       </c>
       <c r="C266" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>322</v>
+        <v>741</v>
       </c>
       <c r="C267" t="s">
         <v>320</v>
       </c>
-      <c r="E267" s="4"/>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>323</v>
+        <v>673</v>
       </c>
       <c r="C268" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B269" s="4" t="s">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>674</v>
+      </c>
+      <c r="C269" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
+        <v>319</v>
+      </c>
+      <c r="C270" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B271" t="s">
+        <v>675</v>
+      </c>
+      <c r="C271" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>321</v>
+      </c>
+      <c r="C272" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>322</v>
+      </c>
+      <c r="C273" t="s">
+        <v>320</v>
+      </c>
+      <c r="E273" s="4"/>
+    </row>
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>323</v>
+      </c>
+      <c r="C274" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="275" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B275" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="C269" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B270" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C270" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B271" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="C271" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="272" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B272" s="11" t="s">
-        <v>677</v>
-      </c>
-      <c r="C272" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B273" t="s">
-        <v>678</v>
-      </c>
-      <c r="C273" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B274" t="s">
-        <v>326</v>
-      </c>
-      <c r="C274" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B275" t="s">
-        <v>327</v>
       </c>
       <c r="C275" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B276" t="s">
-        <v>328</v>
+    <row r="276" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B276" s="4" t="s">
+        <v>676</v>
       </c>
       <c r="C276" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B277" t="s">
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B277" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C277" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="278" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B278" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="C278" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="279" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B279" s="11" t="s">
+        <v>677</v>
+      </c>
+      <c r="C279" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="280" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>678</v>
+      </c>
+      <c r="C280" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="281" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>326</v>
+      </c>
+      <c r="C281" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>327</v>
+      </c>
+      <c r="C282" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>328</v>
+      </c>
+      <c r="C283" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="284" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
         <v>329</v>
       </c>
-      <c r="C277" t="s">
+      <c r="C284" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B278" t="s">
+    <row r="285" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
         <v>331</v>
       </c>
-      <c r="C278" t="s">
+      <c r="C285" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B279" t="s">
+    <row r="286" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
         <v>333</v>
       </c>
-      <c r="C279" t="s">
+      <c r="C286" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B280" t="s">
+    <row r="287" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
         <v>335</v>
       </c>
-      <c r="C280" t="s">
+      <c r="C287" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B281" t="s">
+    <row r="288" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
         <v>337</v>
       </c>
-      <c r="C281" t="s">
+      <c r="C288" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B282" t="s">
-        <v>339</v>
-      </c>
-      <c r="C282" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B283" t="s">
-        <v>767</v>
-      </c>
-      <c r="C283" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B284" t="s">
-        <v>341</v>
-      </c>
-      <c r="C284" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B285" t="s">
-        <v>343</v>
-      </c>
-      <c r="C285" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B286" t="s">
-        <v>345</v>
-      </c>
-      <c r="C286" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B287" t="s">
-        <v>347</v>
-      </c>
-      <c r="C287" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B288" t="s">
-        <v>349</v>
-      </c>
-      <c r="C288" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="289" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C289" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="290" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>353</v>
+        <v>767</v>
       </c>
       <c r="C290" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="291" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C291" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="292" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>720</v>
+        <v>343</v>
       </c>
       <c r="C292" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="293" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B293" s="10" t="s">
-        <v>679</v>
+      <c r="B293" t="s">
+        <v>345</v>
       </c>
       <c r="C293" t="s">
-        <v>354</v>
-      </c>
-      <c r="F293" s="4"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="294" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>627</v>
+        <v>347</v>
       </c>
       <c r="C294" t="s">
-        <v>357</v>
-      </c>
-      <c r="F294" s="4"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="295" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C295" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="296" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>628</v>
+        <v>351</v>
       </c>
       <c r="C296" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="297" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C297" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="298" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C298" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="299" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="C299" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="300" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B300" t="s">
-        <v>362</v>
+      <c r="B300" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="C300" t="s">
-        <v>363</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="F300" s="4"/>
     </row>
     <row r="301" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>681</v>
+        <v>627</v>
       </c>
       <c r="C301" t="s">
-        <v>363</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="F301" s="4"/>
     </row>
     <row r="302" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B302" s="4" t="s">
-        <v>364</v>
+      <c r="B302" t="s">
+        <v>356</v>
       </c>
       <c r="C302" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="303" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>365</v>
+        <v>628</v>
       </c>
       <c r="C303" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="304" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>768</v>
+        <v>358</v>
       </c>
       <c r="C304" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C305" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>369</v>
+        <v>680</v>
       </c>
       <c r="C306" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="C307" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>373</v>
+        <v>681</v>
       </c>
       <c r="C308" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B309" t="s">
-        <v>375</v>
+      <c r="B309" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C309" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="C310" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>379</v>
+        <v>768</v>
       </c>
       <c r="C311" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="C312" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="C313" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="13" t="s">
-        <v>746</v>
+      <c r="B314" t="s">
+        <v>371</v>
       </c>
       <c r="C314" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="C315" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>769</v>
+        <v>375</v>
       </c>
       <c r="C316" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C317" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B318" s="4" t="s">
-        <v>389</v>
+      <c r="B318" t="s">
+        <v>379</v>
       </c>
       <c r="C318" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C319" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C320" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B321" t="s">
-        <v>393</v>
+      <c r="B321" s="13" t="s">
+        <v>746</v>
       </c>
       <c r="C321" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C322" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>397</v>
+        <v>769</v>
       </c>
       <c r="C323" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="C324" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B325" t="s">
-        <v>401</v>
+      <c r="B325" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C325" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="C326" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="C327" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="C328" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="C329" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="C330" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="C331" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C332" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="C333" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="C334" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="C335" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="C336" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
     </row>
     <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C337" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="C338" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>682</v>
+        <v>413</v>
       </c>
       <c r="C339" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="C340" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>752</v>
+        <v>417</v>
       </c>
       <c r="C341" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>683</v>
+        <v>419</v>
       </c>
       <c r="C342" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C343" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B344" s="4" t="s">
-        <v>430</v>
+      <c r="B344" t="s">
+        <v>423</v>
       </c>
       <c r="C344" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="345" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>684</v>
+        <v>425</v>
       </c>
       <c r="C345" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="346" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>431</v>
+        <v>682</v>
       </c>
       <c r="C346" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="347" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>771</v>
+        <v>427</v>
       </c>
       <c r="C347" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="348" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>433</v>
+        <v>752</v>
       </c>
       <c r="C348" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="349" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>435</v>
+        <v>683</v>
       </c>
       <c r="C349" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="350" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="C350" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="351" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B351" t="s">
-        <v>439</v>
+      <c r="B351" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C351" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>441</v>
+        <v>684</v>
       </c>
       <c r="C352" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="353" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="C353" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="354" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>631</v>
+        <v>771</v>
       </c>
       <c r="C354" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
     </row>
     <row r="355" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="C355" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
     </row>
     <row r="356" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C356" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="357" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="C357" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
     <row r="358" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="C358" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
     </row>
     <row r="359" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="C359" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
     </row>
     <row r="360" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="C360" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="361" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>456</v>
+        <v>631</v>
       </c>
       <c r="C361" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
     </row>
     <row r="362" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>780</v>
+        <v>445</v>
       </c>
       <c r="C362" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="363" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="C363" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row r="364" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="C364" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
     </row>
     <row r="365" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>685</v>
+        <v>451</v>
       </c>
       <c r="C365" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
     </row>
     <row r="366" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>632</v>
+        <v>453</v>
       </c>
       <c r="C366" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="367" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="C367" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="368" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
+        <v>456</v>
+      </c>
+      <c r="C368" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
+        <v>780</v>
+      </c>
+      <c r="C369" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
+        <v>458</v>
+      </c>
+      <c r="C370" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>460</v>
+      </c>
+      <c r="C371" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
+        <v>685</v>
+      </c>
+      <c r="C372" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
+        <v>632</v>
+      </c>
+      <c r="C373" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B374" t="s">
+        <v>462</v>
+      </c>
+      <c r="C374" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B375" t="s">
         <v>464</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C375" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="369" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B369" t="s">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B376" t="s">
         <v>774</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C376" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="370" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B370" t="s">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B377" t="s">
         <v>465</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C377" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="371" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B371" t="s">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B378" t="s">
         <v>466</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C378" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="372" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B372" t="s">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B379" t="s">
         <v>468</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C379" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="373" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B373" t="s">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B380" t="s">
         <v>775</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C380" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="374" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B374" s="11" t="s">
+    <row r="381" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B381" s="11" t="s">
         <v>730</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C381" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="375" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B375" s="11" t="s">
+    <row r="382" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B382" s="11" t="s">
         <v>714</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C382" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="376" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B376" t="s">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B383" t="s">
         <v>470</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C383" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="377" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B377" s="4" t="s">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B384" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="C377" t="s">
+      <c r="C384" t="s">
         <v>471</v>
-      </c>
-    </row>
-    <row r="378" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B378" t="s">
-        <v>473</v>
-      </c>
-      <c r="C378" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="379" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B379" t="s">
-        <v>475</v>
-      </c>
-      <c r="C379" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="380" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B380" t="s">
-        <v>477</v>
-      </c>
-      <c r="C380" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="381" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B381" t="s">
-        <v>479</v>
-      </c>
-      <c r="C381" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="382" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B382" t="s">
-        <v>481</v>
-      </c>
-      <c r="C382" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="383" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B383" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="C383" t="s">
-        <v>483</v>
-      </c>
-      <c r="E383" s="4"/>
-    </row>
-    <row r="384" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B384" t="s">
-        <v>484</v>
-      </c>
-      <c r="C384" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="385" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="C385" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
     </row>
     <row r="386" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="C386" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
     </row>
     <row r="387" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="C387" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
     </row>
     <row r="388" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="C388" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
     </row>
     <row r="389" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="C389" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
     </row>
     <row r="390" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B390" t="s">
-        <v>495</v>
+      <c r="B390" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C390" t="s">
-        <v>496</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E390" s="4"/>
     </row>
     <row r="391" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="C391" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
     </row>
     <row r="392" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="C392" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
     </row>
     <row r="393" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="C393" t="s">
-        <v>502</v>
-      </c>
-      <c r="E393" s="4"/>
+        <v>488</v>
+      </c>
     </row>
     <row r="394" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>686</v>
+        <v>489</v>
       </c>
       <c r="C394" t="s">
-        <v>19</v>
-      </c>
-      <c r="E394" s="4"/>
+        <v>490</v>
+      </c>
     </row>
     <row r="395" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="C395" t="s">
-        <v>19</v>
+        <v>492</v>
       </c>
     </row>
     <row r="396" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>776</v>
+        <v>493</v>
       </c>
       <c r="C396" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="397" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>687</v>
+        <v>495</v>
       </c>
       <c r="C397" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="398" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="C398" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="399" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C399" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="400" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
+        <v>501</v>
+      </c>
+      <c r="C400" t="s">
+        <v>502</v>
+      </c>
+      <c r="E400" s="4"/>
+    </row>
+    <row r="401" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B401" t="s">
+        <v>686</v>
+      </c>
+      <c r="C401" t="s">
+        <v>19</v>
+      </c>
+      <c r="E401" s="4"/>
+    </row>
+    <row r="402" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B402" t="s">
+        <v>503</v>
+      </c>
+      <c r="C402" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="403" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B403" t="s">
+        <v>776</v>
+      </c>
+      <c r="C403" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="404" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B404" t="s">
+        <v>687</v>
+      </c>
+      <c r="C404" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="405" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B405" t="s">
+        <v>504</v>
+      </c>
+      <c r="C405" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="406" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B406" t="s">
+        <v>506</v>
+      </c>
+      <c r="C406" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="407" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B407" t="s">
         <v>777</v>
       </c>
-      <c r="C400" t="s">
+      <c r="C407" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B401" t="s">
+    <row r="408" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B408" t="s">
         <v>688</v>
       </c>
-      <c r="C401" t="s">
+      <c r="C408" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B402" t="s">
+    <row r="409" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B409" t="s">
         <v>507</v>
       </c>
-      <c r="C402" t="s">
+      <c r="C409" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B403" t="s">
+    <row r="410" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B410" t="s">
         <v>509</v>
       </c>
-      <c r="C403" t="s">
+      <c r="C410" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B404" t="s">
+    <row r="411" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B411" t="s">
         <v>689</v>
       </c>
-      <c r="C404" t="s">
+      <c r="C411" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B405" t="s">
+    <row r="412" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B412" t="s">
         <v>511</v>
       </c>
-      <c r="C405" t="s">
+      <c r="C412" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B406" t="s">
+    <row r="413" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B413" t="s">
         <v>513</v>
       </c>
-      <c r="C406" t="s">
+      <c r="C413" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B407" t="s">
+    <row r="414" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B414" t="s">
         <v>514</v>
       </c>
-      <c r="C407" t="s">
+      <c r="C414" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B408" t="s">
+    <row r="415" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B415" t="s">
         <v>690</v>
       </c>
-      <c r="C408" t="s">
+      <c r="C415" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B409" t="s">
+    <row r="416" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B416" t="s">
         <v>516</v>
       </c>
-      <c r="C409" t="s">
+      <c r="C416" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B410" t="s">
+    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B417" t="s">
         <v>517</v>
       </c>
-      <c r="C410" t="s">
+      <c r="C417" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B411" t="s">
+    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B418" t="s">
         <v>519</v>
       </c>
-      <c r="C411" t="s">
+      <c r="C418" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B412" t="s">
+    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B419" t="s">
         <v>721</v>
       </c>
-      <c r="C412" t="s">
+      <c r="C419" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B413" t="s">
+    <row r="420" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B420" t="s">
         <v>691</v>
       </c>
-      <c r="C413" t="s">
+      <c r="C420" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B414" t="s">
+    <row r="421" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B421" t="s">
         <v>692</v>
       </c>
-      <c r="C414" t="s">
+      <c r="C421" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B415" t="s">
+    <row r="422" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B422" t="s">
         <v>521</v>
       </c>
-      <c r="C415" t="s">
+      <c r="C422" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B416" t="s">
+    <row r="423" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B423" t="s">
         <v>778</v>
       </c>
-      <c r="C416" t="s">
+      <c r="C423" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="417" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B417" t="s">
+    <row r="424" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B424" t="s">
         <v>523</v>
       </c>
-      <c r="C417" t="s">
+      <c r="C424" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="418" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B418" t="s">
+    <row r="425" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B425" t="s">
         <v>525</v>
       </c>
-      <c r="C418" t="s">
+      <c r="C425" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="419" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B419" t="s">
+    <row r="426" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B426" t="s">
         <v>527</v>
       </c>
-      <c r="C419" t="s">
+      <c r="C426" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="420" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B420" t="s">
+    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B427" t="s">
         <v>529</v>
       </c>
-      <c r="C420" t="s">
+      <c r="C427" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="421" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B421" t="s">
+    <row r="428" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B428" t="s">
         <v>531</v>
       </c>
-      <c r="C421" t="s">
+      <c r="C428" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="422" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B422" t="s">
+    <row r="429" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B429" t="s">
         <v>533</v>
       </c>
-      <c r="C422" t="s">
+      <c r="C429" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="423" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B423" t="s">
+    <row r="430" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B430" t="s">
         <v>693</v>
-      </c>
-      <c r="C423" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="424" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B424" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="C424" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="425" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B425" t="s">
-        <v>744</v>
-      </c>
-      <c r="C425" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="426" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B426" t="s">
-        <v>735</v>
-      </c>
-      <c r="C426" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="427" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B427" t="s">
-        <v>534</v>
-      </c>
-      <c r="C427" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="428" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B428" t="s">
-        <v>536</v>
-      </c>
-      <c r="C428" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="429" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B429" t="s">
-        <v>537</v>
-      </c>
-      <c r="C429" t="s">
-        <v>535</v>
-      </c>
-      <c r="D429" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="430" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B430" t="s">
-        <v>538</v>
       </c>
       <c r="C430" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="431" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B431" t="s">
+    <row r="431" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B431" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="C431" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B432" t="s">
+        <v>744</v>
+      </c>
+      <c r="C432" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="433" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B433" t="s">
+        <v>735</v>
+      </c>
+      <c r="C433" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="434" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B434" t="s">
+        <v>534</v>
+      </c>
+      <c r="C434" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="435" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B435" t="s">
+        <v>536</v>
+      </c>
+      <c r="C435" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="436" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B436" t="s">
+        <v>537</v>
+      </c>
+      <c r="C436" t="s">
+        <v>535</v>
+      </c>
+      <c r="D436" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="437" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B437" t="s">
+        <v>538</v>
+      </c>
+      <c r="C437" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="438" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B438" t="s">
         <v>539</v>
       </c>
-      <c r="C431" t="s">
+      <c r="C438" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="432" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B432" t="s">
+    <row r="439" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B439" t="s">
         <v>722</v>
       </c>
-      <c r="C432" t="s">
+      <c r="C439" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B433" s="10" t="s">
+    <row r="440" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B440" s="10" t="s">
         <v>694</v>
       </c>
-      <c r="C433" t="s">
+      <c r="C440" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B434" t="s">
+    <row r="441" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B441" t="s">
         <v>541</v>
       </c>
-      <c r="C434" t="s">
+      <c r="C441" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B435" t="s">
+    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B442" t="s">
         <v>723</v>
       </c>
-      <c r="C435" t="s">
+      <c r="C442" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="436" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B436" s="11" t="s">
+    <row r="443" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B443" s="11" t="s">
         <v>696</v>
       </c>
-      <c r="C436" t="s">
+      <c r="C443" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B437" t="s">
+    <row r="444" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B444" t="s">
         <v>697</v>
       </c>
-      <c r="C437" t="s">
+      <c r="C444" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B438" s="1" t="s">
+    <row r="445" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B445" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C438" s="1" t="s">
+      <c r="C445" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B439" s="10" t="s">
+    <row r="446" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B446" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="C439" t="s">
+      <c r="C446" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B440" s="4" t="s">
+    <row r="447" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B447" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C440" t="s">
+      <c r="C447" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B441" t="s">
+    <row r="448" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B448" t="s">
         <v>544</v>
       </c>
-      <c r="C441" t="s">
+      <c r="C448" t="s">
         <v>545</v>
-      </c>
-    </row>
-    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B442" t="s">
-        <v>700</v>
-      </c>
-      <c r="C442" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B443" t="s">
-        <v>546</v>
-      </c>
-      <c r="C443" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B444" t="s">
-        <v>548</v>
-      </c>
-      <c r="C444" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B445" t="s">
-        <v>550</v>
-      </c>
-      <c r="C445" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B446" t="s">
-        <v>552</v>
-      </c>
-      <c r="C446" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B447" t="s">
-        <v>718</v>
-      </c>
-      <c r="C447" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B448" t="s">
-        <v>756</v>
-      </c>
-      <c r="C448" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>554</v>
+        <v>700</v>
       </c>
       <c r="C449" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="C450" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="C451" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="C452" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="C453" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>751</v>
+        <v>718</v>
       </c>
       <c r="C454" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>563</v>
+        <v>756</v>
       </c>
       <c r="C455" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B456" s="4" t="s">
-        <v>565</v>
+      <c r="B456" t="s">
+        <v>554</v>
       </c>
       <c r="C456" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="C457" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="C458" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="C459" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="C460" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>738</v>
+        <v>751</v>
       </c>
       <c r="C461" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>779</v>
+        <v>563</v>
       </c>
       <c r="C462" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B463" t="s">
-        <v>737</v>
+      <c r="B463" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C463" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C464" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>701</v>
+        <v>567</v>
       </c>
       <c r="C465" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>763</v>
+        <v>569</v>
       </c>
       <c r="C466" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C467" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
-        <v>578</v>
+        <v>738</v>
       </c>
       <c r="C468" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>577</v>
+        <v>779</v>
       </c>
       <c r="C469" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="470" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B470" s="4" t="s">
-        <v>579</v>
+      <c r="B470" t="s">
+        <v>737</v>
       </c>
       <c r="C470" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="471" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="C471" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="472" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>582</v>
+        <v>701</v>
       </c>
       <c r="C472" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="473" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>584</v>
+        <v>763</v>
       </c>
       <c r="C473" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
     </row>
     <row r="474" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>702</v>
+        <v>575</v>
       </c>
       <c r="C474" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>703</v>
+        <v>578</v>
       </c>
       <c r="C475" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="476" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B476" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="C476" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="477" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B477" t="s">
-        <v>588</v>
+      <c r="B477" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C477" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="478" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="C478" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
     </row>
     <row r="479" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B479" s="4" t="s">
-        <v>591</v>
+      <c r="B479" t="s">
+        <v>582</v>
       </c>
       <c r="C479" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
     </row>
     <row r="480" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="C480" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="481" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
-        <v>594</v>
+        <v>702</v>
       </c>
       <c r="C481" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="482" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
-        <v>595</v>
+        <v>703</v>
       </c>
       <c r="C482" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="483" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B483" s="11" t="s">
-        <v>704</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B483" t="s">
+        <v>586</v>
       </c>
       <c r="C483" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="484" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B484" s="10" t="s">
-        <v>705</v>
+      <c r="B484" t="s">
+        <v>588</v>
       </c>
       <c r="C484" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="485" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C485" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B486" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C486" t="s">
         <v>592</v>
-      </c>
-    </row>
-    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B486" t="s">
-        <v>597</v>
-      </c>
-      <c r="C486" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="487" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C487" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="488" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B488" t="s">
-        <v>736</v>
+        <v>594</v>
       </c>
       <c r="C488" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="489" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B489" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="C489" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B490" t="s">
-        <v>602</v>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="490" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B490" s="11" t="s">
+        <v>704</v>
       </c>
       <c r="C490" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="491" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B491" t="s">
-        <v>706</v>
+      <c r="B491" s="10" t="s">
+        <v>705</v>
       </c>
       <c r="C491" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="492" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="C492" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="493" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C493" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="494" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B494" s="4" t="s">
-        <v>606</v>
+      <c r="B494" t="s">
+        <v>599</v>
       </c>
       <c r="C494" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="495" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B495" s="4" t="s">
-        <v>707</v>
+      <c r="B495" t="s">
+        <v>736</v>
       </c>
       <c r="C495" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="496" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
-        <v>708</v>
+        <v>600</v>
       </c>
       <c r="C496" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="C497" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="498" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="C498" t="s">
-        <v>711</v>
+        <v>604</v>
       </c>
     </row>
     <row r="499" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C499" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="500" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="C500" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="501" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B501" t="s">
-        <v>613</v>
+      <c r="B501" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C501" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
     </row>
     <row r="502" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B502" t="s">
-        <v>709</v>
+      <c r="B502" s="4" t="s">
+        <v>707</v>
       </c>
       <c r="C502" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="503" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B503" s="4" t="s">
-        <v>615</v>
+      <c r="B503" t="s">
+        <v>708</v>
       </c>
       <c r="C503" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="504" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="C504" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="505" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
-        <v>617</v>
+        <v>710</v>
       </c>
       <c r="C505" t="s">
-        <v>614</v>
+        <v>711</v>
       </c>
     </row>
     <row r="506" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="C506" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
     </row>
     <row r="507" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
+        <v>611</v>
+      </c>
+      <c r="C507" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="508" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B508" t="s">
+        <v>613</v>
+      </c>
+      <c r="C508" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="509" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B509" t="s">
+        <v>709</v>
+      </c>
+      <c r="C509" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="510" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B510" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C510" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="511" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B511" t="s">
+        <v>616</v>
+      </c>
+      <c r="C511" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="512" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B512" t="s">
+        <v>617</v>
+      </c>
+      <c r="C512" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="513" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B513" t="s">
+        <v>618</v>
+      </c>
+      <c r="C513" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B514" t="s">
         <v>620</v>
       </c>
-      <c r="C507" t="s">
+      <c r="C514" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
second version of merging after removing duplicate rows
</commit_message>
<xml_diff>
--- a/data/Country List with ISO3.xlsx
+++ b/data/Country List with ISO3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="787">
   <si>
     <t>Country Name</t>
   </si>
@@ -2051,9 +2051,6 @@
   </si>
   <si>
     <t>TFYR of Macedonia</t>
-  </si>
-  <si>
-    <t>Micronesia (Federated States of)</t>
   </si>
   <si>
     <t>Republic of Moldova</t>
@@ -3502,10 +3499,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F514"/>
+  <dimension ref="A1:F513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A490" workbookViewId="0">
-      <selection activeCell="B514" sqref="B514"/>
+    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
+      <selection activeCell="B513" sqref="B513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3582,7 +3579,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -3609,7 +3606,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -3745,7 +3742,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
@@ -3817,7 +3814,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C39" t="s">
         <v>62</v>
@@ -3825,7 +3822,7 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C40" t="s">
         <v>62</v>
@@ -3953,7 +3950,7 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C56" t="s">
         <v>88</v>
@@ -4001,7 +3998,7 @@
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C62" t="s">
         <v>97</v>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C63" t="s">
         <v>97</v>
@@ -4065,7 +4062,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C70" t="s">
         <v>105</v>
@@ -4073,7 +4070,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C71" t="s">
         <v>105</v>
@@ -4097,7 +4094,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C74" t="s">
         <v>105</v>
@@ -4164,7 +4161,7 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C82" t="s">
         <v>111</v>
@@ -4172,7 +4169,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C83" t="s">
         <v>111</v>
@@ -4204,7 +4201,7 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C87" t="s">
         <v>118</v>
@@ -4220,7 +4217,7 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C89" t="s">
         <v>118</v>
@@ -4284,7 +4281,7 @@
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C97" t="s">
         <v>127</v>
@@ -4308,7 +4305,7 @@
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C100" t="s">
         <v>131</v>
@@ -4340,7 +4337,7 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C104" t="s">
         <v>137</v>
@@ -4444,7 +4441,7 @@
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C117" t="s">
         <v>153</v>
@@ -4468,7 +4465,7 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C120" t="s">
         <v>157</v>
@@ -4484,7 +4481,7 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C122" t="s">
         <v>159</v>
@@ -4500,7 +4497,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C124" t="s">
         <v>159</v>
@@ -4636,7 +4633,7 @@
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C141" t="s">
         <v>181</v>
@@ -4684,7 +4681,7 @@
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C147" t="s">
         <v>190</v>
@@ -4796,7 +4793,7 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C161" t="s">
         <v>212</v>
@@ -4876,7 +4873,7 @@
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C171" t="s">
         <v>229</v>
@@ -4884,7 +4881,7 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C172" t="s">
         <v>229</v>
@@ -4892,7 +4889,7 @@
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C173" t="s">
         <v>229</v>
@@ -4964,7 +4961,7 @@
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C182" t="s">
         <v>233</v>
@@ -5020,7 +5017,7 @@
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C189" t="s">
         <v>242</v>
@@ -5028,7 +5025,7 @@
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C190" t="s">
         <v>242</v>
@@ -5220,7 +5217,7 @@
     </row>
     <row r="214" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B214" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C214" t="s">
         <v>272</v>
@@ -5228,7 +5225,7 @@
     </row>
     <row r="215" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B215" s="11" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C215" t="s">
         <v>272</v>
@@ -5252,7 +5249,7 @@
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" s="10" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C218" t="s">
         <v>272</v>
@@ -5260,7 +5257,7 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="10" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C219" t="s">
         <v>272</v>
@@ -5284,7 +5281,7 @@
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C222" t="s">
         <v>275</v>
@@ -5300,7 +5297,7 @@
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C224" t="s">
         <v>275</v>
@@ -5316,7 +5313,7 @@
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C226" t="s">
         <v>275</v>
@@ -5444,7 +5441,7 @@
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C242" t="s">
         <v>287</v>
@@ -5540,7 +5537,7 @@
     </row>
     <row r="254" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B254" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C254" t="s">
         <v>305</v>
@@ -5612,7 +5609,7 @@
     </row>
     <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C263" t="s">
         <v>318</v>
@@ -5628,7 +5625,7 @@
     </row>
     <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C265" t="s">
         <v>320</v>
@@ -5636,7 +5633,7 @@
     </row>
     <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C266" t="s">
         <v>320</v>
@@ -5644,7 +5641,7 @@
     </row>
     <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C267" t="s">
         <v>320</v>
@@ -5725,7 +5722,7 @@
     </row>
     <row r="277" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B277" s="4" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C277" t="s">
         <v>325</v>
@@ -5733,7 +5730,7 @@
     </row>
     <row r="278" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B278" s="4" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C278" t="s">
         <v>325</v>
@@ -5829,7 +5826,7 @@
     </row>
     <row r="290" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C290" t="s">
         <v>342</v>
@@ -5901,41 +5898,40 @@
     </row>
     <row r="299" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C299" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="300" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B300" s="10" t="s">
-        <v>679</v>
+      <c r="B300" t="s">
+        <v>627</v>
       </c>
       <c r="C300" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F300" s="4"/>
     </row>
     <row r="301" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>627</v>
+        <v>356</v>
       </c>
       <c r="C301" t="s">
         <v>357</v>
       </c>
-      <c r="F301" s="4"/>
     </row>
     <row r="302" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>356</v>
+        <v>628</v>
       </c>
       <c r="C302" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="303" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>628</v>
+        <v>358</v>
       </c>
       <c r="C303" t="s">
         <v>359</v>
@@ -5943,23 +5939,23 @@
     </row>
     <row r="304" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C304" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>360</v>
+        <v>679</v>
       </c>
       <c r="C305" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>680</v>
+        <v>362</v>
       </c>
       <c r="C306" t="s">
         <v>363</v>
@@ -5967,39 +5963,39 @@
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>362</v>
+        <v>680</v>
       </c>
       <c r="C307" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B308" t="s">
-        <v>681</v>
+      <c r="B308" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="C308" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B309" s="4" t="s">
-        <v>364</v>
+      <c r="B309" t="s">
+        <v>365</v>
       </c>
       <c r="C309" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>365</v>
+        <v>767</v>
       </c>
       <c r="C310" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>768</v>
+        <v>367</v>
       </c>
       <c r="C311" t="s">
         <v>368</v>
@@ -6007,111 +6003,111 @@
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C312" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C313" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C314" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C315" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C316" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C317" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C318" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C319" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B320" t="s">
-        <v>383</v>
+      <c r="B320" s="13" t="s">
+        <v>745</v>
       </c>
       <c r="C320" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B321" s="13" t="s">
-        <v>746</v>
+      <c r="B321" t="s">
+        <v>385</v>
       </c>
       <c r="C321" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>385</v>
+        <v>768</v>
       </c>
       <c r="C322" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>769</v>
+        <v>387</v>
       </c>
       <c r="C323" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B324" t="s">
-        <v>387</v>
+      <c r="B324" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C324" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B325" s="4" t="s">
-        <v>389</v>
+      <c r="B325" t="s">
+        <v>390</v>
       </c>
       <c r="C325" t="s">
         <v>388</v>
@@ -6119,63 +6115,63 @@
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C326" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C327" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C328" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C329" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C330" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C331" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C332" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C333" t="s">
         <v>404</v>
@@ -6183,23 +6179,23 @@
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C334" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C335" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C336" t="s">
         <v>409</v>
@@ -6207,79 +6203,79 @@
     </row>
     <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C337" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C338" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C339" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C340" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C341" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C342" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C343" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C344" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="345" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>425</v>
+        <v>681</v>
       </c>
       <c r="C345" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="346" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>682</v>
+        <v>427</v>
       </c>
       <c r="C346" t="s">
         <v>428</v>
@@ -6287,7 +6283,7 @@
     </row>
     <row r="347" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>427</v>
+        <v>751</v>
       </c>
       <c r="C347" t="s">
         <v>428</v>
@@ -6295,7 +6291,7 @@
     </row>
     <row r="348" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>752</v>
+        <v>682</v>
       </c>
       <c r="C348" t="s">
         <v>428</v>
@@ -6303,31 +6299,31 @@
     </row>
     <row r="349" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>683</v>
+        <v>429</v>
       </c>
       <c r="C349" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="350" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B350" t="s">
-        <v>429</v>
+      <c r="B350" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="C350" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="351" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B351" s="4" t="s">
-        <v>430</v>
+      <c r="B351" t="s">
+        <v>683</v>
       </c>
       <c r="C351" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>684</v>
+        <v>431</v>
       </c>
       <c r="C352" t="s">
         <v>432</v>
@@ -6335,15 +6331,15 @@
     </row>
     <row r="353" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>431</v>
+        <v>770</v>
       </c>
       <c r="C353" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="354" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>771</v>
+        <v>433</v>
       </c>
       <c r="C354" t="s">
         <v>434</v>
@@ -6351,55 +6347,55 @@
     </row>
     <row r="355" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C355" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="356" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C356" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="357" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C357" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="358" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C358" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="359" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C359" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="360" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>443</v>
+        <v>631</v>
       </c>
       <c r="C360" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="361" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>631</v>
+        <v>445</v>
       </c>
       <c r="C361" t="s">
         <v>446</v>
@@ -6407,39 +6403,39 @@
     </row>
     <row r="362" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C362" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="363" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C363" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="364" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C364" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="365" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C365" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="366" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C366" t="s">
         <v>454</v>
@@ -6447,23 +6443,23 @@
     </row>
     <row r="367" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C367" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="368" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>456</v>
+        <v>779</v>
       </c>
       <c r="C368" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>780</v>
+        <v>458</v>
       </c>
       <c r="C369" t="s">
         <v>459</v>
@@ -6471,23 +6467,23 @@
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C370" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>460</v>
+        <v>684</v>
       </c>
       <c r="C371" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>685</v>
+        <v>632</v>
       </c>
       <c r="C372" t="s">
         <v>463</v>
@@ -6495,7 +6491,7 @@
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>632</v>
+        <v>462</v>
       </c>
       <c r="C373" t="s">
         <v>463</v>
@@ -6503,7 +6499,7 @@
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C374" t="s">
         <v>463</v>
@@ -6511,7 +6507,7 @@
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>464</v>
+        <v>773</v>
       </c>
       <c r="C375" t="s">
         <v>463</v>
@@ -6519,7 +6515,7 @@
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>774</v>
+        <v>465</v>
       </c>
       <c r="C376" t="s">
         <v>463</v>
@@ -6527,31 +6523,31 @@
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C377" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C378" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>468</v>
+        <v>774</v>
       </c>
       <c r="C379" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B380" t="s">
-        <v>775</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="380" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B380" s="11" t="s">
+        <v>729</v>
       </c>
       <c r="C380" t="s">
         <v>471</v>
@@ -6559,314 +6555,314 @@
     </row>
     <row r="381" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B381" s="11" t="s">
-        <v>730</v>
+        <v>713</v>
       </c>
       <c r="C381" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="382" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B382" s="11" t="s">
-        <v>714</v>
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B382" t="s">
+        <v>470</v>
       </c>
       <c r="C382" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B383" t="s">
-        <v>470</v>
+      <c r="B383" s="4" t="s">
+        <v>472</v>
       </c>
       <c r="C383" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B384" s="4" t="s">
-        <v>472</v>
+      <c r="B384" t="s">
+        <v>473</v>
       </c>
       <c r="C384" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="385" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C385" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="386" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C386" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="387" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C387" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="388" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C388" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="389" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B389" t="s">
-        <v>481</v>
+      <c r="B389" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="C389" t="s">
-        <v>480</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E389" s="4"/>
     </row>
     <row r="390" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B390" s="4" t="s">
-        <v>482</v>
+      <c r="B390" t="s">
+        <v>484</v>
       </c>
       <c r="C390" t="s">
         <v>483</v>
       </c>
-      <c r="E390" s="4"/>
     </row>
     <row r="391" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C391" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="392" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C392" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="393" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C393" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="394" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C394" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="395" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C395" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="396" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C396" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="397" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C397" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="398" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C398" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="399" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C399" t="s">
-        <v>500</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E399" s="4"/>
     </row>
     <row r="400" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>501</v>
+        <v>685</v>
       </c>
       <c r="C400" t="s">
-        <v>502</v>
+        <v>19</v>
       </c>
       <c r="E400" s="4"/>
     </row>
-    <row r="401" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>686</v>
+        <v>503</v>
       </c>
       <c r="C401" t="s">
         <v>19</v>
       </c>
-      <c r="E401" s="4"/>
-    </row>
-    <row r="402" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>503</v>
+        <v>775</v>
       </c>
       <c r="C402" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="403" spans="2:5" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>776</v>
+        <v>686</v>
       </c>
       <c r="C403" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="404" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>687</v>
+        <v>504</v>
       </c>
       <c r="C404" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="405" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C405" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="406" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>506</v>
+        <v>776</v>
       </c>
       <c r="C406" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="407" spans="2:5" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>777</v>
+        <v>687</v>
       </c>
       <c r="C407" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="408" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>688</v>
+        <v>507</v>
       </c>
       <c r="C408" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="409" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C409" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="410" spans="2:5" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>509</v>
+        <v>688</v>
       </c>
       <c r="C410" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="411" spans="2:5" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>689</v>
+        <v>511</v>
       </c>
       <c r="C411" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="412" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C412" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="413" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C413" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="414" spans="2:5" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>514</v>
+        <v>689</v>
       </c>
       <c r="C414" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="415" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>690</v>
+        <v>516</v>
       </c>
       <c r="C415" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="416" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C416" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C417" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>519</v>
+        <v>720</v>
       </c>
       <c r="C418" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>721</v>
+        <v>690</v>
       </c>
       <c r="C419" t="s">
         <v>522</v>
@@ -6882,7 +6878,7 @@
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>692</v>
+        <v>521</v>
       </c>
       <c r="C421" t="s">
         <v>522</v>
@@ -6890,15 +6886,15 @@
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>521</v>
+        <v>777</v>
       </c>
       <c r="C422" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>778</v>
+        <v>523</v>
       </c>
       <c r="C423" t="s">
         <v>524</v>
@@ -6906,39 +6902,39 @@
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C424" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C425" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C426" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C427" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C428" t="s">
         <v>532</v>
@@ -6946,23 +6942,23 @@
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>533</v>
+        <v>692</v>
       </c>
       <c r="C429" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B430" t="s">
-        <v>693</v>
+      <c r="B430" s="13" t="s">
+        <v>744</v>
       </c>
       <c r="C430" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B431" s="13" t="s">
-        <v>745</v>
+      <c r="B431" t="s">
+        <v>743</v>
       </c>
       <c r="C431" t="s">
         <v>535</v>
@@ -6970,7 +6966,7 @@
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="C432" t="s">
         <v>535</v>
@@ -6978,7 +6974,7 @@
     </row>
     <row r="433" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>735</v>
+        <v>534</v>
       </c>
       <c r="C433" t="s">
         <v>535</v>
@@ -6986,7 +6982,7 @@
     </row>
     <row r="434" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C434" t="s">
         <v>535</v>
@@ -6994,73 +6990,73 @@
     </row>
     <row r="435" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C435" t="s">
         <v>535</v>
       </c>
+      <c r="D435" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="436" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C436" t="s">
         <v>535</v>
       </c>
-      <c r="D436" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="437" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C437" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="438" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>539</v>
+        <v>721</v>
       </c>
       <c r="C438" t="s">
-        <v>540</v>
+        <v>694</v>
       </c>
     </row>
     <row r="439" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B439" t="s">
-        <v>722</v>
+      <c r="B439" s="10" t="s">
+        <v>693</v>
       </c>
       <c r="C439" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="440" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B440" s="10" t="s">
-        <v>694</v>
+      <c r="B440" t="s">
+        <v>541</v>
       </c>
       <c r="C440" t="s">
-        <v>695</v>
+        <v>542</v>
       </c>
     </row>
     <row r="441" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>541</v>
+        <v>722</v>
       </c>
       <c r="C441" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B442" t="s">
-        <v>723</v>
+    <row r="442" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B442" s="11" t="s">
+        <v>695</v>
       </c>
       <c r="C442" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="443" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B443" s="11" t="s">
+    <row r="443" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B443" t="s">
         <v>696</v>
       </c>
       <c r="C443" t="s">
@@ -7068,48 +7064,48 @@
       </c>
     </row>
     <row r="444" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B444" t="s">
+      <c r="B444" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="C444" t="s">
+      <c r="C444" s="1" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="445" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B445" s="1" t="s">
+      <c r="B445" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="C445" s="1" t="s">
+      <c r="C445" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="446" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B446" s="10" t="s">
-        <v>699</v>
+      <c r="B446" s="4" t="s">
+        <v>543</v>
       </c>
       <c r="C446" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="447" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B447" s="4" t="s">
-        <v>543</v>
+      <c r="B447" t="s">
+        <v>544</v>
       </c>
       <c r="C447" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="448" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>544</v>
+        <v>699</v>
       </c>
       <c r="C448" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>700</v>
+        <v>546</v>
       </c>
       <c r="C449" t="s">
         <v>547</v>
@@ -7117,31 +7113,31 @@
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C450" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C451" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C452" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>552</v>
+        <v>717</v>
       </c>
       <c r="C453" t="s">
         <v>553</v>
@@ -7149,15 +7145,15 @@
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>718</v>
+        <v>755</v>
       </c>
       <c r="C454" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>756</v>
+        <v>554</v>
       </c>
       <c r="C455" t="s">
         <v>555</v>
@@ -7165,7 +7161,7 @@
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C456" t="s">
         <v>555</v>
@@ -7173,55 +7169,55 @@
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C457" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C458" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C459" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>561</v>
+        <v>750</v>
       </c>
       <c r="C460" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>751</v>
+        <v>563</v>
       </c>
       <c r="C461" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B462" t="s">
-        <v>563</v>
+      <c r="B462" s="4" t="s">
+        <v>565</v>
       </c>
       <c r="C462" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B463" s="4" t="s">
-        <v>565</v>
+      <c r="B463" t="s">
+        <v>566</v>
       </c>
       <c r="C463" t="s">
         <v>564</v>
@@ -7229,39 +7225,39 @@
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C464" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C465" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C466" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>571</v>
+        <v>737</v>
       </c>
       <c r="C467" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
-        <v>738</v>
+        <v>778</v>
       </c>
       <c r="C468" t="s">
         <v>574</v>
@@ -7269,7 +7265,7 @@
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>779</v>
+        <v>736</v>
       </c>
       <c r="C469" t="s">
         <v>574</v>
@@ -7277,7 +7273,7 @@
     </row>
     <row r="470" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
-        <v>737</v>
+        <v>573</v>
       </c>
       <c r="C470" t="s">
         <v>574</v>
@@ -7285,15 +7281,15 @@
     </row>
     <row r="471" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
-        <v>573</v>
+        <v>700</v>
       </c>
       <c r="C471" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="472" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>701</v>
+        <v>762</v>
       </c>
       <c r="C472" t="s">
         <v>576</v>
@@ -7301,7 +7297,7 @@
     </row>
     <row r="473" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>763</v>
+        <v>575</v>
       </c>
       <c r="C473" t="s">
         <v>576</v>
@@ -7309,58 +7305,58 @@
     </row>
     <row r="474" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="C474" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C475" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="476" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B476" t="s">
-        <v>577</v>
+      <c r="B476" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="C476" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="477" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B477" s="4" t="s">
-        <v>579</v>
+      <c r="B477" t="s">
+        <v>580</v>
       </c>
       <c r="C477" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="478" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C478" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="479" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C479" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="480" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>584</v>
+        <v>701</v>
       </c>
       <c r="C480" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="481" spans="2:3" x14ac:dyDescent="0.25">
@@ -7373,7 +7369,7 @@
     </row>
     <row r="482" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
-        <v>703</v>
+        <v>586</v>
       </c>
       <c r="C482" t="s">
         <v>587</v>
@@ -7381,7 +7377,7 @@
     </row>
     <row r="483" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B483" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C483" t="s">
         <v>587</v>
@@ -7389,23 +7385,23 @@
     </row>
     <row r="484" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B484" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C484" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="485" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B485" t="s">
-        <v>589</v>
+      <c r="B485" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C485" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="486" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B486" s="4" t="s">
-        <v>591</v>
+      <c r="B486" t="s">
+        <v>593</v>
       </c>
       <c r="C486" t="s">
         <v>592</v>
@@ -7413,7 +7409,7 @@
     </row>
     <row r="487" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C487" t="s">
         <v>592</v>
@@ -7421,22 +7417,22 @@
     </row>
     <row r="488" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B488" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C488" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="489" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B489" t="s">
-        <v>595</v>
+    <row r="489" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B489" s="11" t="s">
+        <v>703</v>
       </c>
       <c r="C489" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="490" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B490" s="11" t="s">
+    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B490" s="10" t="s">
         <v>704</v>
       </c>
       <c r="C490" t="s">
@@ -7444,8 +7440,8 @@
       </c>
     </row>
     <row r="491" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B491" s="10" t="s">
-        <v>705</v>
+      <c r="B491" t="s">
+        <v>596</v>
       </c>
       <c r="C491" t="s">
         <v>592</v>
@@ -7453,15 +7449,15 @@
     </row>
     <row r="492" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C492" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
     </row>
     <row r="493" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C493" t="s">
         <v>598</v>
@@ -7469,15 +7465,15 @@
     </row>
     <row r="494" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B494" t="s">
-        <v>599</v>
+        <v>735</v>
       </c>
       <c r="C494" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="495" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B495" t="s">
-        <v>736</v>
+        <v>600</v>
       </c>
       <c r="C495" t="s">
         <v>601</v>
@@ -7485,7 +7481,7 @@
     </row>
     <row r="496" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C496" t="s">
         <v>601</v>
@@ -7493,15 +7489,15 @@
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
-        <v>602</v>
+        <v>705</v>
       </c>
       <c r="C497" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="498" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>706</v>
+        <v>603</v>
       </c>
       <c r="C498" t="s">
         <v>604</v>
@@ -7509,15 +7505,15 @@
     </row>
     <row r="499" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C499" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="500" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B500" t="s">
-        <v>605</v>
+      <c r="B500" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="C500" t="s">
         <v>604</v>
@@ -7525,14 +7521,14 @@
     </row>
     <row r="501" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B501" s="4" t="s">
-        <v>606</v>
+        <v>706</v>
       </c>
       <c r="C501" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="502" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B502" s="4" t="s">
+      <c r="B502" t="s">
         <v>707</v>
       </c>
       <c r="C502" t="s">
@@ -7541,7 +7537,7 @@
     </row>
     <row r="503" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
-        <v>708</v>
+        <v>607</v>
       </c>
       <c r="C503" t="s">
         <v>608</v>
@@ -7549,55 +7545,55 @@
     </row>
     <row r="504" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
-        <v>607</v>
+        <v>709</v>
       </c>
       <c r="C504" t="s">
-        <v>608</v>
+        <v>710</v>
       </c>
     </row>
     <row r="505" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
-        <v>710</v>
+        <v>609</v>
       </c>
       <c r="C505" t="s">
-        <v>711</v>
+        <v>610</v>
       </c>
     </row>
     <row r="506" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C506" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="507" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C507" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="508" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
-        <v>613</v>
+        <v>708</v>
       </c>
       <c r="C508" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="509" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B509" t="s">
-        <v>709</v>
+      <c r="B509" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="C509" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="510" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B510" s="4" t="s">
-        <v>615</v>
+      <c r="B510" t="s">
+        <v>616</v>
       </c>
       <c r="C510" t="s">
         <v>614</v>
@@ -7605,7 +7601,7 @@
     </row>
     <row r="511" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C511" t="s">
         <v>614</v>
@@ -7613,25 +7609,17 @@
     </row>
     <row r="512" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C512" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="513" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C513" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B514" t="s">
-        <v>620</v>
-      </c>
-      <c r="C514" t="s">
         <v>621</v>
       </c>
     </row>

</xml_diff>